<commit_message>
[feat][Operating System][Operating System Concepts]
</commit_message>
<xml_diff>
--- a/Operations-System/DevOps-Documents.xlsx
+++ b/Operations-System/DevOps-Documents.xlsx
@@ -5,20 +5,20 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="1" activeTab="10"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Trang_tính1" sheetId="1" state="hidden" r:id="rId3"/>
-    <sheet name="1.Git" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="1. Operations System" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Trang_tính1" sheetId="2" state="hidden" r:id="rId4"/>
     <sheet name="2. Linux" sheetId="3" state="visible" r:id="rId5"/>
     <sheet name="3.Networking &amp; Security" sheetId="4" state="visible" r:id="rId6"/>
-    <sheet name="4.Server Management" sheetId="5" state="visible" r:id="rId7"/>
-    <sheet name="5.Containers" sheetId="6" state="visible" r:id="rId8"/>
-    <sheet name="6.Container Orchestration" sheetId="7" state="visible" r:id="rId9"/>
-    <sheet name="7.Infrastructure as a code" sheetId="8" state="visible" r:id="rId10"/>
-    <sheet name="8.CI&amp;CD" sheetId="9" state="visible" r:id="rId11"/>
-    <sheet name="9.Cloud" sheetId="10" state="visible" r:id="rId12"/>
-    <sheet name="1. Operations System" sheetId="11" state="visible" r:id="rId13"/>
+    <sheet name="1.Git" sheetId="5" state="visible" r:id="rId7"/>
+    <sheet name="4.Server Management" sheetId="6" state="visible" r:id="rId8"/>
+    <sheet name="5.Containers" sheetId="7" state="visible" r:id="rId9"/>
+    <sheet name="6.Container Orchestration" sheetId="8" state="visible" r:id="rId10"/>
+    <sheet name="7.Infrastructure as a code" sheetId="9" state="visible" r:id="rId11"/>
+    <sheet name="8.CI&amp;CD" sheetId="10" state="visible" r:id="rId12"/>
+    <sheet name="9.Cloud" sheetId="11" state="visible" r:id="rId13"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -30,7 +30,1507 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="218">
+  <si>
+    <t xml:space="preserve">Operating System Concepts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overview</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Introduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What Operating Systems Do</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> An operating system (OS) is the foundational software that bridges the gap between computer hardware and application programs. It is responsible for managing hardware resources, providing a consistent environment for software to run, and ensuring that multiple applications can operate concurrently without conflict. 
+- An operating system is software that manages a computer’s hardware.
+- A fundamental responsibility of an operating system is to allocate these resources to programs.
+- Computer system as consisting: hardware, software, and data.
+- OS provides the means for proper use of these resources in the operation of the computer system, provides an an environment within other programs can do useful work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User View</t>
+  </si>
+  <si>
+    <t xml:space="preserve">System View</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> - From the computer’s point of view, the operating system is the program most </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">intimately involved with the hardware</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">. In this context, we can view an operating system as a resource allocator
+ - An operating system is a control program, manages the execution of user programs to prevent errors and improper use of the computer. It is especially concerned with the operation and control of I/O devices.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Defining OS</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> - Operating systems exist because they offer a reasonable way to solve the problem of creating a usable computing system. The common functions of controlling and allocating resources are then brought together into one piece of software: the operating system.
+ - A more common definition, and the one that we usually follow, is that the operating system is the one program running at all times on the computer—usually called the </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">kernel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">.
+ - Mobile operating systems often include not only a core kernel but also middleware—a set of software frameworks that provide additional services to application developers.
+ - </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">Kernel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">: A kernel is a computer program at the core of a computer's operating system that always has complete control over everything in the system.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Computer-System Organization</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> - A modern general-purpose computer system consists of one or more CPUs and a number of device controllers connected through a common bus that provides access between components and shared memory. Each device controller is in charge of a specific type of device (for example, a disk drive, audio device, or graphics display).
+ - Typically, OS have a </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">device driver</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> for each device controller. This device driver understands the device controller and provides the rest of os with a uniform interface to the device.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Interrupts</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> - Interrupts are used for many other purposes as well and are a key part of how operating systems and hardware interact.
+ - Interrupts are signals sent to the CPU that temporarily halt the current execution flow. They </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">serve as notifications that some event requires immediate attention</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">-for example, an I/O device needs servicing or a software condition has occurred.
+ - Interrupts are key to enabling multitasking, efficient I/O handling, and responsive systems without the need for constant polling.
+ - Asynchronous Events: Most interrupts occur asynchronously-that is, they happen independently of the currently running program.
+ - Synchronous Events (Exceptions): Some events, like division by zero or invalid memory access, trigger interrupts as well, these are often called exceptions.
+ - When the CPU is interrupted, it stops what it is doing and immediately transfer execution to fixed location, which usually contains the starting address where the service routine for the interrupt is located. The interrupt service routine executes; on completion, the CPU resumes the interrupted computation.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Types of Interrupts</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> - Hardware Interrupts
+  + Definition: Generated by external hardware devices (e.g., keyboards, mice, network cards, timers,…) when they need to communicate with the CPU.
+  + Examples: I/O Interrupts: When a disk finishes reading or writing, an interrupts signals that the data is ready. Timer interrupts: Periodic interrupts generated by a system timer, allowing the OS to perform regular tasks such as process scheduling.
+  + Handling: The hardware interrupts signals the CPU, which then suspends the current process, saves its state, and jumps to an </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">interrupts service routine</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> (ISR) in the kernel.
+ - Software Interrupts
+  + Definition: Generated by programs or the OS itself to request kernel-level services.
+  + Example: 
+   - System calls: When a user application needs to perform an operation like file I/O, it triggers a software interrupt to transition into kernel mode.
+   - Explicit Interrupt Instructions: Some architectures use dedicated instructions (like the x86INT instruction) to generate software interrupts.
+  + Handling: These trigger the ISR, but they are initiated by software for controlled tasks rather than external events
+ - Exceptions (Traps):
+  + Definition: Special cases of interrupts that occur due to errors or unusual conditions in the execution of a program.
+  + Handling: Exceptions often lead to the termination of the offending process or are handle by specific error routines in the OS to maintain system stability.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">How interrupts are handled by the Kernel</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> 1. Interrupt Request (IRQ): The device or software issues an interrupt signal to the CPU. The CPU, which monitors the interrupt lines, recognizes the signal.
+ 2. Interrupt </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">Acknowledgment</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">(thừa nhận) and Saving Context: The CPU suspends the execution of the current process. It saves the state of the process(register, program counter, etc) so that execution can resume later without data loss.
+ 3. Interrupt Vectoring: The CPU consults an interrupt vector table-a structure mapping each interrupt type to its corresponding handler routine. This table ensures that the correct interrupt service routine(ISR) is invoked.
+ 4. Execution of the Interrupt Service Routine (ISR): ISR is a part of the kernel, executes the specific instructions required to handle the interrupt. For hardware interrupts, this might involve reading data form an I/O port; for software interrupts, it might involve executing a system call.
+ 5. Restoring Context: Once the ISR has completed its task, the kernel restores the saved context of the interrupted process. The CPU then resumes execution from where it was interrupted.
+ 6. Return from Interrupt: Finally, control is returned to the previously running process, and normal operation continues.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Additional Concepts Related to Interrupts</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1. Interrupt masking and Prioritization:
+  - Masking: The kernel can temporarily disable(mask) certain interrupts during critical operations to prevent interference.
+  - Prioritization: Interrupts often have priorities assigned so that more critical events (like a hardware failure) are handled before less urgent ones (like a keyboard press).
+ 2. Context Switching Overhead
+  - Performance Impact: Although interrupts allow rapid response to events, each interrupt requires saving and restoring process state. High frequencies of interrupts can lead to overhead and impact system performance.
+  - Optimization: Modern systems optimize this process through techniques such as interrupt coalescing and prioritizing interrupt sources.
+ 3. Real-Time Considerations 
+  - In real-time operating system (RTOS), the timing of interrupt handling is crucial. Interrupt latencies must be minimized to ensure that high-priority tasks are serviced within strict time constraints</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Storage Structure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Storage Definitions and Notation</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> - The basic unit of computer storage is the bit. A bit can contain one of two values, 0 and 1. </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">All other storage in a computer is based on collections of bits</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">.
+ - A byte is 8 bits, and on most computers it is the </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">smallest convenient chunk of storage(byte)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">. Most computers don’t have an instruction to move a bit but do have one to move a byte.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Structure</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve"> - The CPU can load </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">instructions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve"> only from memory, so any programs must first be loaded into memory to run. 
+ - General-purpose computers run most of their programs from rewritable memory, called main memory (also called random-access memory, or RAM). RAM is volatile—loses its content when power is turned off or otherwise lost
+ - The first program to run on computer power-on is a bootstrap program, which then loads the operating system. Since RAM is volatile we cannot trust it to hold the bootstrap program. Instead, the computer uses electrically erasable programmable read-only memory (</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">EEPROM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">) and other forms of </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">firmwar</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve"> —storage that is infrequently(not often) written to and is nonvolatile.
+ - All forms of memory provide an array of bytes. Each byte has its own address.  Interaction is achieved through a sequence of load or store instructions to specific memory addresses.  The load instruction moves a byte or word from main memory to an internal register within the CPU, whereas the store instruction moves the content of a register to main memory. 
+ - A typical instruction-execution cycle, as executed on a system with a vonNeumann architecture: 
+  + First fetches instruction from memory and stores in the </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">instruction register</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">.
+  + Decode instruction stored in some internal register.
+  + Final instruction has been executed, result may be stored back in memory.
+ - Main memory is not possible hold large quantities of data </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">permanently</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">(vĩnh viễn) because volatile and small → We need </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">secondary storage</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">(hard-disk drives, nonvolatile memory(NVM) devices, ...).
+ </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">→</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">  The main differences among the various storage systems lie in speed, size, and volatility. The trade-off between size and speed, with smaller and faster memory closer to the
+CPU.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">I/O Structure</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> - G</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">eneral-purpose computer system consists of multiple devices, all of which exchange data via a common bus. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">A large portion of operating system code is dedicated to managing I/O, both because of its importance to the reliability and performance of a system and because of the varying nature of the devices.
+ - The form of interrupt-driven I/O is fine for moving small amounts of data but can produce high overhead when used for bulk data movement such as NVS I/O. 
+ → </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">Direct memory access</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> (DMA) is used. The device controller transfers an entire block of data directly to or from the device and main memory, with no intervention by the CPU. Only one interrupt is generated per block, to tell the device driver that the operation has completed, rather than the one interrupt per byte generated for low-speed devices. While the device controller is performing these operations, the CPU is
+available to accomplish other work.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Computer-System Architecture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Single-Processor Systems</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> - Many years ago, most computer systems used a single processor containing one CPU with a single processing core. The </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">core</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> is the component that executes instructions and registers for storing data locally. The one main CPU with its core is capable of executing a general-purpose instruction set, including instructions from processes.
+ - A single-processor system is built around one CPU that executes the fetch–decode–execute cycle. In these systems, all system components—memory, input/output (I/O) devices, storage, and peripheral interfaces—are connected via a common bus or similar interconnection mechanism. Although modern single-processor systems may support features like hardware multithreading or pipelining, they still </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">rely on one processing unit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> to perform computations.
+ - Only one processing unit exists, so true parallel execution of independent instruction streams isn’t possible. Instead, the operating system uses techniques like context switching and preemptive scheduling to create the illusion of simultaneous execution among multiple processes.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiprocessor Systems</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">Traditionally</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">:
+ - The primary advantage of multiprocessor systems is increased throughput.
+ - The most common multiprocessor systems use </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">symmetric multiprocessing</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> (SMP).
+  + Each CPU processor has its own set of registers, as well as a private or local cache.
+  + P</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">eer CPU processor performs all tasks, including operating-system functions and user processes.
+  + Many processes can run simultaneously N processes can run if there are N CPUs without causing performance to deteriorate significantly.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">Now</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">:
+ - The definition of multiprocessor has evolved over time and now includes multicore systems, in which </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">multiple computing cores reside on a single chip</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">.
+  + Multicore systems can be more efficient than multiple chips with single cores because on-chip communication is faster than between-chip communication.
+  + One chip with multiple cores uses significantly less power than multiple single-core chips.
+  + Each core has its own register set, as well as its own local cache, often known as a level 1, or L1, cache.
+  + Level 2 (L2) cache is local to the chip but is shared by the two processing cores.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Definitions of computer system components</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">- Processor: A physical chip that contains one or more CPUs.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> - CPU: The hardware that executes instructions.
+ - Core: The basic computation unit of the CPU.
+ - Multiprocessor: Including multiple processors.
+ - Multicore: Including multiple compiting cores on the same CPU
+→ Although virually all systems are now multicore, we use the general term CPU when refering to a single computational unit of a computer system and core as well as multicore when specifically referring to one or more cores on a CPU.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Clustered Systems</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> - They are composed of two or more individual systems—or nodes—joined together; each node is typically a multicore system: 
+ - Such systems are considered </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">loosely coupled</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">.
+ - Provide high-availability service—that is, service that will continue even if one or more systems in the cluster fail.
+ - The ability to continue providing service proportional to the level of surviving hardware is called </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">graceful degradation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">. 
+ - Some systems go beyond graceful degradation and are called </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">fault tolerant</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">, because they can suffer a failure of any single component and still continue operation.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Operating - System Operations</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> - An operating system provides the environment within which programs are executed.
+ - Computer need “an </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">initial program</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> to run” (start running, powered up, rebooted, initializes CPU registers, devices controllers, memory contens, OS,…), it is stored within the computer hardware in </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">firmware</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">.
+ - To accomplish these goal, the </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">bootstrap program</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> must </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">locate</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">(xác định) the operating-system kernel and </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">load it into memory</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">. 
+  + Once the kernel is loaded and executing, it can start providing services to the system and its users.
+  + Some services are provided outside of the kernel by system programs that are loaded into memory at boot time to become </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">system daemons</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">, which run the entire time the kernel is running.
+ - On Linux, the first system program is “systemd,” and it starts many other daemons.
+ - If no processes, I/O, users, OS waiting for something to happen. Events are almost always </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">signaled</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">(báo hiệu) by the occurrence(sự xuất hiện) of an interrupt.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">Multiprogramming</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> &amp; </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">Multitasking</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> - One of the most important aspects of operating systems is the ability to run multiple programs, as a single program cannot.
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">Multiprogramming</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">:
+  + Multiprogramming refers to an operating system’s ability to load multiple programs (or jobs) into memory simultaneously. The CPU then switches among these programs—typically when one program is waiting for I/O—so that the processor is never idle.
+  + I</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">ncreases CPU utilization</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">, as well as keeping users satisfied, by organizing programs so that the CPU always has one to execute.
+  + A program in execution is termed a </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">process</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">.
+  + When that process needs to wait, the CPU switches to another process, and so on. Eventually, the first process finishes waiting and gets the CPU back.
+  + The OS loads multiple programs into memory. Each program is assigned a section of memory and given a process control block (PCB) that stores its state. When one program (process) blocks (for example, waiting for I/O), the OS scheduler switches the CPU to another program that is ready to run.
+ - </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">Multitasking</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">:
+  + Multitasking is the capability of an operating system to execute more than one task </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">concurrently</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">. 
+  + In a single-processor system, this is achieved by </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">rapidly context switching between tasks,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve"> giving the user the illusion that tasks are </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">running simultaneously</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">.
+  + The OS divides CPU time into small slices (time-sharing). When one task’s time slice expires, the OS saves its state (context) and switches to another task, making it appear that tasks run in parallel.
+  + Even on a single CPU, multitasking allows multiple tasks to progress concurrently. On multiprocessor or multicore systems, true parallelism is achieved as different processors or cores run different tasks simultaneously.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Dual-Mode &amp; Multimode Operation</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> - Os and its users share resources(hardware, software,…), a properly design OS must ensure that an incorrect (or malicious) program cannot cause other programs or OS. We must be able to distinguish between the execution of OS code and user-defined code, and the approach is provide differentiation among </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">various modes of execution</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">.
+ - Two modes of operation: user mode and kernel mode.
+ - At system boot time, the hardware starts in kernel mode. The operating system is then loaded and starts user applications in user mode.
+ - The dual mode of operation provides us with the means for protecting the operating system from </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">errant users</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">(người dùng xấu)—and errant users from one another:
+  + Designating(chỉ định) some of the machine instructions that may cause harm as </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">privileged instructions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">.
+  + The hardware allows </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">privileged instructions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> to be executed only in kernel mode. If an attempt is made to execute a </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">privileged instruction</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> in </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">user mode</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">, the hardware does not execute the instruction but rather treats it as </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">illegal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">(bất hợp pháp) and traps(giữ) it to the OS.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">System call</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overview and Purpose</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - A system call is a well-defined interface provided by the OS that enables user programs to request kernel-level services. These services include process control, file management, interprocess communication, network operations, and more.
+ -  Since user programs run in a restricted environment (user mode) for safety and stability, they cannot directly perform operations that affect the hardware or other processes. System calls allow these programs to safely delegate such tasks to the OS (which runs in kernel mode), ensuring that resource management and security policies are enforced.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invocation Mechanism</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">Triggering the System Call
+ - Trap or Software Interrupt: A system call is typically initiated via a special instruction that causes a </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">trap</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> – a kind of software interrupt.
+ - Transition to Kernel Mode: Executing this trap causes the processor to switch from user mode to kernel mode by setting a mode bit (0/1). This ensures that the subsequent operations have full access to the hardware and protected system resources.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Handling in the OS Kernel
+ - Interrupt Vector Table: The trap directs the CPU to a predetermined location in the interrupt vector table that points to the system call handler in the OS kernel.
+ - Identification of the Call: Once inside the kernel, the system call handler examines a system call number—usually passed in a specific register—to determine which service is being requested. Additional parameters (like file descriptors, memory pointers, or numeric values) are provided through registers, the stack, or memory.
+ - Parameter Verification: The OS verifies that the parameters are valid and that the calling process has the necessary privileges. This step is crucial for maintaining system stability and security.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Executing the Request and Returning
+ - Service Execution: The OS performs the requested service (for example, reading data from a disk). The actual operation is executed in kernel mode, ensuring that it can safely access hardware devices and system resources.
+ - Returning Results: Once the operation completes, the OS prepares a return value (or error code) and then performs a context switch back to the user process. The processor’s mode is switched back to user mode, and control resumes at the instruction immediately following the original system call.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Timer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resource Management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Security and Protection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Virtualization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Distributed Systems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kernel Data Structures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Computing Environments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Free and Open-Source Operating Systems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operating-System Structure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Process Management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Processes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Threads &amp; Concurrency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CPU Scheduling</t>
+  </si>
   <si>
     <t xml:space="preserve">Kiến Trúc về Microservice</t>
   </si>
@@ -702,24 +2202,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Sự khác nhau giữa Merge và Rebase, out put có giống nhau ko?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Merge: Phương pháp Merge dùng để kết hợp các thay đổi từ một nhánh khác vào nhánh hiện tại. Khi sử dụng Merge, Git sẽ tạo ra một commit mới trên nhánh hiện tại để tích hợp các commit từ nhánh khác. Kết quả đầu ra của Merge là một cây lịch sử mới với các commit từ cả hai nhá
- - Rebase: Phương pháp Rebase cũng dùng để kết hợp các thay đổi từ một nhánh khác vào nhánh hiện tại. Tuy nhiên, thay vì tạo ra một commit mới, Rebase sẽ di chuyển các commit của nhánh hiện tại và đặt chúng lên đầu của nhánh khác. Kết quả đầu ra của Rebase là một cây lịch sử mới với các commit được sắp xếp theo thứ tự thời gian.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chuẩn của Git Flow?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mô hình Git Flow bao gồm các nhánh chính sau:
-Master: Nhánh Master chứa mã nguồn ổn định và đã được phê duyệt để triển khai.
-Develop: Nhánh Develop chứa mã nguồn của tất cả các tính năng được phát triển và đang được kiểm tra.
-Feature: Nhánh Feature được tạo ra để phát triển tính năng mới hoặc sửa đổi tính năng hiện có. Mỗi tính năng sẽ có một nhánh Feature riêng.
-Release: Nhánh Release được sử dụng để chuẩn bị cho việc phát hành sản phẩm. Ở đây, các lỗi nhỏ được sửa đổi và bản phát hành được chuẩn bị.
-Hotfix: Nhánh Hotfix được tạo ra để sửa lỗi ngay lập tức trên nhánh Master.</t>
-  </si>
-  <si>
     <t xml:space="preserve">SETUP ENVIROMENT</t>
   </si>
   <si>
@@ -1467,6 +2949,24 @@
   </si>
   <si>
     <t xml:space="preserve"> &lt;identifier&gt; : &lt;runlevel&gt; : &lt;action&gt; : &lt;process&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sự khác nhau giữa Merge và Rebase, out put có giống nhau ko?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Merge: Phương pháp Merge dùng để kết hợp các thay đổi từ một nhánh khác vào nhánh hiện tại. Khi sử dụng Merge, Git sẽ tạo ra một commit mới trên nhánh hiện tại để tích hợp các commit từ nhánh khác. Kết quả đầu ra của Merge là một cây lịch sử mới với các commit từ cả hai nhá
+ - Rebase: Phương pháp Rebase cũng dùng để kết hợp các thay đổi từ một nhánh khác vào nhánh hiện tại. Tuy nhiên, thay vì tạo ra một commit mới, Rebase sẽ di chuyển các commit của nhánh hiện tại và đặt chúng lên đầu của nhánh khác. Kết quả đầu ra của Rebase là một cây lịch sử mới với các commit được sắp xếp theo thứ tự thời gian.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chuẩn của Git Flow?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mô hình Git Flow bao gồm các nhánh chính sau:
+Master: Nhánh Master chứa mã nguồn ổn định và đã được phê duyệt để triển khai.
+Develop: Nhánh Develop chứa mã nguồn của tất cả các tính năng được phát triển và đang được kiểm tra.
+Feature: Nhánh Feature được tạo ra để phát triển tính năng mới hoặc sửa đổi tính năng hiện có. Mỗi tính năng sẽ có một nhánh Feature riêng.
+Release: Nhánh Release được sử dụng để chuẩn bị cho việc phát hành sản phẩm. Ở đây, các lỗi nhỏ được sửa đổi và bản phát hành được chuẩn bị.
+Hotfix: Nhánh Hotfix được tạo ra để sửa lỗi ngay lập tức trên nhánh Master.</t>
   </si>
   <si>
     <t xml:space="preserve">Reverse Proxy</t>
@@ -2198,323 +3698,6 @@
    - variables: biến môi trường sử dụng trong pipeline
    - _job: định nghĩa các giai đoạn (job) thực thi trong pipeline. bao gồm : stage, script</t>
   </si>
-  <si>
-    <t xml:space="preserve">Operating System Concepts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Overview</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Introduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What Operating Systems Do</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> An operating system (OS) is the foundational software that bridges the gap between computer hardware and application programs. It is responsible for managing hardware resources, providing a consistent environment for software to run, and ensuring that multiple applications can operate concurrently without conflict. 
-- An operating system is software that manages a computer’s hardware.
-- A fundamental responsibility of an operating system is to allocate these resources to programs.
-- Computer system as consisting: hardware, software, and data.
-- OS provides the means for proper use of these resources in the operation of the computer system, provides an an environment within other programs can do useful work</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User View</t>
-  </si>
-  <si>
-    <t xml:space="preserve">System View</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="15"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve"> - From the computer’s point of view, the operating system is the program most </t>
-    </r>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="15"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">intimately involved with the hardware</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">. In this context, we can view an operating system as a resource allocator
- - An operating system is a control program, manages the execution of user programs to prevent errors and improper use of the computer. It is especially concerned with the operation and control of I/O devices.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Defining OS</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="15"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve"> - Operating systems exist because they offer a reasonable way to solve the problem of creating a usable computing system. The common functions of controlling and allocating resources are then brought together into one piece of software: the operating system.
- - A more common definition, and the one that we usually follow, is that the operating system is the one program running at all times on the computer—usually called the </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="15"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">kernel</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">.
- - Mobile operating systems often include not only a core kernel but also middleware—a set of software frameworks that provide additional services to application developers.
- - </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="15"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">Kernel</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">: A kernel is a computer program at the core of a computer's operating system that always has complete control over everything in the system.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Computer-System Organization</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="15"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve"> - A modern general-purpose computer system consists of one or more CPUs and a number of device controllers connected through a common bus that provides access between components and shared memory. Each device controller is in charge of a specific type of device (for example, a disk drive, audio device, or graphics display).
- - Typically, OS have a </t>
-    </r>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="15"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">device driver</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve"> for each device controller. This device driver understands the device controller and provides the rest of os with a uniform interface to the device.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Interrupts</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="15"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve"> - Interrupts are used for many other purposes as well and are a key part of how operating systems and hardware interact.
- - Interrupts are signals sent to the CPU that temporarily halt the current execution flow. They </t>
-    </r>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="15"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">serve as notifications that some event requires immediate attention</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">-for example, an I/O device needs servicing or a software condition has occurred.
- - Interrupts are key to enabling multitasking, efficient I/O handling, and responsive systems without the need for constant polling.
- - Asynchronous Events: Most interrupts occur asynchronously-that is, they happen independently of the currently running program.
- - Synchronous Events (Exceptions): Some events, like division by zero or invalid memory access, trigger interrupts as well, these are often called exceptions.
- - When the CPU is interrupted, it stops what it is doing and immediately transfer execution to fixed location, which usually contains the starting address where the service routine for the interrupt is located. The interrupt service routine executes; on completion, the CPU resumes the interrupted computation.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Types of Interrupts</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - Hardware Interrupts
-  + Definition: Generated by external hardware devices (e.g., keyboards, mice, network cards, timers,…) when they need to communicate with the CPU.
-  + Examples: I/O Interrupts: When a disk finishes reading or writing, an interrupts signals that the data is ready. Timer interrupts: Periodic interrupts generated by a system timer, allowing the OS to perform regular tasks such as process scheduling.
-  + Handling: The hardware interrupts signals the CPU, which then suspends the current process, saves its state, and jumps to an interrupts service routine (ISR) in the kernel.
- - Software Interrupts
-  + Definition: Generated by programs or the OS itself to request kernel-level services.
-  + Example: 
-   - System calls: When a user application needs to perform an operation like file I/O, it triggers a software interrupt to transition into kernel mode.
-   - Explicit Interrupt Instructions: Some architectures use dedicated instructions (like the x86INT instruction) to generate software interrupts.
-  + Handling: These trigger the ISR, but they are initiated by software for controlled tasks rather than external events
- - Exceptions:
-  + Definition: Special cases of interrupts that occur due to errors or unusual conditions in the execution of a program.
-  + Handling: Exceptions often lead to the termination of the offending process or are handle by specific error routines in the OS to maintain system stability.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">How interrupts are handled by the Kernel</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="15"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve"> 1. Interrupt Request (IRQ): The device or software issues an interrupt signal to the CPU. The CPU, which monitors the interrupt lines, recognizes the signal.
- 2. Interrupt </t>
-    </r>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="15"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">Acknowledgment</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">(thừa nhận) and Saving Context: The CPU suspends the execution of the current process. It saves the state of the process(register, program counter, etc) so that execution can resume later without data loss.
- 3. Interrupt Vectoring: The CPU consults an interrupt vector table-a structure mapping each interrupt type to its corresponding handler routine. This table ensures that the correct interrupt service routine(ISR) is invoked.
- 4. Execution of the Interrupt Service Routine (ISR): ISR is a part of the kernel, executes the specific instructions required to handle the interrupt. For hardware interrupts, this might involve reading data form an I/O port; for software interrupts, it might involve executing a system call.
- 5. Restoring Context: Once the ISR has completed its task, the kernel restores the saved context of the interrupted process. The CPU then resumes execution from where it was interrupted.
- 6. Return from Interrupt: Finally, control is returned to the previously running process, and normal operation continues.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Additional Concepts Related to Interrupts</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1. Interrupt masking and Prioritization:
-  - Masking: The kernel can temporarily disable(mask) certain interrupts during critical operations to prevent interference.
-  - Prioritization: Interrupts often have priorities assigned so that more critical events (like a hardware failure) are handled before less urgent ones (like a keyboard press).
- 2. Context Switching Overhead
-  - Performance Impact: Although interrupts allow rapid response to events, each interrupt requires saving and restoring process state. High frequencies of interrupts can lead to overhead and impact system performance.
-  - Optimization: Modern systems optimize this process through techniques such as interrupt coalescing and prioritizing interrupt sources.
- 3. Real-Time Considerations 
-  - In real-time operating system (RTOS), the timing of interrupt handling is crucial. Interrupt latencies must be minimized to ensure that high-priority tasks are serviced within strict time constraints</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Storage Structure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I/O Structure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Computer-System Architecture</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Operating - System Operations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resource Management</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Security and Protection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Virtualization</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Distributed Systems</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kernel Data Structures</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Computing Environments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Free and Open-Source Operating Systems</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Operating-System Structure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Process Management</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Processes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Threads &amp; Concurrency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CPU Scheduling</t>
-  </si>
 </sst>
 </file>
 
@@ -2523,7 +3706,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="30">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2545,6 +3728,98 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="30"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="25"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="30"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -2646,71 +3921,6 @@
       <family val="0"/>
       <charset val="134"/>
     </font>
-    <font>
-      <sz val="30"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="25"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="20"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="30"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="15"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="15"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -2765,30 +3975,106 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="49">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2796,15 +4082,15 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2812,7 +4098,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2824,11 +4110,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2836,7 +4122,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2844,19 +4130,19 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2864,7 +4150,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="25" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2872,7 +4158,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2880,68 +4166,20 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -3030,9 +4268,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>588960</xdr:colOff>
+      <xdr:colOff>588600</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>2121840</xdr:rowOff>
+      <xdr:rowOff>2121480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3046,7 +4284,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10237320" y="8324640"/>
-          <a:ext cx="4801680" cy="2799000"/>
+          <a:ext cx="4801320" cy="2798640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3067,9 +4305,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>665280</xdr:colOff>
+      <xdr:colOff>664920</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>1797840</xdr:rowOff>
+      <xdr:rowOff>1797480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3083,7 +4321,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10323000" y="11420280"/>
-          <a:ext cx="4792320" cy="2494080"/>
+          <a:ext cx="4791960" cy="2493720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3104,9 +4342,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>522360</xdr:colOff>
+      <xdr:colOff>522000</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>696600</xdr:rowOff>
+      <xdr:rowOff>696240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3120,7 +4358,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10170720" y="24355440"/>
-          <a:ext cx="4801680" cy="2903760"/>
+          <a:ext cx="4801320" cy="2903400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3312,214 +4550,516 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B9" colorId="64" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D25" colorId="64" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G31" activeCellId="0" sqref="G31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="36.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="18.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="19.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="4" width="21.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="5" width="15.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="5" width="19.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="5" width="206.01"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="92.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+    </row>
+    <row r="3" customFormat="false" ht="57.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="10"/>
+    </row>
+    <row r="4" customFormat="false" ht="96.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="10"/>
+    </row>
+    <row r="5" customFormat="false" ht="58.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+    </row>
+    <row r="6" customFormat="false" ht="151.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="10"/>
+    </row>
+    <row r="7" customFormat="false" ht="300.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="183.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="187.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="6"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="57.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="335" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="126.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="16"/>
+    </row>
+    <row r="13" customFormat="false" ht="126.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="216.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="6"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="E14" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="126.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="6"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="91" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="6"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="8"/>
+      <c r="E16" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="133.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="335" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="6"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="8"/>
+      <c r="E18" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="G18" s="16"/>
+    </row>
+    <row r="19" customFormat="false" ht="144.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="6"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="8"/>
+      <c r="E19" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G19" s="16"/>
+    </row>
+    <row r="20" customFormat="false" ht="73.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="6"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="8"/>
+      <c r="E20" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="G20" s="19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="77.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="6"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="8"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="78.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="6"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="8"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="101.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="6"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="8"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="6"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="8"/>
+      <c r="E24" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+    </row>
+    <row r="25" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="6"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="6"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="6"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="6"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="6"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="6"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="88.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="6"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="75.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="6"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="6"/>
+      <c r="B33" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="75.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="6"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="6"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="6"/>
+    </row>
+    <row r="37" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="6"/>
+    </row>
+    <row r="38" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="6"/>
+    </row>
+    <row r="39" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="6"/>
+    </row>
+    <row r="40" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="6"/>
+    </row>
+    <row r="41" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="6"/>
+    </row>
+    <row r="42" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="6"/>
+    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <mergeCells count="27">
+    <mergeCell ref="A1:A42"/>
+    <mergeCell ref="B1:B32"/>
+    <mergeCell ref="C1:C31"/>
+    <mergeCell ref="D1:D4"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="D5:D12"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E6:E9"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="D13:D16"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="D17:D24"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="E20:E23"/>
+    <mergeCell ref="F21:F23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="B33:B35"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="39.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="95.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="60.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="58.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="50"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="49.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="8" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="20" width="23.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="20" width="57.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="3" style="20" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="256.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="245.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="223.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="243.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="288.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="240.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>39</v>
+    <row r="1" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="20" t="s">
+        <v>212</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="23" t="s">
+        <v>214</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="23" t="s">
+        <v>216</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>217</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D10" r:id="rId1" display="https://topdev.vn/blog/trien-khai-ci-cd-voi-gitlab/"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -3527,11 +5067,10 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -3554,373 +5093,219 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:G37"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D8" colorId="64" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="36.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="25.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="31" width="18.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="32" width="19.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="33" width="21.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="34" width="15.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="34" width="19.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="34" width="206.01"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="92.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="35" t="s">
-        <v>156</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>157</v>
-      </c>
-      <c r="C1" s="37" t="s">
-        <v>158</v>
-      </c>
-      <c r="D1" s="33" t="s">
-        <v>159</v>
-      </c>
-      <c r="E1" s="38" t="s">
-        <v>160</v>
-      </c>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-    </row>
-    <row r="2" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="35"/>
-      <c r="B2" s="36"/>
-      <c r="C2" s="37"/>
-      <c r="E2" s="39" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="57.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="35"/>
-      <c r="B3" s="36"/>
-      <c r="C3" s="37"/>
-      <c r="E3" s="39" t="s">
-        <v>162</v>
-      </c>
-      <c r="F3" s="34" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="96.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="35"/>
-      <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
-      <c r="E4" s="39" t="s">
-        <v>164</v>
-      </c>
-      <c r="F4" s="34" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="58.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="35"/>
-      <c r="B5" s="36"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="33" t="s">
-        <v>166</v>
-      </c>
-      <c r="E5" s="34" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="151.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="35"/>
-      <c r="B6" s="36"/>
-      <c r="C6" s="37"/>
-      <c r="E6" s="40" t="s">
-        <v>168</v>
-      </c>
-      <c r="F6" s="34" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="300.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="35"/>
-      <c r="B7" s="36"/>
-      <c r="C7" s="37"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40" t="s">
-        <v>170</v>
-      </c>
-      <c r="G7" s="34" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="183.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="35"/>
-      <c r="B8" s="36"/>
-      <c r="C8" s="37"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40" t="s">
-        <v>172</v>
-      </c>
-      <c r="G8" s="34" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="184.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="35"/>
-      <c r="B9" s="36"/>
-      <c r="C9" s="37"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="G9" s="34" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="35"/>
-      <c r="B10" s="36"/>
-      <c r="C10" s="37"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-    </row>
-    <row r="11" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="35"/>
-      <c r="B11" s="36"/>
-      <c r="C11" s="37"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-    </row>
-    <row r="12" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="35"/>
-      <c r="B12" s="36"/>
-      <c r="C12" s="37"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="40"/>
-    </row>
-    <row r="13" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="35"/>
-      <c r="B13" s="36"/>
-      <c r="C13" s="37"/>
-      <c r="E13" s="40" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="35"/>
-      <c r="B14" s="36"/>
-      <c r="C14" s="37"/>
-      <c r="E14" s="40" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="35"/>
-      <c r="B15" s="36"/>
-      <c r="C15" s="37"/>
-      <c r="E15" s="40"/>
-    </row>
-    <row r="16" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="35"/>
-      <c r="B16" s="36"/>
-      <c r="C16" s="37"/>
-      <c r="E16" s="40"/>
-    </row>
-    <row r="17" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="35"/>
-      <c r="B17" s="36"/>
-      <c r="C17" s="37"/>
-      <c r="E17" s="40"/>
-    </row>
-    <row r="18" customFormat="false" ht="66.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="35"/>
-      <c r="B18" s="36"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="33" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="66.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="35"/>
-      <c r="B19" s="36"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="33" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="35"/>
-      <c r="B20" s="36"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="33" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="35"/>
-      <c r="B21" s="36"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="33" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="35"/>
-      <c r="B22" s="36"/>
-      <c r="C22" s="37"/>
-      <c r="D22" s="33" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="35"/>
-      <c r="B23" s="36"/>
-      <c r="C23" s="37"/>
-      <c r="D23" s="33" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="35"/>
-      <c r="B24" s="36"/>
-      <c r="C24" s="37"/>
-      <c r="D24" s="33" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="35"/>
-      <c r="B25" s="36"/>
-      <c r="C25" s="37"/>
-      <c r="D25" s="33" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="88.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="35"/>
-      <c r="B26" s="36"/>
-      <c r="C26" s="37"/>
-      <c r="D26" s="33" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="75.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="35"/>
-      <c r="B27" s="36"/>
-      <c r="C27" s="32" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="35"/>
-      <c r="B28" s="36" t="s">
-        <v>188</v>
-      </c>
-      <c r="C28" s="32" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="75.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="35"/>
-      <c r="B29" s="36"/>
-      <c r="C29" s="32" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="35"/>
-      <c r="B30" s="36"/>
-      <c r="C30" s="32" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="35"/>
-    </row>
-    <row r="32" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="35"/>
-    </row>
-    <row r="33" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="35"/>
-    </row>
-    <row r="34" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="35"/>
-    </row>
-    <row r="35" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="35"/>
-    </row>
-    <row r="36" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="35"/>
-    </row>
-    <row r="37" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="35"/>
-    </row>
-  </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="A1:A37"/>
-    <mergeCell ref="B1:B27"/>
-    <mergeCell ref="C1:C26"/>
-    <mergeCell ref="D1:D4"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="D5:D17"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E6:E12"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="B28:B30"/>
-  </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B9" colorId="64" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="77.42"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="20" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="20" width="39.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="20" width="95.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="20" width="60.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="20" width="58.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="20" width="50"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="20" width="49.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="8" style="20" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>43</v>
+    <row r="1" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="20" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="20" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="20" t="n">
+        <v>4</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="20" t="n">
+        <v>5</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="20" t="n">
+        <v>6</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="256.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="20" t="n">
+        <v>7</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="245.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="20" t="n">
+        <v>8</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="223.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="20" t="n">
+        <v>9</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="243.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="20" t="n">
+        <v>10</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="288.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B14" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="G14" s="23" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="240.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B16" s="20" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D10" r:id="rId1" display="https://topdev.vn/blog/trien-khai-ci-cd-voi-gitlab/"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -3928,6 +5313,7 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3944,278 +5330,278 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="72.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="139.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="26" width="72.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="27" width="139.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B1" s="9"/>
+      <c r="A1" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="28"/>
     </row>
     <row r="2" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>46</v>
+      <c r="A2" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>48</v>
+      <c r="A3" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>50</v>
+      <c r="A4" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>52</v>
+      <c r="A5" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" s="12"/>
+      <c r="A8" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="B8" s="31"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>55</v>
+      <c r="A9" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="B9" s="33" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>57</v>
+      <c r="A10" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10" s="33" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>59</v>
+      <c r="A11" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="B11" s="35" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>61</v>
+      <c r="A12" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="B12" s="33" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>63</v>
+      <c r="A13" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="B13" s="33" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>65</v>
+      <c r="A14" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="B14" s="33" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>67</v>
+      <c r="A15" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="B15" s="33" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>69</v>
+      <c r="A16" s="33" t="s">
+        <v>126</v>
+      </c>
+      <c r="B16" s="33" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>71</v>
+      <c r="A17" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="B17" s="33" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="B18" s="14" t="s">
-        <v>73</v>
+      <c r="A18" s="33" t="s">
+        <v>130</v>
+      </c>
+      <c r="B18" s="33" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>75</v>
+      <c r="A19" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="B19" s="33" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>77</v>
+      <c r="A20" s="33" t="s">
+        <v>134</v>
+      </c>
+      <c r="B20" s="33" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>79</v>
+      <c r="A21" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="B21" s="33" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="B25" s="9"/>
+      <c r="A25" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="B25" s="28"/>
     </row>
     <row r="26" customFormat="false" ht="283.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>82</v>
+      <c r="A26" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>84</v>
+      <c r="A27" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="B27" s="29" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>86</v>
+      <c r="A28" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="B28" s="29" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>88</v>
+      <c r="A29" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="B29" s="29" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>90</v>
+      <c r="A30" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="B30" s="29" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>92</v>
+      <c r="A31" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="B31" s="29" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>94</v>
+      <c r="A32" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="B32" s="29" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>96</v>
+      <c r="A33" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="B33" s="29" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>98</v>
+      <c r="A34" s="37" t="s">
+        <v>155</v>
+      </c>
+      <c r="B34" s="29" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="18"/>
-      <c r="B35" s="10" t="s">
-        <v>99</v>
+      <c r="A35" s="37"/>
+      <c r="B35" s="29" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="18"/>
-      <c r="B36" s="10" t="s">
-        <v>100</v>
+      <c r="A36" s="37"/>
+      <c r="B36" s="29" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="18"/>
-      <c r="B37" s="10" t="s">
-        <v>101</v>
+      <c r="A37" s="37"/>
+      <c r="B37" s="29" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="18"/>
-      <c r="B38" s="10" t="s">
-        <v>102</v>
+      <c r="A38" s="37"/>
+      <c r="B38" s="29" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="18"/>
-      <c r="B39" s="11" t="s">
-        <v>103</v>
+      <c r="A39" s="37"/>
+      <c r="B39" s="30" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="18"/>
-      <c r="B40" s="10" t="s">
-        <v>104</v>
+      <c r="A40" s="37"/>
+      <c r="B40" s="29" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="B41" s="11" t="s">
-        <v>106</v>
+      <c r="A41" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="B41" s="30" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -4243,7 +5629,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I25" activeCellId="0" sqref="I25"/>
+      <selection pane="topLeft" activeCell="Q31" activeCellId="0" sqref="Q31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4263,40 +5649,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="60.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="20" width="37.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="20" width="77.42"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
-        <v>110</v>
+    <row r="1" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -4315,6 +5693,58 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="27" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="27" width="60.42"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="27" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="27" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="27" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="27" t="s">
+        <v>172</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A29" colorId="64" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -4323,241 +5753,241 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="28.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="49.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="69.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="27" width="28.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="27" width="49.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="27" width="69.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="B1" s="20" t="s">
-        <v>112</v>
+      <c r="A1" s="38" t="s">
+        <v>173</v>
+      </c>
+      <c r="B1" s="39" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="21"/>
+      <c r="A2" s="40"/>
     </row>
     <row r="3" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="22" t="s">
-        <v>113</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>114</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>115</v>
+      <c r="A3" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="B3" s="42" t="s">
+        <v>176</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="22"/>
-      <c r="B4" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>117</v>
+      <c r="A4" s="41"/>
+      <c r="B4" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="22"/>
-      <c r="B5" s="8" t="s">
-        <v>118</v>
+      <c r="A5" s="41"/>
+      <c r="B5" s="27" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="22"/>
-      <c r="B6" s="8" t="s">
-        <v>119</v>
+      <c r="A6" s="41"/>
+      <c r="B6" s="27" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="22"/>
-      <c r="B7" s="8" t="s">
-        <v>120</v>
+      <c r="A7" s="41"/>
+      <c r="B7" s="27" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="22"/>
-      <c r="B8" s="24" t="s">
-        <v>121</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>122</v>
+      <c r="A8" s="41"/>
+      <c r="B8" s="43" t="s">
+        <v>183</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="22"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="10" t="s">
-        <v>123</v>
+      <c r="A9" s="41"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="29" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="22"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="10" t="s">
-        <v>124</v>
+      <c r="A10" s="41"/>
+      <c r="B10" s="43"/>
+      <c r="C10" s="29" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="22"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="8" t="s">
-        <v>125</v>
+      <c r="A11" s="41"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="27" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="22"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="10" t="s">
-        <v>126</v>
+      <c r="A12" s="41"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="29" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="22"/>
-      <c r="B13" s="8" t="s">
-        <v>127</v>
+      <c r="A13" s="41"/>
+      <c r="B13" s="27" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="216.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="22"/>
-      <c r="B14" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>129</v>
+      <c r="A14" s="41"/>
+      <c r="B14" s="44" t="s">
+        <v>190</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="22"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="26" t="s">
-        <v>130</v>
+      <c r="A15" s="41"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="45" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="22"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="26" t="s">
-        <v>131</v>
+      <c r="A16" s="41"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="45" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="22"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="26" t="s">
-        <v>132</v>
+      <c r="A17" s="41"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="45" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="22"/>
-      <c r="B18" s="25"/>
-      <c r="C18" s="10" t="s">
-        <v>133</v>
+      <c r="A18" s="41"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="29" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="22"/>
+      <c r="A19" s="41"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="22"/>
-      <c r="B20" s="27" t="s">
-        <v>134</v>
+      <c r="A20" s="41"/>
+      <c r="B20" s="46" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="22"/>
-      <c r="B21" s="8" t="s">
-        <v>135</v>
+      <c r="A21" s="41"/>
+      <c r="B21" s="27" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="21"/>
+      <c r="A22" s="40"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="21"/>
+      <c r="A23" s="40"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="22" t="s">
-        <v>136</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>137</v>
+      <c r="A24" s="41" t="s">
+        <v>198</v>
+      </c>
+      <c r="B24" s="27" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="22"/>
-      <c r="B25" s="8" t="s">
-        <v>138</v>
+      <c r="A25" s="41"/>
+      <c r="B25" s="27" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="22"/>
-      <c r="B26" s="8" t="s">
-        <v>139</v>
+      <c r="A26" s="41"/>
+      <c r="B26" s="27" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="22"/>
-      <c r="B27" s="8" t="s">
-        <v>140</v>
+      <c r="A27" s="41"/>
+      <c r="B27" s="27" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="22"/>
-      <c r="B28" s="10" t="s">
-        <v>141</v>
+      <c r="A28" s="41"/>
+      <c r="B28" s="29" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="22"/>
-      <c r="B29" s="10" t="s">
-        <v>142</v>
+      <c r="A29" s="41"/>
+      <c r="B29" s="29" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="28"/>
+      <c r="A30" s="47"/>
     </row>
     <row r="31" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="22" t="s">
-        <v>143</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="F31" s="29"/>
+      <c r="A31" s="41" t="s">
+        <v>205</v>
+      </c>
+      <c r="B31" s="29" t="s">
+        <v>206</v>
+      </c>
+      <c r="F31" s="48"/>
     </row>
     <row r="32" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="22"/>
-      <c r="B32" s="10" t="s">
-        <v>145</v>
+      <c r="A32" s="41"/>
+      <c r="B32" s="29" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="22"/>
-      <c r="B33" s="10" t="s">
-        <v>146</v>
+      <c r="A33" s="41"/>
+      <c r="B33" s="29" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="22"/>
-      <c r="B34" s="10" t="s">
-        <v>147</v>
+      <c r="A34" s="41"/>
+      <c r="B34" s="29" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="22"/>
-      <c r="B35" s="10" t="s">
-        <v>148</v>
+      <c r="A35" s="41"/>
+      <c r="B35" s="29" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="22"/>
-      <c r="B36" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="C36" s="10"/>
+      <c r="A36" s="41"/>
+      <c r="B36" s="29" t="s">
+        <v>211</v>
+      </c>
+      <c r="C36" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -4577,7 +6007,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -4600,7 +6030,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -4621,57 +6051,4 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="57.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="3" style="1" width="9.14"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>155</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
[feat][OS][Operating System: Resources management]
</commit_message>
<xml_diff>
--- a/Operations-System/DevOps-Documents.xlsx
+++ b/Operations-System/DevOps-Documents.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="223">
   <si>
     <t xml:space="preserve">Operating System Concepts</t>
   </si>
@@ -401,6 +401,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> - The CPU can load </t>
     </r>
@@ -411,6 +412,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">instructions</t>
     </r>
@@ -420,6 +422,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> only from memory, so any programs must first be loaded into memory to run. 
  - General-purpose computers run most of their programs from rewritable memory, called main memory (also called random-access memory, or RAM). RAM is volatile—loses its content when power is turned off or otherwise lost
@@ -432,6 +435,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">EEPROM</t>
     </r>
@@ -441,6 +445,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">) and other forms of </t>
     </r>
@@ -451,6 +456,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">firmwar</t>
     </r>
@@ -460,6 +466,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> —storage that is infrequently(not often) written to and is nonvolatile.
  - All forms of memory provide an array of bytes. Each byte has its own address.  Interaction is achieved through a sequence of load or store instructions to specific memory addresses.  The load instruction moves a byte or word from main memory to an internal register within the CPU, whereas the store instruction moves the content of a register to main memory. 
@@ -473,6 +480,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">instruction register</t>
     </r>
@@ -482,6 +490,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">.
   + Decode instruction stored in some internal register.
@@ -495,6 +504,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">permanently</t>
     </r>
@@ -504,6 +514,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(vĩnh viễn) because volatile and small → We need </t>
     </r>
@@ -514,6 +525,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">secondary storage</t>
     </r>
@@ -523,6 +535,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(hard-disk drives, nonvolatile memory(NVM) devices, ...).
  </t>
@@ -534,6 +547,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">→</t>
     </r>
@@ -543,6 +557,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">  The main differences among the various storage systems lie in speed, size, and volatility. The trade-off between size and speed, with smaller and faster memory closer to the
 CPU.</t>
@@ -568,6 +583,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">eneral-purpose computer system consists of multiple devices, all of which exchange data via a common bus. </t>
     </r>
@@ -734,6 +750,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">eer CPU processor performs all tasks, including operating-system functions and user processes.
   + Many processes can run simultaneously N processes can run if there are N CPUs without causing performance to deteriorate significantly.
@@ -746,6 +763,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Now</t>
     </r>
@@ -755,6 +773,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">:
  - The definition of multiprocessor has evolved over time and now includes multicore systems, in which </t>
@@ -766,6 +785,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">multiple computing cores reside on a single chip</t>
     </r>
@@ -775,6 +795,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">.
   + Multicore systems can be more efficient than multiple chips with single cores because on-chip communication is faster than between-chip communication.
@@ -803,6 +824,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">- Processor: A physical chip that contains one or more CPUs.
 </t>
@@ -1148,6 +1170,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ncreases CPU utilization</t>
     </r>
@@ -1157,6 +1180,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">, as well as keeping users satisfied, by organizing programs so that the CPU always has one to execute.
   + A program in execution is termed a </t>
@@ -1168,6 +1192,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">process</t>
     </r>
@@ -1177,6 +1202,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">.
   + When that process needs to wait, the CPU switches to another process, and so on. Eventually, the first process finishes waiting and gets the CPU back.
@@ -1190,6 +1216,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Multitasking</t>
     </r>
@@ -1199,6 +1226,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">:
   + Multitasking is the capability of an operating system to execute more than one task </t>
@@ -1210,6 +1238,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">concurrently</t>
     </r>
@@ -1219,6 +1248,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">. 
   + In a single-processor system, this is achieved by </t>
@@ -1230,6 +1260,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">rapidly context switching between tasks,</t>
     </r>
@@ -1239,6 +1270,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> giving the user the illusion that tasks are </t>
     </r>
@@ -1249,6 +1281,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">running simultaneously</t>
     </r>
@@ -1258,6 +1291,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">.
   + The OS divides CPU time into small slices (time-sharing). When one task’s time slice expires, the OS saves its state (context) and switches to another task, making it appear that tasks run in parallel.
@@ -1499,6 +1533,148 @@
     <t xml:space="preserve">Resource Management</t>
   </si>
   <si>
+    <t xml:space="preserve">Process Management</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> - A program(</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">passive entity</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">) include instructions(các lệnh/ các phép toán).
+ - A CPU execute instruction → process
+ - A process(</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">active entity</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">) to be an instance of a program in execution. Process execute instructions one by one (sequential) by </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">program counter</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> specifying the next instruction.
+ - At any time, </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">1 instruction at most is executed on behalf of process</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> → 2 processes may be associated with the same program, they are nevertheless considered 2 </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">separate execution sequences</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">.
+ - A process needs certain resources(physical and logical)-including CPU time, memory, files, and I/O devices-to accomplish its task. When the process terminates, the OS will reclaim resources.
+ - A process is unit of work in a system(OS processes and user processes) these processes can potentially execute concurrently—by multiplexing on a single CPU core—or in parallel across multiple CPU cores.
+ - The operating system is responsible for the following activities in connection with process management:
+  + Create and deleting both user and system processes.
+  + Scheduling processes and threads on the CPUs.
+  + Suspending and resuming processes.
+  + Providing mechanisms for process sync and communication.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Memory Management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">File-System Management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mass-Storage Management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I/O System Management</t>
+  </si>
+  <si>
     <t xml:space="preserve">Security and Protection</t>
   </si>
   <si>
@@ -1518,9 +1694,6 @@
   </si>
   <si>
     <t xml:space="preserve">Operating-System Structure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Process Management</t>
   </si>
   <si>
     <t xml:space="preserve">Processes</t>
@@ -3706,7 +3879,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="30">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3800,6 +3973,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -3807,6 +3981,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -3814,12 +3989,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -3975,17 +4145,17 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="47">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4042,15 +4212,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4058,11 +4220,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4070,11 +4232,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4082,15 +4244,15 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4098,7 +4260,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4110,11 +4272,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4122,7 +4284,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4130,19 +4292,19 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4150,7 +4312,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="24" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4158,7 +4320,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4166,19 +4328,19 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4268,9 +4430,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>588600</xdr:colOff>
+      <xdr:colOff>587880</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>2121480</xdr:rowOff>
+      <xdr:rowOff>2120760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4284,7 +4446,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10237320" y="8324640"/>
-          <a:ext cx="4801320" cy="2798640"/>
+          <a:ext cx="4800600" cy="2797920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4305,9 +4467,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>664920</xdr:colOff>
+      <xdr:colOff>664200</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>1797480</xdr:rowOff>
+      <xdr:rowOff>1796760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4321,7 +4483,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10323000" y="11420280"/>
-          <a:ext cx="4791960" cy="2493720"/>
+          <a:ext cx="4791240" cy="2493000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4342,9 +4504,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>522000</xdr:colOff>
+      <xdr:colOff>521280</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>696240</xdr:rowOff>
+      <xdr:rowOff>695520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4358,7 +4520,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10170720" y="24355440"/>
-          <a:ext cx="4801320" cy="2903400"/>
+          <a:ext cx="4800600" cy="2902680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4550,10 +4712,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G1048576"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D25" colorId="64" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G31" activeCellId="0" sqref="G31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D20" colorId="64" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="36.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4693,13 +4855,13 @@
       <c r="B10" s="7"/>
       <c r="C10" s="8"/>
       <c r="D10" s="9"/>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="11" t="s">
         <v>20</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="5" t="s">
         <v>22</v>
       </c>
     </row>
@@ -4708,11 +4870,11 @@
       <c r="B11" s="7"/>
       <c r="C11" s="8"/>
       <c r="D11" s="9"/>
-      <c r="E11" s="12"/>
+      <c r="E11" s="11"/>
       <c r="F11" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="G11" s="14" t="s">
         <v>24</v>
       </c>
     </row>
@@ -4724,41 +4886,45 @@
       <c r="E12" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="F12" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="G12" s="16"/>
+      <c r="G12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="126.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="6"/>
       <c r="B13" s="7"/>
       <c r="C13" s="8"/>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="9" t="s">
         <v>27</v>
       </c>
       <c r="E13" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="10" t="s">
         <v>29</v>
       </c>
+      <c r="G13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="216.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="6"/>
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
-      <c r="E14" s="12" t="s">
+      <c r="D14" s="9"/>
+      <c r="E14" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="10" t="s">
         <v>31</v>
       </c>
+      <c r="G14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="126.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6"/>
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
-      <c r="E15" s="12"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="11"/>
       <c r="F15" s="12" t="s">
         <v>32</v>
       </c>
@@ -4770,59 +4936,66 @@
       <c r="A16" s="6"/>
       <c r="B16" s="7"/>
       <c r="C16" s="8"/>
+      <c r="D16" s="9"/>
       <c r="E16" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F16" s="10" t="s">
         <v>35</v>
       </c>
+      <c r="G16" s="10"/>
     </row>
     <row r="17" customFormat="false" ht="133.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="6"/>
       <c r="B17" s="7"/>
       <c r="C17" s="8"/>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="10" t="s">
         <v>37</v>
       </c>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
     </row>
     <row r="18" customFormat="false" ht="335" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="6"/>
       <c r="B18" s="7"/>
       <c r="C18" s="8"/>
-      <c r="E18" s="17" t="s">
+      <c r="D18" s="9"/>
+      <c r="E18" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="F18" s="16" t="s">
+      <c r="F18" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="16"/>
+      <c r="G18" s="10"/>
     </row>
     <row r="19" customFormat="false" ht="144.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="6"/>
       <c r="B19" s="7"/>
       <c r="C19" s="8"/>
+      <c r="D19" s="9"/>
       <c r="E19" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="F19" s="16" t="s">
+      <c r="F19" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="G19" s="16"/>
+      <c r="G19" s="10"/>
     </row>
     <row r="20" customFormat="false" ht="73.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="6"/>
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
-      <c r="E20" s="18" t="s">
+      <c r="D20" s="9"/>
+      <c r="E20" s="16" t="s">
         <v>42</v>
       </c>
       <c r="F20" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="G20" s="19" t="s">
+      <c r="G20" s="17" t="s">
         <v>44</v>
       </c>
     </row>
@@ -4830,8 +5003,9 @@
       <c r="A21" s="6"/>
       <c r="B21" s="7"/>
       <c r="C21" s="8"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="12" t="s">
+      <c r="D21" s="9"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="11" t="s">
         <v>45</v>
       </c>
       <c r="G21" s="5" t="s">
@@ -4842,8 +5016,9 @@
       <c r="A22" s="6"/>
       <c r="B22" s="7"/>
       <c r="C22" s="8"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="12"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="11"/>
       <c r="G22" s="5" t="s">
         <v>47</v>
       </c>
@@ -4852,8 +5027,9 @@
       <c r="A23" s="6"/>
       <c r="B23" s="7"/>
       <c r="C23" s="8"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="12"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="11"/>
       <c r="G23" s="5" t="s">
         <v>48</v>
       </c>
@@ -4862,50 +5038,61 @@
       <c r="A24" s="6"/>
       <c r="B24" s="7"/>
       <c r="C24" s="8"/>
+      <c r="D24" s="9"/>
       <c r="E24" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-    </row>
-    <row r="25" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+    </row>
+    <row r="25" customFormat="false" ht="220.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="6"/>
       <c r="B25" s="7"/>
       <c r="C25" s="8"/>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="9" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E25" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="6"/>
       <c r="B26" s="7"/>
       <c r="C26" s="8"/>
-      <c r="D26" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D26" s="9"/>
+      <c r="E26" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="6"/>
       <c r="B27" s="7"/>
       <c r="C27" s="8"/>
-      <c r="D27" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D27" s="9"/>
+      <c r="E27" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="56.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="6"/>
       <c r="B28" s="7"/>
       <c r="C28" s="8"/>
-      <c r="D28" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D28" s="9"/>
+      <c r="E28" s="12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="6"/>
       <c r="B29" s="7"/>
       <c r="C29" s="8"/>
-      <c r="D29" s="4" t="s">
-        <v>54</v>
+      <c r="D29" s="9"/>
+      <c r="E29" s="12" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4913,58 +5100,78 @@
       <c r="B30" s="7"/>
       <c r="C30" s="8"/>
       <c r="D30" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="88.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="6"/>
       <c r="B31" s="7"/>
       <c r="C31" s="8"/>
       <c r="D31" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="75.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="6"/>
       <c r="B32" s="7"/>
-      <c r="C32" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C32" s="8"/>
+      <c r="D32" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="6"/>
-      <c r="B33" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="75.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="7"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="6"/>
       <c r="B34" s="7"/>
-      <c r="C34" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C34" s="8"/>
+      <c r="D34" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="88.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="6"/>
       <c r="B35" s="7"/>
-      <c r="C35" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C35" s="8"/>
+      <c r="D35" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="75.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="6"/>
-    </row>
-    <row r="37" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="7"/>
+      <c r="C36" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="6"/>
-    </row>
-    <row r="38" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="75.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="6"/>
-    </row>
-    <row r="39" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="7"/>
+      <c r="C38" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="6"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="3" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="6"/>
@@ -4975,13 +5182,23 @@
     <row r="42" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="6"/>
     </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="43" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="6"/>
+    </row>
+    <row r="44" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="6"/>
+    </row>
+    <row r="45" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="6"/>
+    </row>
+    <row r="46" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="A1:A42"/>
-    <mergeCell ref="B1:B32"/>
-    <mergeCell ref="C1:C31"/>
+  <mergeCells count="29">
+    <mergeCell ref="A1:A46"/>
+    <mergeCell ref="B1:B36"/>
+    <mergeCell ref="C1:C35"/>
     <mergeCell ref="D1:D4"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="F2:G2"/>
@@ -5005,7 +5222,9 @@
     <mergeCell ref="E20:E23"/>
     <mergeCell ref="F21:F23"/>
     <mergeCell ref="F24:G24"/>
-    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="D25:D29"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="B37:B39"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
@@ -5030,33 +5249,33 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="20" width="23.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="20" width="57.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="3" style="20" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="18" width="23.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="18" width="57.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="3" style="18" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="20" t="s">
-        <v>212</v>
-      </c>
-      <c r="B1" s="23" t="s">
-        <v>213</v>
+      <c r="A1" s="18" t="s">
+        <v>217</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="23" t="s">
-        <v>214</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>215</v>
+      <c r="A2" s="21" t="s">
+        <v>219</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="23" t="s">
-        <v>216</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>217</v>
+      <c r="A3" s="21" t="s">
+        <v>221</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -5106,200 +5325,200 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="20" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="20" width="39.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="20" width="95.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="20" width="60.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="20" width="58.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="20" width="50"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="20" width="49.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="8" style="20" width="9.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="18" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="18" width="39.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="18" width="95.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="18" width="60.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="18" width="58.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="18" width="50"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="18" width="49.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="8" style="18" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="20" t="n">
+      <c r="A1" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="B1" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="C1" s="21" t="s">
-        <v>63</v>
+      <c r="B1" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="20" t="n">
+      <c r="A2" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="B2" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>65</v>
+      <c r="B2" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="20" t="n">
+      <c r="A3" s="18" t="n">
         <v>3</v>
       </c>
-      <c r="B3" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>67</v>
+      <c r="B3" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="20" t="n">
+      <c r="A4" s="18" t="n">
         <v>4</v>
       </c>
-      <c r="B4" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>69</v>
+      <c r="B4" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="20" t="n">
+      <c r="A5" s="18" t="n">
         <v>5</v>
       </c>
-      <c r="B5" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>71</v>
+      <c r="B5" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="20" t="n">
+      <c r="A6" s="18" t="n">
         <v>6</v>
       </c>
-      <c r="B6" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="C6" s="23" t="s">
-        <v>73</v>
+      <c r="B6" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="256.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="20" t="n">
+      <c r="A7" s="18" t="n">
         <v>7</v>
       </c>
-      <c r="B7" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="C7" s="24" t="s">
-        <v>75</v>
+      <c r="B7" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="245.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="20" t="n">
+      <c r="A8" s="18" t="n">
         <v>8</v>
       </c>
-      <c r="B8" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="C8" s="21" t="s">
-        <v>77</v>
+      <c r="B8" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="223.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="20" t="n">
+      <c r="A9" s="18" t="n">
         <v>9</v>
       </c>
-      <c r="B9" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>79</v>
+      <c r="B9" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="243.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="20" t="n">
+      <c r="A10" s="18" t="n">
         <v>10</v>
       </c>
-      <c r="B10" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="D10" s="25" t="s">
-        <v>82</v>
+      <c r="B10" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="C11" s="23" t="s">
-        <v>84</v>
+      <c r="B11" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>86</v>
+      <c r="B12" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="C13" s="23" t="s">
-        <v>88</v>
+      <c r="B13" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="288.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="C14" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="D14" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="E14" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="F14" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="G14" s="23" t="s">
+      <c r="B14" s="18" t="s">
         <v>94</v>
       </c>
+      <c r="C14" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="G14" s="21" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="C15" s="23" t="s">
-        <v>96</v>
+      <c r="B15" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="240.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="20" t="s">
-        <v>97</v>
+      <c r="B16" s="18" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="C17" s="21" t="s">
-        <v>99</v>
+      <c r="B17" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="C18" s="21" t="s">
-        <v>101</v>
+      <c r="B18" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -5330,278 +5549,278 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="26" width="72.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="27" width="139.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="24" width="72.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="139.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="28" t="s">
-        <v>102</v>
-      </c>
-      <c r="B1" s="28"/>
+      <c r="A1" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="26"/>
     </row>
     <row r="2" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="B2" s="29" t="s">
-        <v>104</v>
+      <c r="A2" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="26" t="s">
-        <v>105</v>
-      </c>
-      <c r="B3" s="30" t="s">
-        <v>106</v>
+      <c r="A3" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="B4" s="30" t="s">
-        <v>108</v>
+      <c r="A4" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="26" t="s">
-        <v>109</v>
-      </c>
-      <c r="B5" s="30" t="s">
-        <v>110</v>
+      <c r="A5" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="31" t="s">
-        <v>111</v>
-      </c>
-      <c r="B8" s="31"/>
+      <c r="A8" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" s="29"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="32" t="s">
-        <v>112</v>
-      </c>
-      <c r="B9" s="33" t="s">
-        <v>113</v>
+      <c r="A9" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="34" t="s">
-        <v>114</v>
-      </c>
-      <c r="B10" s="33" t="s">
-        <v>115</v>
+      <c r="A10" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="B10" s="31" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="34" t="s">
-        <v>116</v>
-      </c>
-      <c r="B11" s="35" t="s">
-        <v>117</v>
+      <c r="A11" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="B11" s="33" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="33" t="s">
-        <v>118</v>
-      </c>
-      <c r="B12" s="33" t="s">
-        <v>119</v>
+      <c r="A12" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="B12" s="31" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="33" t="s">
-        <v>120</v>
-      </c>
-      <c r="B13" s="33" t="s">
-        <v>121</v>
+      <c r="A13" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="B13" s="31" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="33" t="s">
-        <v>122</v>
-      </c>
-      <c r="B14" s="33" t="s">
-        <v>123</v>
+      <c r="A14" s="31" t="s">
+        <v>127</v>
+      </c>
+      <c r="B14" s="31" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="33" t="s">
-        <v>124</v>
-      </c>
-      <c r="B15" s="33" t="s">
-        <v>125</v>
+      <c r="A15" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="B15" s="31" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="33" t="s">
-        <v>126</v>
-      </c>
-      <c r="B16" s="33" t="s">
-        <v>127</v>
+      <c r="A16" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="B16" s="31" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="33" t="s">
-        <v>128</v>
-      </c>
-      <c r="B17" s="33" t="s">
-        <v>129</v>
+      <c r="A17" s="31" t="s">
+        <v>133</v>
+      </c>
+      <c r="B17" s="31" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="33" t="s">
-        <v>130</v>
-      </c>
-      <c r="B18" s="33" t="s">
-        <v>131</v>
+      <c r="A18" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="B18" s="31" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="33" t="s">
-        <v>132</v>
-      </c>
-      <c r="B19" s="33" t="s">
-        <v>133</v>
+      <c r="A19" s="31" t="s">
+        <v>137</v>
+      </c>
+      <c r="B19" s="31" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="33" t="s">
-        <v>134</v>
-      </c>
-      <c r="B20" s="33" t="s">
-        <v>135</v>
+      <c r="A20" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="B20" s="31" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="33" t="s">
-        <v>136</v>
-      </c>
-      <c r="B21" s="33" t="s">
-        <v>137</v>
+      <c r="A21" s="31" t="s">
+        <v>141</v>
+      </c>
+      <c r="B21" s="31" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="28" t="s">
-        <v>138</v>
-      </c>
-      <c r="B25" s="28"/>
+      <c r="A25" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="B25" s="26"/>
     </row>
     <row r="26" customFormat="false" ht="283.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="26" t="s">
-        <v>139</v>
-      </c>
-      <c r="B26" s="29" t="s">
-        <v>140</v>
+      <c r="A26" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="B26" s="27" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="26" t="s">
-        <v>141</v>
-      </c>
-      <c r="B27" s="29" t="s">
-        <v>142</v>
+      <c r="A27" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="B27" s="27" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="36" t="s">
-        <v>143</v>
-      </c>
-      <c r="B28" s="29" t="s">
-        <v>144</v>
+      <c r="A28" s="34" t="s">
+        <v>148</v>
+      </c>
+      <c r="B28" s="27" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="26" t="s">
-        <v>145</v>
-      </c>
-      <c r="B29" s="29" t="s">
-        <v>146</v>
+      <c r="A29" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="B29" s="27" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="26" t="s">
-        <v>147</v>
-      </c>
-      <c r="B30" s="29" t="s">
-        <v>148</v>
+      <c r="A30" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="B30" s="27" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="26" t="s">
-        <v>149</v>
-      </c>
-      <c r="B31" s="29" t="s">
-        <v>150</v>
+      <c r="A31" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="B31" s="27" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="26" t="s">
-        <v>151</v>
-      </c>
-      <c r="B32" s="29" t="s">
-        <v>152</v>
+      <c r="A32" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="B32" s="27" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="26" t="s">
-        <v>153</v>
-      </c>
-      <c r="B33" s="29" t="s">
-        <v>154</v>
+      <c r="A33" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="B33" s="27" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="37" t="s">
-        <v>155</v>
-      </c>
-      <c r="B34" s="29" t="s">
-        <v>156</v>
+      <c r="A34" s="35" t="s">
+        <v>160</v>
+      </c>
+      <c r="B34" s="27" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="37"/>
-      <c r="B35" s="29" t="s">
-        <v>157</v>
+      <c r="A35" s="35"/>
+      <c r="B35" s="27" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="37"/>
-      <c r="B36" s="29" t="s">
-        <v>158</v>
+      <c r="A36" s="35"/>
+      <c r="B36" s="27" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="37"/>
-      <c r="B37" s="29" t="s">
-        <v>159</v>
+      <c r="A37" s="35"/>
+      <c r="B37" s="27" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="37"/>
-      <c r="B38" s="29" t="s">
-        <v>160</v>
+      <c r="A38" s="35"/>
+      <c r="B38" s="27" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="37"/>
-      <c r="B39" s="30" t="s">
-        <v>161</v>
+      <c r="A39" s="35"/>
+      <c r="B39" s="28" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="37"/>
-      <c r="B40" s="29" t="s">
-        <v>162</v>
+      <c r="A40" s="35"/>
+      <c r="B40" s="27" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="26" t="s">
-        <v>163</v>
-      </c>
-      <c r="B41" s="30" t="s">
-        <v>164</v>
+      <c r="A41" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="B41" s="28" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -5657,24 +5876,24 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="20" width="37.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="20" width="77.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="18" width="37.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="18" width="77.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="23" t="s">
-        <v>165</v>
-      </c>
-      <c r="B1" s="23" t="s">
-        <v>166</v>
+      <c r="A1" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="20" t="s">
-        <v>167</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>168</v>
+      <c r="A2" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -5701,32 +5920,32 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="27" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="27" width="60.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="25" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="60.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="27" t="s">
-        <v>169</v>
+      <c r="A2" s="25" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="27" t="s">
-        <v>170</v>
+      <c r="A4" s="25" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="27" t="s">
-        <v>171</v>
+      <c r="A6" s="25" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="27" t="s">
-        <v>172</v>
+      <c r="A8" s="25" t="s">
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -5753,241 +5972,241 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="27" width="28.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="27" width="49.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="27" width="69.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="25" width="28.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="49.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="25" width="69.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="38" t="s">
-        <v>173</v>
-      </c>
-      <c r="B1" s="39" t="s">
-        <v>174</v>
+      <c r="A1" s="36" t="s">
+        <v>178</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="40"/>
+      <c r="A2" s="38"/>
     </row>
     <row r="3" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="B3" s="42" t="s">
-        <v>176</v>
-      </c>
-      <c r="C3" s="29" t="s">
-        <v>177</v>
+      <c r="A3" s="39" t="s">
+        <v>180</v>
+      </c>
+      <c r="B3" s="40" t="s">
+        <v>181</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="41"/>
-      <c r="B4" s="42" t="s">
-        <v>178</v>
-      </c>
-      <c r="C4" s="29" t="s">
-        <v>179</v>
+      <c r="A4" s="39"/>
+      <c r="B4" s="40" t="s">
+        <v>183</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="41"/>
-      <c r="B5" s="27" t="s">
-        <v>180</v>
+      <c r="A5" s="39"/>
+      <c r="B5" s="25" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="41"/>
-      <c r="B6" s="27" t="s">
-        <v>181</v>
+      <c r="A6" s="39"/>
+      <c r="B6" s="25" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="41"/>
-      <c r="B7" s="27" t="s">
-        <v>182</v>
+      <c r="A7" s="39"/>
+      <c r="B7" s="25" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="41"/>
-      <c r="B8" s="43" t="s">
-        <v>183</v>
-      </c>
-      <c r="C8" s="29" t="s">
-        <v>184</v>
+      <c r="A8" s="39"/>
+      <c r="B8" s="41" t="s">
+        <v>188</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="41"/>
-      <c r="B9" s="43"/>
-      <c r="C9" s="29" t="s">
-        <v>185</v>
+      <c r="A9" s="39"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="27" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="41"/>
-      <c r="B10" s="43"/>
-      <c r="C10" s="29" t="s">
-        <v>186</v>
+      <c r="A10" s="39"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="27" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="41"/>
-      <c r="B11" s="43"/>
-      <c r="C11" s="27" t="s">
-        <v>187</v>
+      <c r="A11" s="39"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="25" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="41"/>
-      <c r="B12" s="43"/>
-      <c r="C12" s="29" t="s">
-        <v>188</v>
+      <c r="A12" s="39"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="27" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="41"/>
-      <c r="B13" s="27" t="s">
-        <v>189</v>
+      <c r="A13" s="39"/>
+      <c r="B13" s="25" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="216.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="41"/>
-      <c r="B14" s="44" t="s">
-        <v>190</v>
-      </c>
-      <c r="C14" s="29" t="s">
-        <v>191</v>
+      <c r="A14" s="39"/>
+      <c r="B14" s="42" t="s">
+        <v>195</v>
+      </c>
+      <c r="C14" s="27" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="41"/>
-      <c r="B15" s="44"/>
-      <c r="C15" s="45" t="s">
-        <v>192</v>
+      <c r="A15" s="39"/>
+      <c r="B15" s="42"/>
+      <c r="C15" s="43" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="41"/>
-      <c r="B16" s="44"/>
-      <c r="C16" s="45" t="s">
-        <v>193</v>
+      <c r="A16" s="39"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="43" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="41"/>
-      <c r="B17" s="44"/>
-      <c r="C17" s="45" t="s">
-        <v>194</v>
+      <c r="A17" s="39"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="43" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="41"/>
-      <c r="B18" s="44"/>
-      <c r="C18" s="29" t="s">
-        <v>195</v>
+      <c r="A18" s="39"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="27" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="41"/>
+      <c r="A19" s="39"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="41"/>
-      <c r="B20" s="46" t="s">
-        <v>196</v>
+      <c r="A20" s="39"/>
+      <c r="B20" s="44" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="41"/>
-      <c r="B21" s="27" t="s">
-        <v>197</v>
+      <c r="A21" s="39"/>
+      <c r="B21" s="25" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="40"/>
+      <c r="A22" s="38"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="40"/>
+      <c r="A23" s="38"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="41" t="s">
-        <v>198</v>
-      </c>
-      <c r="B24" s="27" t="s">
-        <v>199</v>
+      <c r="A24" s="39" t="s">
+        <v>203</v>
+      </c>
+      <c r="B24" s="25" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="41"/>
-      <c r="B25" s="27" t="s">
-        <v>200</v>
+      <c r="A25" s="39"/>
+      <c r="B25" s="25" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="41"/>
-      <c r="B26" s="27" t="s">
-        <v>201</v>
+      <c r="A26" s="39"/>
+      <c r="B26" s="25" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="41"/>
-      <c r="B27" s="27" t="s">
-        <v>202</v>
+      <c r="A27" s="39"/>
+      <c r="B27" s="25" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="41"/>
-      <c r="B28" s="29" t="s">
-        <v>203</v>
+      <c r="A28" s="39"/>
+      <c r="B28" s="27" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="41"/>
-      <c r="B29" s="29" t="s">
-        <v>204</v>
+      <c r="A29" s="39"/>
+      <c r="B29" s="27" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="47"/>
+      <c r="A30" s="45"/>
     </row>
     <row r="31" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="41" t="s">
-        <v>205</v>
-      </c>
-      <c r="B31" s="29" t="s">
-        <v>206</v>
-      </c>
-      <c r="F31" s="48"/>
+      <c r="A31" s="39" t="s">
+        <v>210</v>
+      </c>
+      <c r="B31" s="27" t="s">
+        <v>211</v>
+      </c>
+      <c r="F31" s="46"/>
     </row>
     <row r="32" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="41"/>
-      <c r="B32" s="29" t="s">
-        <v>207</v>
+      <c r="A32" s="39"/>
+      <c r="B32" s="27" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="41"/>
-      <c r="B33" s="29" t="s">
-        <v>208</v>
+      <c r="A33" s="39"/>
+      <c r="B33" s="27" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="41"/>
-      <c r="B34" s="29" t="s">
-        <v>209</v>
+      <c r="A34" s="39"/>
+      <c r="B34" s="27" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="41"/>
-      <c r="B35" s="29" t="s">
-        <v>210</v>
+      <c r="A35" s="39"/>
+      <c r="B35" s="27" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="41"/>
-      <c r="B36" s="29" t="s">
-        <v>211</v>
-      </c>
-      <c r="C36" s="29"/>
+      <c r="A36" s="39"/>
+      <c r="B36" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="C36" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
[feat][Docs][Java: NIO Buffer internally, OS: Virtualization]
</commit_message>
<xml_diff>
--- a/Operations-System/DevOps-Documents.xlsx
+++ b/Operations-System/DevOps-Documents.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="231">
   <si>
     <t xml:space="preserve">Operating System Concepts</t>
   </si>
@@ -1666,22 +1666,166 @@
     <t xml:space="preserve">Memory Management</t>
   </si>
   <si>
+    <t xml:space="preserve"> - Main memory is a large array of bytes. Is a repository of quickly accessible data shared by the CPU and I/O devices.
+ - The main memory is generally the only large storage device that the CPU is able to address and access directly. 
+ - Ex: CPU to process data from disk, those data must first be transferred to main memory by CPU-generated I/O calls. In the same way, instructions must be in memory for the CPU to execute them.</t>
+  </si>
+  <si>
     <t xml:space="preserve">File-System Management</t>
   </si>
   <si>
+    <t xml:space="preserve"> - File-system is logical view of information storage, abstracts form the physical properties of its storage devices to define a logical storage unit.
+ - Files represent programs (both source and object forms) and data. </t>
+  </si>
+  <si>
     <t xml:space="preserve">Mass-Storage Management</t>
   </si>
   <si>
+    <t xml:space="preserve">Cache Management</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> - </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">Caching</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> is an important principle of computer systems.
+ - In addition, internal programmable </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">registers</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> provide a high-speed cache for main memory. The programmer (or compiler) implements the register- allocation and register-replacement algorithms to decide which information to keep in registers and which to keep in main memory.
+ - Other caches are implemented totally in hardware.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve"> - Most systems have an instruction cache to hold the instructions expected to be executed next. Without this cache, the CPU would have to wait several cycles while an instruction was fetched from main memory.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> - Because caches have limited size, cache management is an important design problem. The movement of information between levels of a storage hierarchy may be
+either explicit or implicit, depending on the hardware design and the controlling operating-system software.
+ - In a hierarchical storage structure, the same data may appear in different levels of the storage system.
+ - Cache coherency.
+ - In a distributed environment: 
+  + Same file can be kept on different computers.
+  + Various replicas may be accessed and updated concurrently.
+  + Distributed systems ensure that, when a replica is updated in one place, all other replicas are brought up to date as soon as possible</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">I/O System Management</t>
   </si>
   <si>
+    <t xml:space="preserve"> - One of the purposes of an operating system is to hide the peculiarities of specific hardware devices from the user.
+ - Only the device driver knows the peculiarities of the specific device to which it is assigned.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Security and Protection</t>
   </si>
   <si>
+    <t xml:space="preserve"> - Multiple users and allows concurrent execution of multiple processes → resources authorization from OS.
+ - Protection: is any mechanism for controlling the access of processes or users to the resources defined by a computer system. Protection can improve reliability by detecting latent errors at the interfaces
+between component subsystems. A protection-oriented system provides a means to distinguish between authorized and unauthorized usage.
+ - Security: to defend a system from external and internal attacks
+ - Protection and security require the system to be able to distinguish among all its users: userID, groupID</t>
+  </si>
+  <si>
     <t xml:space="preserve">Virtualization</t>
   </si>
   <si>
+    <t xml:space="preserve"> - Virtualization is a technology that allows us to abstract(tách) the hardware of single computer into several different execution environments →  thereby creating the illusion(ảo giác, ảo hóa) that each separate environment is running on its own private computer.
+ - Virtualization allows operating systems to run as applications within other operating systems.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Distributed Systems</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> - A distributed system is a collection of physically separate, </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">possibly heterogeneous</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">(có thể không đồng nhất) computer systems that are networked to provide users with access to the various resources that the system maintains.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Kernel Data Structures</t>
@@ -3879,7 +4023,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="30">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3990,6 +4134,12 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -4145,13 +4295,13 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
@@ -4232,11 +4382,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4244,15 +4394,15 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4260,7 +4410,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4272,11 +4422,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4284,7 +4434,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4292,19 +4442,19 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4312,7 +4462,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="25" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4320,7 +4470,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4328,19 +4478,19 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4430,9 +4580,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>587880</xdr:colOff>
+      <xdr:colOff>587520</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>2120760</xdr:rowOff>
+      <xdr:rowOff>2120400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4446,7 +4596,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10237320" y="8324640"/>
-          <a:ext cx="4800600" cy="2797920"/>
+          <a:ext cx="4800240" cy="2797560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4467,9 +4617,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>664200</xdr:colOff>
+      <xdr:colOff>663840</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>1796760</xdr:rowOff>
+      <xdr:rowOff>1796400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4483,7 +4633,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10323000" y="11420280"/>
-          <a:ext cx="4791240" cy="2493000"/>
+          <a:ext cx="4790880" cy="2492640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4504,9 +4654,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>521280</xdr:colOff>
+      <xdr:colOff>520920</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>695520</xdr:rowOff>
+      <xdr:rowOff>695160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4520,7 +4670,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10170720" y="24355440"/>
-          <a:ext cx="4800600" cy="2902680"/>
+          <a:ext cx="4800240" cy="2902320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4712,10 +4862,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D20" colorId="64" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D30" colorId="64" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E32" activeCellId="0" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="36.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5055,11 +5205,12 @@
       <c r="E25" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="F25" s="10" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G25" s="10"/>
+    </row>
+    <row r="26" customFormat="false" ht="55.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="6"/>
       <c r="B26" s="7"/>
       <c r="C26" s="8"/>
@@ -5067,64 +5218,86 @@
       <c r="E26" s="12" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F26" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="38.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="6"/>
       <c r="B27" s="7"/>
       <c r="C27" s="8"/>
       <c r="D27" s="9"/>
       <c r="E27" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="56.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>55</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="6"/>
       <c r="B28" s="7"/>
       <c r="C28" s="8"/>
       <c r="D28" s="9"/>
       <c r="E28" s="12" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="257.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="6"/>
       <c r="B29" s="7"/>
       <c r="C29" s="8"/>
       <c r="D29" s="9"/>
       <c r="E29" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>58</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="38.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="6"/>
       <c r="B30" s="7"/>
       <c r="C30" s="8"/>
-      <c r="D30" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D30" s="9"/>
+      <c r="E30" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="106.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="6"/>
       <c r="B31" s="7"/>
       <c r="C31" s="8"/>
       <c r="D31" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>62</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="56.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="6"/>
       <c r="B32" s="7"/>
       <c r="C32" s="8"/>
       <c r="D32" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>64</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="46" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="6"/>
       <c r="B33" s="7"/>
       <c r="C33" s="8"/>
       <c r="D33" s="4" t="s">
-        <v>60</v>
+        <v>66</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5132,49 +5305,54 @@
       <c r="B34" s="7"/>
       <c r="C34" s="8"/>
       <c r="D34" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="88.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="6"/>
       <c r="B35" s="7"/>
       <c r="C35" s="8"/>
       <c r="D35" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="75.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="88.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="6"/>
       <c r="B36" s="7"/>
-      <c r="C36" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C36" s="8"/>
+      <c r="D36" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="75.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="6"/>
-      <c r="B37" s="7" t="s">
+      <c r="B37" s="7"/>
+      <c r="C37" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="6"/>
+      <c r="B38" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="75.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="6"/>
-      <c r="B38" s="7"/>
       <c r="C38" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="75.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="6"/>
       <c r="B39" s="7"/>
       <c r="C39" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="6"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="3" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="6"/>
@@ -5194,11 +5372,14 @@
     <row r="46" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="6"/>
     </row>
+    <row r="47" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="29">
-    <mergeCell ref="A1:A46"/>
-    <mergeCell ref="B1:B36"/>
-    <mergeCell ref="C1:C35"/>
+  <mergeCells count="37">
+    <mergeCell ref="A1:A47"/>
+    <mergeCell ref="B1:B37"/>
+    <mergeCell ref="C1:C36"/>
     <mergeCell ref="D1:D4"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="F2:G2"/>
@@ -5222,9 +5403,17 @@
     <mergeCell ref="E20:E23"/>
     <mergeCell ref="F21:F23"/>
     <mergeCell ref="F24:G24"/>
-    <mergeCell ref="D25:D29"/>
+    <mergeCell ref="D25:D30"/>
     <mergeCell ref="F25:G25"/>
-    <mergeCell ref="B37:B39"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="B38:B40"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
@@ -5256,26 +5445,26 @@
   <sheetData>
     <row r="1" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="18" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="21" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="21" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -5340,10 +5529,10 @@
         <v>1</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5351,10 +5540,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5362,10 +5551,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5373,10 +5562,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5384,10 +5573,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5395,10 +5584,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="256.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5406,10 +5595,10 @@
         <v>7</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="245.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5417,10 +5606,10 @@
         <v>8</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="223.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5428,10 +5617,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="243.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5439,86 +5628,86 @@
         <v>10</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="18" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="18" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="18" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="288.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="18" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="E14" s="21" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="F14" s="21" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="G14" s="21" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="18" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="240.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B16" s="18" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="18" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="18" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -5555,272 +5744,272 @@
   <sheetData>
     <row r="1" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="26" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="B1" s="26"/>
     </row>
     <row r="2" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="24" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="24" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="24" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="24" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="29" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="B8" s="29"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="30" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="32" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="32" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="B11" s="33" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="31" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="31" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="31" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="31" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="B15" s="31" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="31" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B16" s="31" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="31" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="B17" s="31" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="31" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="B18" s="31" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="31" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="B19" s="31" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="31" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="B20" s="31" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="31" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="B21" s="31" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="26" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="B25" s="26"/>
     </row>
     <row r="26" customFormat="false" ht="283.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="24" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="B26" s="27" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="24" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="B27" s="27" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="34" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="B28" s="27" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="24" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="B29" s="27" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="24" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="B30" s="27" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="24" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="B31" s="27" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="24" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="B32" s="27" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="24" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="B33" s="27" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="35" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="B34" s="27" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="35"/>
       <c r="B35" s="27" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="35"/>
       <c r="B36" s="27" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="35"/>
       <c r="B37" s="27" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="35"/>
       <c r="B38" s="27" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="35"/>
       <c r="B39" s="28" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="35"/>
       <c r="B40" s="27" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="24" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="B41" s="28" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -5882,18 +6071,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="21" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="18" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -5927,25 +6116,25 @@
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="25" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="25" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="25" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -5979,10 +6168,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="36" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5990,120 +6179,120 @@
     </row>
     <row r="3" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="39" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="B3" s="40" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="39"/>
       <c r="B4" s="40" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="39"/>
       <c r="B5" s="25" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="39"/>
       <c r="B6" s="25" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="39"/>
       <c r="B7" s="25" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="39"/>
       <c r="B8" s="41" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="39"/>
       <c r="B9" s="41"/>
       <c r="C9" s="27" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="39"/>
       <c r="B10" s="41"/>
       <c r="C10" s="27" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="39"/>
       <c r="B11" s="41"/>
       <c r="C11" s="25" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="39"/>
       <c r="B12" s="41"/>
       <c r="C12" s="27" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="39"/>
       <c r="B13" s="25" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="216.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="39"/>
       <c r="B14" s="42" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="39"/>
       <c r="B15" s="42"/>
       <c r="C15" s="43" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="39"/>
       <c r="B16" s="42"/>
       <c r="C16" s="43" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="39"/>
       <c r="B17" s="42"/>
       <c r="C17" s="43" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="39"/>
       <c r="B18" s="42"/>
       <c r="C18" s="27" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6112,13 +6301,13 @@
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="39"/>
       <c r="B20" s="44" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="39"/>
       <c r="B21" s="25" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6129,40 +6318,40 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="39" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="B24" s="25" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="39"/>
       <c r="B25" s="25" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="39"/>
       <c r="B26" s="25" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="39"/>
       <c r="B27" s="25" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="39"/>
       <c r="B28" s="27" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="39"/>
       <c r="B29" s="27" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6170,41 +6359,41 @@
     </row>
     <row r="31" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="39" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="B31" s="27" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="F31" s="46"/>
     </row>
     <row r="32" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="39"/>
       <c r="B32" s="27" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="39"/>
       <c r="B33" s="27" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="39"/>
       <c r="B34" s="27" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="39"/>
       <c r="B35" s="27" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="39"/>
       <c r="B36" s="27" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="C36" s="27"/>
     </row>

</xml_diff>

<commit_message>
[feat][OS][OS: Datastructures in OS]
</commit_message>
<xml_diff>
--- a/Operations-System/DevOps-Documents.xlsx
+++ b/Operations-System/DevOps-Documents.xlsx
@@ -1832,14 +1832,82 @@
     <t xml:space="preserve">Kernel Data Structures</t>
   </si>
   <si>
-    <t xml:space="preserve">Lists, Stacks, and Queues:
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">Lists, Stacks, and Queues:
  -  Arrays: Each element can be accessed directly, main memory is constructed as an array.
  - Lists: 
   + Represents a collection of data values as a sequence, the items in a list must be accessed in a particular order.
   + Singly Linked List: Each item points to its successor.
   + Double Linked List: A given item can refer either to its predecessor or to its successor.
   + Circularly Link List: The last element in the list refers to the first element, rather than to null.
-  + Disadvantage of using a list is that performance for retrieving a specified item in a list of size n is linear—O(n), as it requires potentially traversing all n elements in the worst case.</t>
+  + Disadvantage of using a list is that performance for retrieving a specified item in a list of size n is linear—O(n), as it requires potentially traversing all n elements in the worst case.
+ - Stack: Is a sequentially ordered data structure that uses the last in, first out (LIFO) principle for adding and removing items.
+ - Queue: A queue, in contrast, is a sequentially ordered data structure that uses the first in, first out (FIFO) principle.
+ - Trees: 
+  + Is a data structure that can be used to represent </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">data hierarchically</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">(dữ liệu phân cấp). Data values in a tree structure are linked through parent–child relationships.
+  + In a binary tree, a parent may have at most two children, which we term the left child and the right child. 
+  + A binary search tree additionally requires an ordering between the parent’s two children in which left child &lt;= right child
+ - Hash Functions and Map:
+  + Takes data as its input, performs a numeric operation on the data, and returns a numeric value.
+  + Using a hash function for retrieving data from a table can be as good as O(1), depending on implementation details. Because of this performance, hash functions are used extensively in operating systems.
+  + hash collision: 2 unique inputs can result in the same output value
+ - Bitmaps:
+  + Is a string of n binary digits that can be used to represent the status of n items.
+  + A bitmap is a compact data structure that uses individual bits to </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">represent the state of a collection of items</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">. In the context of operating systems and file systems, bitmaps are commonly used to track the allocation status of resources such as disk blocks or memory pages.
+  + Binary Representation: Each bit in a bitmap typically represents a single resource. For example, a bit might be set to 0 to indicate that a disk block is free, or 1 to indicate that it is occupied.
+  + Efficiency: Because each resource is tracked by just one bit, bitmaps are very memory efficient. They allow the OS to quickly determine the availability of resources without needing large data structures.
+  + Common Uses: File Systems, Memory Management, …
+</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Computing Environments</t>
@@ -4585,9 +4653,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>586800</xdr:colOff>
+      <xdr:colOff>586440</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>2119680</xdr:rowOff>
+      <xdr:rowOff>2119320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4601,7 +4669,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10237320" y="8324640"/>
-          <a:ext cx="4799520" cy="2796840"/>
+          <a:ext cx="4799160" cy="2796480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4622,9 +4690,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>663120</xdr:colOff>
+      <xdr:colOff>662760</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>1795680</xdr:rowOff>
+      <xdr:rowOff>1795320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4638,7 +4706,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10323000" y="11420280"/>
-          <a:ext cx="4790160" cy="2491920"/>
+          <a:ext cx="4789800" cy="2491560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4659,9 +4727,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>520200</xdr:colOff>
+      <xdr:colOff>519840</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>694440</xdr:rowOff>
+      <xdr:rowOff>694080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4675,7 +4743,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10170720" y="24355440"/>
-          <a:ext cx="4799520" cy="2901600"/>
+          <a:ext cx="4799160" cy="2901240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4869,8 +4937,8 @@
   </sheetPr>
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D30" colorId="64" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G36" activeCellId="0" sqref="G36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D32" colorId="64" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D34" activeCellId="0" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="36.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5317,16 +5385,18 @@
       <c r="F33" s="10"/>
       <c r="G33" s="10"/>
     </row>
-    <row r="34" customFormat="false" ht="147.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="464.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="6"/>
       <c r="B34" s="7"/>
       <c r="C34" s="8"/>
       <c r="D34" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E34" s="5" t="s">
+      <c r="E34" s="10" t="s">
         <v>69</v>
       </c>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
     </row>
     <row r="35" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="6"/>

</xml_diff>

<commit_message>
[feat][OS][Computing: What is computing]
</commit_message>
<xml_diff>
--- a/Operations-System/DevOps-Documents.xlsx
+++ b/Operations-System/DevOps-Documents.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="235">
   <si>
     <t xml:space="preserve">Operating System Concepts</t>
   </si>
@@ -1911,6 +1911,47 @@
   </si>
   <si>
     <t xml:space="preserve">Computing Environments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Computers and Computing</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> - A computer is just a device that accepts data or input and processes it in some way to automatically produce a result.
+ - Computing means calculating. When computer is doing any kind of work, whether it’s opening an application , editing an image, or playing a song, it is computing.
+ - The process of translating inputs into outputs is known as the </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">computational process</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">, and will likely involve performing a series of calculations in the form of an algorithm.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Traditional computing</t>
   </si>
   <si>
     <t xml:space="preserve">Free and Open-Source Operating Systems</t>
@@ -4653,9 +4694,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>586440</xdr:colOff>
+      <xdr:colOff>586080</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>2119320</xdr:rowOff>
+      <xdr:rowOff>2118960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4669,7 +4710,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10237320" y="8324640"/>
-          <a:ext cx="4799160" cy="2796480"/>
+          <a:ext cx="4798800" cy="2796120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4690,9 +4731,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>662760</xdr:colOff>
+      <xdr:colOff>662400</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>1795320</xdr:rowOff>
+      <xdr:rowOff>1794960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4706,7 +4747,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10323000" y="11420280"/>
-          <a:ext cx="4789800" cy="2491560"/>
+          <a:ext cx="4789440" cy="2491200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4727,9 +4768,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>519840</xdr:colOff>
+      <xdr:colOff>519480</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>694080</xdr:rowOff>
+      <xdr:rowOff>693720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4743,7 +4784,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10170720" y="24355440"/>
-          <a:ext cx="4799160" cy="2901240"/>
+          <a:ext cx="4798800" cy="2900880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4935,10 +4976,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D32" colorId="64" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D34" activeCellId="0" sqref="D34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D35" colorId="64" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F38" activeCellId="0" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="36.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5398,66 +5439,89 @@
       <c r="F34" s="10"/>
       <c r="G34" s="10"/>
     </row>
-    <row r="35" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="56.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="6"/>
       <c r="B35" s="7"/>
       <c r="C35" s="8"/>
       <c r="D35" s="4" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="36" customFormat="false" ht="88.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E35" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="6"/>
       <c r="B36" s="7"/>
       <c r="C36" s="8"/>
-      <c r="D36" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="75.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E36" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="6"/>
       <c r="B37" s="7"/>
-      <c r="C37" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C37" s="8"/>
+      <c r="E37" s="12"/>
+    </row>
+    <row r="38" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="6"/>
-      <c r="B38" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="75.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="7"/>
+      <c r="C38" s="8"/>
+      <c r="E38" s="12"/>
+    </row>
+    <row r="39" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="6"/>
       <c r="B39" s="7"/>
-      <c r="C39" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C39" s="8"/>
+      <c r="E39" s="12"/>
+    </row>
+    <row r="40" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="6"/>
       <c r="B40" s="7"/>
-      <c r="C40" s="3" t="s">
+      <c r="C40" s="8"/>
+      <c r="E40" s="12"/>
+    </row>
+    <row r="41" customFormat="false" ht="88.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="6"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="75.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="6"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="6"/>
-    </row>
-    <row r="42" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="6"/>
-    </row>
-    <row r="43" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="6"/>
-    </row>
-    <row r="44" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="75.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="6"/>
-    </row>
-    <row r="45" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="7"/>
+      <c r="C44" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="6"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="3" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="6"/>
@@ -5465,11 +5529,26 @@
     <row r="47" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="6"/>
     </row>
+    <row r="48" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="6"/>
+    </row>
+    <row r="49" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="6"/>
+    </row>
+    <row r="50" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="6"/>
+    </row>
+    <row r="51" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="6"/>
+    </row>
+    <row r="52" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="38">
-    <mergeCell ref="A1:A47"/>
-    <mergeCell ref="B1:B37"/>
-    <mergeCell ref="C1:C36"/>
+  <mergeCells count="45">
+    <mergeCell ref="A1:A52"/>
+    <mergeCell ref="B1:B42"/>
+    <mergeCell ref="C1:C41"/>
     <mergeCell ref="D1:D4"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="F2:G2"/>
@@ -5504,7 +5583,14 @@
     <mergeCell ref="E32:G32"/>
     <mergeCell ref="E33:G33"/>
     <mergeCell ref="E34:G34"/>
-    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="D35:D40"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="B43:B45"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
@@ -5536,26 +5622,26 @@
   <sheetData>
     <row r="1" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="18" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="21" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="21" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -5620,10 +5706,10 @@
         <v>1</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5631,10 +5717,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5642,10 +5728,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5653,10 +5739,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5664,10 +5750,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5675,10 +5761,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="256.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5686,10 +5772,10 @@
         <v>7</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="245.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5697,10 +5783,10 @@
         <v>8</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="223.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5708,10 +5794,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="243.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5719,86 +5805,86 @@
         <v>10</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="18" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="18" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="18" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="288.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="18" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="E14" s="21" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F14" s="21" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="G14" s="21" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="18" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="240.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B16" s="18" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="18" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="18" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -5835,272 +5921,272 @@
   <sheetData>
     <row r="1" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="26" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B1" s="26"/>
     </row>
     <row r="2" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="24" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="24" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="24" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="24" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="29" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B8" s="29"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="30" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="32" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="32" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B11" s="33" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="31" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="31" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="31" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="31" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B15" s="31" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="31" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B16" s="31" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="31" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B17" s="31" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="31" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B18" s="31" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="31" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B19" s="31" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="31" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B20" s="31" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="31" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B21" s="31" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="26" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B25" s="26"/>
     </row>
     <row r="26" customFormat="false" ht="283.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="24" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B26" s="27" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="24" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B27" s="27" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="34" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="B28" s="27" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="24" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B29" s="27" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="24" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B30" s="27" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="24" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B31" s="27" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="24" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="B32" s="27" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="24" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B33" s="27" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="35" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B34" s="27" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="35"/>
       <c r="B35" s="27" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="35"/>
       <c r="B36" s="27" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="35"/>
       <c r="B37" s="27" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="35"/>
       <c r="B38" s="27" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="35"/>
       <c r="B39" s="28" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="35"/>
       <c r="B40" s="27" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="24" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="B41" s="28" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -6162,18 +6248,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="21" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="18" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -6207,25 +6293,25 @@
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="25" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="25" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="25" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -6259,10 +6345,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="36" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6270,120 +6356,120 @@
     </row>
     <row r="3" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="39" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="B3" s="40" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="39"/>
       <c r="B4" s="40" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="39"/>
       <c r="B5" s="25" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="39"/>
       <c r="B6" s="25" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="39"/>
       <c r="B7" s="25" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="39"/>
       <c r="B8" s="41" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="39"/>
       <c r="B9" s="41"/>
       <c r="C9" s="27" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="39"/>
       <c r="B10" s="41"/>
       <c r="C10" s="27" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="39"/>
       <c r="B11" s="41"/>
       <c r="C11" s="25" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="39"/>
       <c r="B12" s="41"/>
       <c r="C12" s="27" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="39"/>
       <c r="B13" s="25" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="216.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="39"/>
       <c r="B14" s="42" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="39"/>
       <c r="B15" s="42"/>
       <c r="C15" s="43" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="39"/>
       <c r="B16" s="42"/>
       <c r="C16" s="43" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="39"/>
       <c r="B17" s="42"/>
       <c r="C17" s="43" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="39"/>
       <c r="B18" s="42"/>
       <c r="C18" s="27" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6392,13 +6478,13 @@
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="39"/>
       <c r="B20" s="44" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="39"/>
       <c r="B21" s="25" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6409,40 +6495,40 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="39" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="B24" s="25" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="39"/>
       <c r="B25" s="25" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="39"/>
       <c r="B26" s="25" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="39"/>
       <c r="B27" s="25" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="39"/>
       <c r="B28" s="27" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="39"/>
       <c r="B29" s="27" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6450,41 +6536,41 @@
     </row>
     <row r="31" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="39" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="B31" s="27" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="F31" s="46"/>
     </row>
     <row r="32" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="39"/>
       <c r="B32" s="27" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="39"/>
       <c r="B33" s="27" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="39"/>
       <c r="B34" s="27" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="39"/>
       <c r="B35" s="27" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="39"/>
       <c r="B36" s="27" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="C36" s="27"/>
     </row>

</xml_diff>

<commit_message>
[feat][OS][OS: Environment Computing + OS Services + OS Interfaces]
</commit_message>
<xml_diff>
--- a/Operations-System/DevOps-Documents.xlsx
+++ b/Operations-System/DevOps-Documents.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="256">
   <si>
     <t xml:space="preserve">Operating System Concepts</t>
   </si>
@@ -1954,10 +1954,600 @@
     <t xml:space="preserve">Traditional computing</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> - Before “typical office environment” consisted of PCs connected to a network, with server providing file and print services.
+ - Today, Web techs increasing WAN bandwidth are stretching(mở rộng) the boundaries of traditional computing:
+  + Companies establish </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">portals</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">: providing web accessibility to their internal servers.
+  + Network computers
+ - In the latter half of the 20th century, computing resources were relatively scarce. For a period of time, systems were either </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">batch</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> or </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">interactive</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">.
+ - To optimize the use of the computing resources, </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">multiple users shared time</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> on these systems.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Mobile computing</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Mobile computing refers to computing on handheld smartphones and tablet computers.
+ - Features of a contemporary mobile device allow it to provide functionality that is either unavailable or impractical on a desktop or laptop computer.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Client – Server Computing</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> - Client-server system: Is specialized distributed system,  contemporary network architecture(kiến trúc mạng hiện đại) features arrangements in which </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">server systems</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> satisfy requests generated by </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">client systems</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">.
+ - Server systems can be broadly categorized as compute servers and file servers:
+  + The compute-server system provides an interface to which a client can send a request to perform an action. In response the server executes the action and sends the results to client.
+  + The file-serve system provides a file-system interface where clients can create, update, read, and delete files.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Peer-to-Peer Computing
+(P2P)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> - P2P: Another structure for a distributed system, </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">clients and server are not distinguished(phân biệt) from one another</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">.
+ - In a client–server system, the server is a bottleneck; but in a peer-to-peer system, s</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">ervices can be provided by several nodes distributed throughout the network</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">.
+ - Once a node has joined the network, it can begin providing services to—and requesting services from—other nodes in the network. 
+ - Determining what services are available is accomplished in one of two general ways:
+  + When a node joins a network, it registers its service with a </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">centralized lookup service</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> on the network. Any node desiring(want) a specific service first contacts(liên hệ) this centralized lookup service to determine which node provides the service. The remainder(phần còn lại) of the communication takes place between the client and the service provider.
+  + Instead, a peer acting as a client must discover what node provides a desired service by broadcasting a request for the service to all other nodes in the network. The node (or nodes) providing that service responds to the peer making the request. To support this approach, a discovery protocol must be provided that allows peers to discover services provided by other peers in the network.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Cloud Computing</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> - Cloud computing </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">is a type of computing that delivers computing, storage, and even applications as a service across a network</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">. In some ways, </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">it’s a logical extension of virtualization</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">, because it uses virtualization as a base for its functionality.
+ - Many types of cloud computing: 
+  + Public cloud: A cloud available via the Internet to anyone willing to pay.
+  + Private cloud: A cloud run by a company for that company’s own use.
+  + Hybrid cloud: A cloud that includes both public and private cloud components.
+  + SaaS: One or more applications available via the Internet. Ex: Google Sheet, GG Docs,...
+  + PaaS: A software stack ready for application use via the Internet (Database server).
+  + IaaS: Servers or storage available over the Internet.</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">Free and Open-Source Operating Systems</t>
   </si>
   <si>
     <t xml:space="preserve">Operating-System Structure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operating-System Services</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> - An operating system provides an environment for the execution of programs. One set of operating system services provides functions that are helpful to the user.
+ - User interface (UI):
+  + Most commonly, a graphical user interface (GUI) is used. 
+  + The interface is a window system with a mouse that serves as a pointing device to direct I/O, choose from menus, and make selections and a keyboard to enter text. 
+  + Mobile systems such as phones and tablets provide a touch-screen interface, enabling users to slide their fingers across the screen or press buttons on the screen to select choices. 
+  + Another option is a command-line interface (CLI), which uses text commands and a method for entering them (say, a keyboard for typing in commands in a specific format with specific options). 
+  + Some systems provide two or all three of these variations.
+ - Program execution: The system must be able to load a program into memory and to run that program. The program must be able to end its execution, either normally or abnormally (indicating error).
+ - I/O operations. For efficiency and protection, users usually cannot control I/O devices directly. Therefore, the operating system must provide a means to do I/O.
+ - File-system manipulation.
+ - Communications: One process needs to exchange information with another process or between processes that are executing on different computer systems tied together by a network. Communications may be implemented via shared memory, or message passing.
+ - Error detection: The operating system needs to be detecting and correcting errors constantly. For each type of error, the operating system should take the appropriate action to ensure correct and consistent
+Computing. Sometimes, it has no choice but to halt the system(dừng hệ thống). At other times, it might terminate an error-causing process or return an error code to a process for the process to detect and possibly correct.
+ - Resource allocation: When there are multiple processes running at the same time, resources must be allocated to each of them. The operating system manages many different types of resources. Some (such as CPU cycles, main memory, and file storage) may have special allocation code, whereas others (such as I/O devices) may have much more general request and release code. For instance, in determining how best to use the CPU, operating systems have CPU-scheduling routines that take into account the speed of the CPU, the process that must be executed, the number of processing cores on the CPU, and other factors. There may also be routines to allocate printers, USB storage drives, and other peripheral devices.
+ - Logging.
+ - Protection and security:
+  + Protection involves ensuring that all access to system resources is </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">controlled</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">. 
+  + Security of the system from outsiders is also important. Such security starts with requiring each user to authenticate himself or herself to the system, usually by means of a password, to gain access to system resources.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">User and Operating-System Interface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Command Interpreters</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> - The main function of the command interpreter is to get and execute the next user-specified command.
+ - An approach—used by UNIX, among other operating systems —implements most commands through system programs. In this case, the command interpreter does not understand the command in any way; i</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">t merely uses the command to identify a file to be loaded into memory and executed</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">.
+  rm file.txt  → Search for a file called rm, load the file into memory, and execute it with the parameter file.txt.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Graphical User Interface</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> - Users employ a mouse-based window and-menu system characterized by a </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">desktop</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> metaphor. 
+ - The user moves the mouse to position its pointer on images, or icons, on the screen (the desktop) that represent programs, files, directories, and system functions. 
+ - Depending on the mouse pointer’s location, clicking a button on the mouse can invoke a program, select a file or directory—known as a folder—or pull down a menu
+that </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">contains commands</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Touch-Screen Interface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Users interact by making gestures(cử chỉ) on the touch screen—for example, pressing and swiping fingers across the screen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choice of Interface</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">System administrators</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> who manage computers and </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">power users</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> who have </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">deep knowledge of a system frequently</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> use the command-line interface.  For them, it is </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">more efficient</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">, giving them </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">faster access</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> to the activities they need to perform. Indeed, on some systems, only a subset of system functions is available via the GUI, leaving the less common tasks to those who are command-line knowledgeable. 
+Further, command-line interfaces usually make repetitive tasks easier, in part because they have their own programmability. For example, if a frequent task requires a set of command line steps, those steps can be recorded into a file, and that file can be run just like a program. The program is not compiled into executable code but rather is interpreted by the command-line interface. These shell scripts are very common on systems that are command-line oriented, such as UNIX and Linux.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">System Calls</t>
   </si>
   <si>
     <t xml:space="preserve">Processes</t>
@@ -4419,7 +5009,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4489,6 +5079,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4694,9 +5292,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>586080</xdr:colOff>
+      <xdr:colOff>585720</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>2118960</xdr:rowOff>
+      <xdr:rowOff>2118600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4710,7 +5308,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10237320" y="8324640"/>
-          <a:ext cx="4798800" cy="2796120"/>
+          <a:ext cx="4798440" cy="2795760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4731,9 +5329,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>662400</xdr:colOff>
+      <xdr:colOff>662040</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>1794960</xdr:rowOff>
+      <xdr:rowOff>1794600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4747,7 +5345,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10323000" y="11420280"/>
-          <a:ext cx="4789440" cy="2491200"/>
+          <a:ext cx="4789080" cy="2490840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4768,9 +5366,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>519480</xdr:colOff>
+      <xdr:colOff>519120</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>693720</xdr:rowOff>
+      <xdr:rowOff>693360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4784,7 +5382,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10170720" y="24355440"/>
-          <a:ext cx="4798800" cy="2900880"/>
+          <a:ext cx="4798440" cy="2900520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4976,10 +5574,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D35" colorId="64" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F38" activeCellId="0" sqref="F38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D47" colorId="64" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G54" activeCellId="0" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="36.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5443,111 +6041,235 @@
       <c r="A35" s="6"/>
       <c r="B35" s="7"/>
       <c r="C35" s="8"/>
-      <c r="D35" s="4" t="s">
+      <c r="D35" s="9" t="s">
         <v>70</v>
       </c>
       <c r="E35" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="F35" s="5" t="s">
+      <c r="F35" s="10" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="36" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G35" s="10"/>
+    </row>
+    <row r="36" customFormat="false" ht="108.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="6"/>
       <c r="B36" s="7"/>
       <c r="C36" s="8"/>
+      <c r="D36" s="9"/>
       <c r="E36" s="12" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="37" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F36" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="G36" s="10"/>
+    </row>
+    <row r="37" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="6"/>
       <c r="B37" s="7"/>
       <c r="C37" s="8"/>
-      <c r="E37" s="12"/>
-    </row>
-    <row r="38" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D37" s="9"/>
+      <c r="E37" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="F37" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="G37" s="10"/>
+    </row>
+    <row r="38" customFormat="false" ht="91" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="6"/>
       <c r="B38" s="7"/>
       <c r="C38" s="8"/>
-      <c r="E38" s="12"/>
-    </row>
-    <row r="39" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D38" s="9"/>
+      <c r="E38" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F38" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="G38" s="10"/>
+    </row>
+    <row r="39" customFormat="false" ht="144.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="6"/>
       <c r="B39" s="7"/>
       <c r="C39" s="8"/>
-      <c r="E39" s="12"/>
-    </row>
-    <row r="40" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D39" s="9"/>
+      <c r="E39" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="F39" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="G39" s="10"/>
+    </row>
+    <row r="40" customFormat="false" ht="162.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="6"/>
       <c r="B40" s="7"/>
       <c r="C40" s="8"/>
-      <c r="E40" s="12"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="F40" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="G40" s="18"/>
     </row>
     <row r="41" customFormat="false" ht="88.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="6"/>
       <c r="B41" s="7"/>
       <c r="C41" s="8"/>
       <c r="D41" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="75.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="574.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="6"/>
       <c r="B42" s="7"/>
       <c r="C42" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>84</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="73.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="6"/>
-      <c r="B43" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="75.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="7"/>
+      <c r="D43" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="73.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="6"/>
       <c r="B44" s="7"/>
-      <c r="C44" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E44" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="6"/>
       <c r="B45" s="7"/>
-      <c r="C45" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E45" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="108.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="6"/>
-    </row>
-    <row r="47" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="7"/>
+      <c r="E46" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="F46" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="G46" s="19"/>
+    </row>
+    <row r="47" customFormat="false" ht="36.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="6"/>
+      <c r="B47" s="7"/>
+      <c r="D47" s="4" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="6"/>
+      <c r="B48" s="7"/>
     </row>
     <row r="49" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="6"/>
+      <c r="B49" s="7"/>
     </row>
     <row r="50" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="6"/>
+      <c r="B50" s="7"/>
     </row>
     <row r="51" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="6"/>
+      <c r="B51" s="7"/>
     </row>
     <row r="52" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="6"/>
-    </row>
+      <c r="B52" s="7"/>
+    </row>
+    <row r="53" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="6"/>
+      <c r="B53" s="7"/>
+    </row>
+    <row r="54" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="6"/>
+      <c r="B54" s="7"/>
+    </row>
+    <row r="55" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="6"/>
+      <c r="B55" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="75.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="6"/>
+      <c r="B56" s="7"/>
+      <c r="C56" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="6"/>
+      <c r="B57" s="7"/>
+      <c r="C57" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="6"/>
+    </row>
+    <row r="59" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="6"/>
+    </row>
+    <row r="60" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="6"/>
+    </row>
+    <row r="61" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="6"/>
+    </row>
+    <row r="62" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="6"/>
+    </row>
+    <row r="63" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="6"/>
+    </row>
+    <row r="64" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="6"/>
+    </row>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="45">
-    <mergeCell ref="A1:A52"/>
-    <mergeCell ref="B1:B42"/>
+  <mergeCells count="53">
+    <mergeCell ref="A1:A64"/>
+    <mergeCell ref="B1:B54"/>
     <mergeCell ref="C1:C41"/>
     <mergeCell ref="D1:D4"/>
     <mergeCell ref="E1:G1"/>
@@ -5590,7 +6312,15 @@
     <mergeCell ref="F38:G38"/>
     <mergeCell ref="F39:G39"/>
     <mergeCell ref="F40:G40"/>
-    <mergeCell ref="B43:B45"/>
+    <mergeCell ref="C42:C52"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="D43:D46"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="D47:D50"/>
+    <mergeCell ref="B55:B57"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
@@ -5615,33 +6345,33 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="18" width="23.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="18" width="57.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="3" style="18" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="20" width="23.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="20" width="57.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="3" style="20" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="18" t="s">
-        <v>229</v>
-      </c>
-      <c r="B1" s="21" t="s">
-        <v>230</v>
+      <c r="A1" s="20" t="s">
+        <v>250</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="21" t="s">
-        <v>231</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>232</v>
+      <c r="A2" s="23" t="s">
+        <v>252</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="21" t="s">
-        <v>233</v>
-      </c>
-      <c r="B3" s="21" t="s">
-        <v>234</v>
+      <c r="A3" s="23" t="s">
+        <v>254</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -5691,200 +6421,200 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="18" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="18" width="39.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="18" width="95.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="18" width="60.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="18" width="58.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="18" width="50"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="18" width="49.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="8" style="18" width="9.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="20" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="20" width="39.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="20" width="95.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="20" width="60.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="20" width="58.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="20" width="50"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="20" width="49.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="8" style="20" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="18" t="n">
+      <c r="A1" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="B1" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>80</v>
+      <c r="B1" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="18" t="n">
+      <c r="A2" s="20" t="n">
         <v>2</v>
       </c>
-      <c r="B2" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>82</v>
+      <c r="B2" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="18" t="n">
+      <c r="A3" s="20" t="n">
         <v>3</v>
       </c>
-      <c r="B3" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>84</v>
+      <c r="B3" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="18" t="n">
+      <c r="A4" s="20" t="n">
         <v>4</v>
       </c>
-      <c r="B4" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>86</v>
+      <c r="B4" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="18" t="n">
+      <c r="A5" s="20" t="n">
         <v>5</v>
       </c>
-      <c r="B5" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>88</v>
+      <c r="B5" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="18" t="n">
+      <c r="A6" s="20" t="n">
         <v>6</v>
       </c>
-      <c r="B6" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>90</v>
+      <c r="B6" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="256.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="18" t="n">
+      <c r="A7" s="20" t="n">
         <v>7</v>
       </c>
-      <c r="B7" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="C7" s="22" t="s">
-        <v>92</v>
+      <c r="B7" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="245.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="18" t="n">
+      <c r="A8" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="B8" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="C8" s="19" t="s">
-        <v>94</v>
+      <c r="B8" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="223.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="18" t="n">
+      <c r="A9" s="20" t="n">
         <v>9</v>
       </c>
-      <c r="B9" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>96</v>
+      <c r="B9" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="243.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="18" t="n">
+      <c r="A10" s="20" t="n">
         <v>10</v>
       </c>
-      <c r="B10" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="D10" s="23" t="s">
-        <v>99</v>
+      <c r="B10" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="C11" s="21" t="s">
-        <v>101</v>
+      <c r="B11" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>103</v>
+      <c r="B12" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="C13" s="21" t="s">
-        <v>105</v>
+      <c r="B13" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="288.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="E14" s="21" t="s">
-        <v>109</v>
-      </c>
-      <c r="F14" s="21" t="s">
-        <v>110</v>
-      </c>
-      <c r="G14" s="21" t="s">
-        <v>111</v>
+      <c r="B14" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="G14" s="23" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>113</v>
+      <c r="B15" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="240.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="18" t="s">
-        <v>114</v>
+      <c r="B16" s="20" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="C17" s="19" t="s">
-        <v>116</v>
+      <c r="B17" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="C18" s="19" t="s">
-        <v>118</v>
+      <c r="B18" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -5915,278 +6645,278 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="24" width="72.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="139.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="26" width="72.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="27" width="139.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="26" t="s">
-        <v>119</v>
-      </c>
-      <c r="B1" s="26"/>
+      <c r="A1" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1" s="28"/>
     </row>
     <row r="2" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="24" t="s">
-        <v>120</v>
-      </c>
-      <c r="B2" s="27" t="s">
-        <v>121</v>
+      <c r="A2" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="24" t="s">
-        <v>122</v>
-      </c>
-      <c r="B3" s="28" t="s">
-        <v>123</v>
+      <c r="A3" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="24" t="s">
-        <v>124</v>
-      </c>
-      <c r="B4" s="28" t="s">
-        <v>125</v>
+      <c r="A4" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="24" t="s">
-        <v>126</v>
-      </c>
-      <c r="B5" s="28" t="s">
-        <v>127</v>
+      <c r="A5" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="29" t="s">
-        <v>128</v>
-      </c>
-      <c r="B8" s="29"/>
+      <c r="A8" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="B8" s="31"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="30" t="s">
-        <v>129</v>
-      </c>
-      <c r="B9" s="31" t="s">
-        <v>130</v>
+      <c r="A9" s="32" t="s">
+        <v>150</v>
+      </c>
+      <c r="B9" s="33" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="32" t="s">
-        <v>131</v>
-      </c>
-      <c r="B10" s="31" t="s">
-        <v>132</v>
+      <c r="A10" s="34" t="s">
+        <v>152</v>
+      </c>
+      <c r="B10" s="33" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="32" t="s">
-        <v>133</v>
-      </c>
-      <c r="B11" s="33" t="s">
-        <v>134</v>
+      <c r="A11" s="34" t="s">
+        <v>154</v>
+      </c>
+      <c r="B11" s="35" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="31" t="s">
-        <v>135</v>
-      </c>
-      <c r="B12" s="31" t="s">
-        <v>136</v>
+      <c r="A12" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="B12" s="33" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="31" t="s">
-        <v>137</v>
-      </c>
-      <c r="B13" s="31" t="s">
-        <v>138</v>
+      <c r="A13" s="33" t="s">
+        <v>158</v>
+      </c>
+      <c r="B13" s="33" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="31" t="s">
-        <v>139</v>
-      </c>
-      <c r="B14" s="31" t="s">
-        <v>140</v>
+      <c r="A14" s="33" t="s">
+        <v>160</v>
+      </c>
+      <c r="B14" s="33" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="31" t="s">
-        <v>141</v>
-      </c>
-      <c r="B15" s="31" t="s">
-        <v>142</v>
+      <c r="A15" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="B15" s="33" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="31" t="s">
-        <v>143</v>
-      </c>
-      <c r="B16" s="31" t="s">
-        <v>144</v>
+      <c r="A16" s="33" t="s">
+        <v>164</v>
+      </c>
+      <c r="B16" s="33" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="31" t="s">
-        <v>145</v>
-      </c>
-      <c r="B17" s="31" t="s">
-        <v>146</v>
+      <c r="A17" s="33" t="s">
+        <v>166</v>
+      </c>
+      <c r="B17" s="33" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="31" t="s">
-        <v>147</v>
-      </c>
-      <c r="B18" s="31" t="s">
-        <v>148</v>
+      <c r="A18" s="33" t="s">
+        <v>168</v>
+      </c>
+      <c r="B18" s="33" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="31" t="s">
-        <v>149</v>
-      </c>
-      <c r="B19" s="31" t="s">
-        <v>150</v>
+      <c r="A19" s="33" t="s">
+        <v>170</v>
+      </c>
+      <c r="B19" s="33" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="31" t="s">
-        <v>151</v>
-      </c>
-      <c r="B20" s="31" t="s">
-        <v>152</v>
+      <c r="A20" s="33" t="s">
+        <v>172</v>
+      </c>
+      <c r="B20" s="33" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="31" t="s">
-        <v>153</v>
-      </c>
-      <c r="B21" s="31" t="s">
-        <v>154</v>
+      <c r="A21" s="33" t="s">
+        <v>174</v>
+      </c>
+      <c r="B21" s="33" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="26" t="s">
-        <v>155</v>
-      </c>
-      <c r="B25" s="26"/>
+      <c r="A25" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="B25" s="28"/>
     </row>
     <row r="26" customFormat="false" ht="283.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="24" t="s">
-        <v>156</v>
-      </c>
-      <c r="B26" s="27" t="s">
-        <v>157</v>
+      <c r="A26" s="26" t="s">
+        <v>177</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="24" t="s">
-        <v>158</v>
-      </c>
-      <c r="B27" s="27" t="s">
-        <v>159</v>
+      <c r="A27" s="26" t="s">
+        <v>179</v>
+      </c>
+      <c r="B27" s="29" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="34" t="s">
-        <v>160</v>
-      </c>
-      <c r="B28" s="27" t="s">
-        <v>161</v>
+      <c r="A28" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="B28" s="29" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="24" t="s">
-        <v>162</v>
-      </c>
-      <c r="B29" s="27" t="s">
-        <v>163</v>
+      <c r="A29" s="26" t="s">
+        <v>183</v>
+      </c>
+      <c r="B29" s="29" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="24" t="s">
-        <v>164</v>
-      </c>
-      <c r="B30" s="27" t="s">
-        <v>165</v>
+      <c r="A30" s="26" t="s">
+        <v>185</v>
+      </c>
+      <c r="B30" s="29" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="24" t="s">
-        <v>166</v>
-      </c>
-      <c r="B31" s="27" t="s">
-        <v>167</v>
+      <c r="A31" s="26" t="s">
+        <v>187</v>
+      </c>
+      <c r="B31" s="29" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="24" t="s">
-        <v>168</v>
-      </c>
-      <c r="B32" s="27" t="s">
-        <v>169</v>
+      <c r="A32" s="26" t="s">
+        <v>189</v>
+      </c>
+      <c r="B32" s="29" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="24" t="s">
-        <v>170</v>
-      </c>
-      <c r="B33" s="27" t="s">
-        <v>171</v>
+      <c r="A33" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="B33" s="29" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="35" t="s">
-        <v>172</v>
-      </c>
-      <c r="B34" s="27" t="s">
-        <v>173</v>
+      <c r="A34" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="B34" s="29" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="35"/>
-      <c r="B35" s="27" t="s">
-        <v>174</v>
+      <c r="A35" s="37"/>
+      <c r="B35" s="29" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="35"/>
-      <c r="B36" s="27" t="s">
-        <v>175</v>
+      <c r="A36" s="37"/>
+      <c r="B36" s="29" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="35"/>
-      <c r="B37" s="27" t="s">
-        <v>176</v>
+      <c r="A37" s="37"/>
+      <c r="B37" s="29" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="35"/>
-      <c r="B38" s="27" t="s">
-        <v>177</v>
+      <c r="A38" s="37"/>
+      <c r="B38" s="29" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="35"/>
-      <c r="B39" s="28" t="s">
-        <v>178</v>
+      <c r="A39" s="37"/>
+      <c r="B39" s="30" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="35"/>
-      <c r="B40" s="27" t="s">
-        <v>179</v>
+      <c r="A40" s="37"/>
+      <c r="B40" s="29" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="24" t="s">
-        <v>180</v>
-      </c>
-      <c r="B41" s="28" t="s">
-        <v>181</v>
+      <c r="A41" s="26" t="s">
+        <v>201</v>
+      </c>
+      <c r="B41" s="30" t="s">
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -6242,24 +6972,24 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="18" width="37.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="18" width="77.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="20" width="37.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="20" width="77.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="21" t="s">
-        <v>182</v>
-      </c>
-      <c r="B1" s="21" t="s">
-        <v>183</v>
+      <c r="A1" s="23" t="s">
+        <v>203</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="18" t="s">
-        <v>184</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>185</v>
+      <c r="A2" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -6286,32 +7016,32 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="25" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="60.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="27" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="27" width="60.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="25" t="s">
-        <v>186</v>
+      <c r="A2" s="27" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="25" t="s">
-        <v>187</v>
+      <c r="A4" s="27" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="25" t="s">
-        <v>188</v>
+      <c r="A6" s="27" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="25" t="s">
-        <v>189</v>
+      <c r="A8" s="27" t="s">
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -6338,241 +7068,241 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="25" width="28.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="49.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="25" width="69.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="27" width="28.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="27" width="49.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="27" width="69.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="36" t="s">
-        <v>190</v>
-      </c>
-      <c r="B1" s="37" t="s">
-        <v>191</v>
+      <c r="A1" s="38" t="s">
+        <v>211</v>
+      </c>
+      <c r="B1" s="39" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="38"/>
+      <c r="A2" s="40"/>
     </row>
     <row r="3" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="39" t="s">
-        <v>192</v>
-      </c>
-      <c r="B3" s="40" t="s">
-        <v>193</v>
-      </c>
-      <c r="C3" s="27" t="s">
-        <v>194</v>
+      <c r="A3" s="41" t="s">
+        <v>213</v>
+      </c>
+      <c r="B3" s="42" t="s">
+        <v>214</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="39"/>
-      <c r="B4" s="40" t="s">
-        <v>195</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>196</v>
+      <c r="A4" s="41"/>
+      <c r="B4" s="42" t="s">
+        <v>216</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="39"/>
-      <c r="B5" s="25" t="s">
-        <v>197</v>
+      <c r="A5" s="41"/>
+      <c r="B5" s="27" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="39"/>
-      <c r="B6" s="25" t="s">
-        <v>198</v>
+      <c r="A6" s="41"/>
+      <c r="B6" s="27" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="39"/>
-      <c r="B7" s="25" t="s">
-        <v>199</v>
+      <c r="A7" s="41"/>
+      <c r="B7" s="27" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="39"/>
-      <c r="B8" s="41" t="s">
-        <v>200</v>
-      </c>
-      <c r="C8" s="27" t="s">
-        <v>201</v>
+      <c r="A8" s="41"/>
+      <c r="B8" s="43" t="s">
+        <v>221</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="39"/>
-      <c r="B9" s="41"/>
-      <c r="C9" s="27" t="s">
-        <v>202</v>
+      <c r="A9" s="41"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="29" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="39"/>
-      <c r="B10" s="41"/>
-      <c r="C10" s="27" t="s">
-        <v>203</v>
+      <c r="A10" s="41"/>
+      <c r="B10" s="43"/>
+      <c r="C10" s="29" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="39"/>
-      <c r="B11" s="41"/>
-      <c r="C11" s="25" t="s">
-        <v>204</v>
+      <c r="A11" s="41"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="27" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="39"/>
-      <c r="B12" s="41"/>
-      <c r="C12" s="27" t="s">
-        <v>205</v>
+      <c r="A12" s="41"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="29" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="39"/>
-      <c r="B13" s="25" t="s">
-        <v>206</v>
+      <c r="A13" s="41"/>
+      <c r="B13" s="27" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="216.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="39"/>
-      <c r="B14" s="42" t="s">
-        <v>207</v>
-      </c>
-      <c r="C14" s="27" t="s">
-        <v>208</v>
+      <c r="A14" s="41"/>
+      <c r="B14" s="44" t="s">
+        <v>228</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="39"/>
-      <c r="B15" s="42"/>
-      <c r="C15" s="43" t="s">
-        <v>209</v>
+      <c r="A15" s="41"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="45" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="39"/>
-      <c r="B16" s="42"/>
-      <c r="C16" s="43" t="s">
-        <v>210</v>
+      <c r="A16" s="41"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="45" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="39"/>
-      <c r="B17" s="42"/>
-      <c r="C17" s="43" t="s">
-        <v>211</v>
+      <c r="A17" s="41"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="45" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="39"/>
-      <c r="B18" s="42"/>
-      <c r="C18" s="27" t="s">
-        <v>212</v>
+      <c r="A18" s="41"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="29" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="39"/>
+      <c r="A19" s="41"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="39"/>
-      <c r="B20" s="44" t="s">
-        <v>213</v>
+      <c r="A20" s="41"/>
+      <c r="B20" s="46" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="39"/>
-      <c r="B21" s="25" t="s">
-        <v>214</v>
+      <c r="A21" s="41"/>
+      <c r="B21" s="27" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="38"/>
+      <c r="A22" s="40"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="38"/>
+      <c r="A23" s="40"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="39" t="s">
-        <v>215</v>
-      </c>
-      <c r="B24" s="25" t="s">
-        <v>216</v>
+      <c r="A24" s="41" t="s">
+        <v>236</v>
+      </c>
+      <c r="B24" s="27" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="39"/>
-      <c r="B25" s="25" t="s">
-        <v>217</v>
+      <c r="A25" s="41"/>
+      <c r="B25" s="27" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="39"/>
-      <c r="B26" s="25" t="s">
-        <v>218</v>
+      <c r="A26" s="41"/>
+      <c r="B26" s="27" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="39"/>
-      <c r="B27" s="25" t="s">
-        <v>219</v>
+      <c r="A27" s="41"/>
+      <c r="B27" s="27" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="39"/>
-      <c r="B28" s="27" t="s">
-        <v>220</v>
+      <c r="A28" s="41"/>
+      <c r="B28" s="29" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="39"/>
-      <c r="B29" s="27" t="s">
-        <v>221</v>
+      <c r="A29" s="41"/>
+      <c r="B29" s="29" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="45"/>
+      <c r="A30" s="47"/>
     </row>
     <row r="31" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="39" t="s">
-        <v>222</v>
-      </c>
-      <c r="B31" s="27" t="s">
-        <v>223</v>
-      </c>
-      <c r="F31" s="46"/>
+      <c r="A31" s="41" t="s">
+        <v>243</v>
+      </c>
+      <c r="B31" s="29" t="s">
+        <v>244</v>
+      </c>
+      <c r="F31" s="48"/>
     </row>
     <row r="32" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="39"/>
-      <c r="B32" s="27" t="s">
-        <v>224</v>
+      <c r="A32" s="41"/>
+      <c r="B32" s="29" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="39"/>
-      <c r="B33" s="27" t="s">
-        <v>225</v>
+      <c r="A33" s="41"/>
+      <c r="B33" s="29" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="39"/>
-      <c r="B34" s="27" t="s">
-        <v>226</v>
+      <c r="A34" s="41"/>
+      <c r="B34" s="29" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="39"/>
-      <c r="B35" s="27" t="s">
-        <v>227</v>
+      <c r="A35" s="41"/>
+      <c r="B35" s="29" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="39"/>
-      <c r="B36" s="27" t="s">
-        <v>228</v>
-      </c>
-      <c r="C36" s="27"/>
+      <c r="A36" s="41"/>
+      <c r="B36" s="29" t="s">
+        <v>249</v>
+      </c>
+      <c r="C36" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
[feat][OS][OS: System calls + API + System-call types]
</commit_message>
<xml_diff>
--- a/Operations-System/DevOps-Documents.xlsx
+++ b/Operations-System/DevOps-Documents.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="263">
   <si>
     <t xml:space="preserve">Operating System Concepts</t>
   </si>
@@ -2550,6 +2550,321 @@
     <t xml:space="preserve">System Calls</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> - A system call is the </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">primary interface</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> through which </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">a user-level process requests a service from the OS’s kernel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">. In essence, it’s a controlled gateway that enables applications running in </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">user mode (which have limited privileges) to perform operations that require higher privileges</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">—such as accessing hardware devices, managing files, or creating processes.
+ - System calls provide an interface to the services </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">made available</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">(được cung cấp) by an OS
+ - How:
+  + Invocation: A user program triggers a system call by executing a special instruction (often called a trap or syscall instruction). This instruction notifies the processor that it should transfer control to the kernel.
+  + Mode Switch: When the system call is invoked, the CPU switches from user mode to kernel mode. This change grants the operating system full access to all hardware and memory, ensuring that sensitive operations are executed securely.
+  + Parameter Passing and Handling:
+  + Execution
+  + Return to User Mode</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Application Programming Interface</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> - The API specifies a set of functions that are available to an application programmer, including the parameters that are passed to each function and the return values the programmer can expect.
+ - API is benefit concerns program portability(tính linh động), program to compile and run on any system that supports API,…
+ - A programmer accesses an API via a library of code provided by the OS. Ex: UNIX and LINUX for programs written in the C language, the lib called </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">libc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">.
+ - Behind the scenes, the f</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">unctions that make up an API </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">typically invoke the </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">actual system calls</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> on behalf of the application programmer.
+ → System-call Interface: that serves as the link to system calls made available by the operating system.
+ =&gt; 1. User Program Calls an API Function: An application calls a high-level function provided by a standard library (e.g read(), write() or open())
+  2. API Wrapper Logic: The library function performs necessary error checking, sets up parameters, and invokes the corresponding system call through a special instruction or trap (like syscall or INT 0x80).
+  3. System-Call Interface Action: The system call transfers control to the kernel. The kernel uses the system-call number to index its system call table and execute the corresponding service routine with the provided parameters.
+  4. Kernel Execution and Return: After executing the service (e.g., reading from a file), the kernel returns a status or result to the API wrapper, which then passes it back to the application.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Types of System Calls</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> - System calls can be grouped roughly into </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">six major categories</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">: process control, fil management, device management, information maintenance, communications, and protection.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Process Control</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> - Process control system calls are a </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">set of kernel-level interfaces</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> that allow user-space programs to create, manage, and terminate processes. They form a core component of </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">process management</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> in an operating system and </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">enable multitasking</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, allowing the OS to execute multiple programs </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">concurrently</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">.</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">Processes</t>
   </si>
   <si>
@@ -4733,7 +5048,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="31">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4844,6 +5159,19 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -4999,13 +5327,13 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="27" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
@@ -5082,11 +5410,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5094,11 +5422,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5106,15 +5434,15 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5122,7 +5450,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5134,11 +5462,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5146,7 +5474,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5154,19 +5482,19 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5174,7 +5502,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5182,7 +5510,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5190,19 +5518,19 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5292,9 +5620,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>585720</xdr:colOff>
+      <xdr:colOff>585360</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>2118600</xdr:rowOff>
+      <xdr:rowOff>2118240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5308,7 +5636,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10237320" y="8324640"/>
-          <a:ext cx="4798440" cy="2795760"/>
+          <a:ext cx="4798080" cy="2795400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5329,9 +5657,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>662040</xdr:colOff>
+      <xdr:colOff>661680</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>1794600</xdr:rowOff>
+      <xdr:rowOff>1794240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5345,7 +5673,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10323000" y="11420280"/>
-          <a:ext cx="4789080" cy="2490840"/>
+          <a:ext cx="4788720" cy="2490480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5366,9 +5694,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>519120</xdr:colOff>
+      <xdr:colOff>518760</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>693360</xdr:rowOff>
+      <xdr:rowOff>693000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5382,7 +5710,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10170720" y="24355440"/>
-          <a:ext cx="4798440" cy="2900520"/>
+          <a:ext cx="4798080" cy="2900160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5574,10 +5902,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G1048576"/>
+  <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D47" colorId="64" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G54" activeCellId="0" sqref="G54"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D49" colorId="64" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F48" activeCellId="0" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="36.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6112,10 +6440,10 @@
       <c r="E40" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="F40" s="18" t="s">
+      <c r="F40" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="G40" s="18"/>
+      <c r="G40" s="10"/>
     </row>
     <row r="41" customFormat="false" ht="88.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="6"/>
@@ -6128,132 +6456,200 @@
     <row r="42" customFormat="false" ht="574.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="6"/>
       <c r="B42" s="7"/>
-      <c r="C42" s="3" t="s">
+      <c r="C42" s="8" t="s">
         <v>84</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E42" s="5" t="s">
+      <c r="E42" s="10" t="s">
         <v>86</v>
       </c>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
     </row>
     <row r="43" customFormat="false" ht="73.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="6"/>
       <c r="B43" s="7"/>
-      <c r="D43" s="4" t="s">
+      <c r="C43" s="8"/>
+      <c r="D43" s="9" t="s">
         <v>87</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="F43" s="5" t="s">
+      <c r="F43" s="10" t="s">
         <v>89</v>
       </c>
+      <c r="G43" s="10"/>
     </row>
     <row r="44" customFormat="false" ht="73.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="6"/>
       <c r="B44" s="7"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="9"/>
       <c r="E44" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="F44" s="5" t="s">
+      <c r="F44" s="10" t="s">
         <v>91</v>
       </c>
+      <c r="G44" s="10"/>
     </row>
     <row r="45" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="6"/>
       <c r="B45" s="7"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="9"/>
       <c r="E45" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="F45" s="5" t="s">
+      <c r="F45" s="10" t="s">
         <v>93</v>
       </c>
+      <c r="G45" s="10"/>
     </row>
     <row r="46" customFormat="false" ht="108.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="6"/>
       <c r="B46" s="7"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="9"/>
       <c r="E46" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="F46" s="19" t="s">
+      <c r="F46" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="G46" s="19"/>
-    </row>
-    <row r="47" customFormat="false" ht="36.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G46" s="18"/>
+    </row>
+    <row r="47" customFormat="false" ht="180.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="6"/>
       <c r="B47" s="7"/>
-      <c r="D47" s="4" t="s">
+      <c r="C47" s="8"/>
+      <c r="D47" s="9" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="48" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E47" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="220.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="6"/>
       <c r="B48" s="7"/>
-    </row>
-    <row r="49" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C48" s="8"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="26.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="6"/>
       <c r="B49" s="7"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="6"/>
       <c r="B50" s="7"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="12"/>
+      <c r="F50" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="G50" s="19" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="6"/>
       <c r="B51" s="7"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="12"/>
+      <c r="F51" s="12"/>
     </row>
     <row r="52" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="6"/>
       <c r="B52" s="7"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="12"/>
+      <c r="F52" s="12"/>
     </row>
     <row r="53" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="6"/>
       <c r="B53" s="7"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="12"/>
+      <c r="F53" s="12"/>
     </row>
     <row r="54" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="6"/>
       <c r="B54" s="7"/>
-    </row>
-    <row r="55" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C54" s="8"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="12"/>
+      <c r="F54" s="12"/>
+    </row>
+    <row r="55" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="6"/>
-      <c r="B55" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="75.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="7"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="12"/>
+      <c r="F55" s="12"/>
+    </row>
+    <row r="56" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="6"/>
       <c r="B56" s="7"/>
-      <c r="C56" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C56" s="8"/>
+    </row>
+    <row r="57" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="6"/>
       <c r="B57" s="7"/>
-      <c r="C57" s="3" t="s">
-        <v>99</v>
-      </c>
+      <c r="C57" s="8"/>
     </row>
     <row r="58" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="6"/>
+      <c r="B58" s="7"/>
     </row>
     <row r="59" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="6"/>
-    </row>
-    <row r="60" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B59" s="7"/>
+    </row>
+    <row r="60" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="6"/>
-    </row>
-    <row r="61" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="75.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="6"/>
-    </row>
-    <row r="62" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B61" s="7"/>
+      <c r="C61" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="6"/>
+      <c r="B62" s="7"/>
+      <c r="C62" s="3" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="6"/>
@@ -6261,15 +6657,25 @@
     <row r="64" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="6"/>
     </row>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="65" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="6"/>
+    </row>
+    <row r="66" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="6"/>
+    </row>
+    <row r="67" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="6"/>
+    </row>
+    <row r="68" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="6"/>
+    </row>
+    <row r="69" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="53">
-    <mergeCell ref="A1:A64"/>
-    <mergeCell ref="B1:B54"/>
+  <mergeCells count="57">
+    <mergeCell ref="A1:A69"/>
+    <mergeCell ref="B1:B59"/>
     <mergeCell ref="C1:C41"/>
     <mergeCell ref="D1:D4"/>
     <mergeCell ref="E1:G1"/>
@@ -6312,15 +6718,19 @@
     <mergeCell ref="F38:G38"/>
     <mergeCell ref="F39:G39"/>
     <mergeCell ref="F40:G40"/>
-    <mergeCell ref="C42:C52"/>
+    <mergeCell ref="C42:C57"/>
     <mergeCell ref="E42:G42"/>
     <mergeCell ref="D43:D46"/>
     <mergeCell ref="F43:G43"/>
     <mergeCell ref="F44:G44"/>
     <mergeCell ref="F45:G45"/>
     <mergeCell ref="F46:G46"/>
-    <mergeCell ref="D47:D50"/>
-    <mergeCell ref="B55:B57"/>
+    <mergeCell ref="D47:D55"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="E49:E55"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="B60:B62"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
@@ -6352,26 +6762,26 @@
   <sheetData>
     <row r="1" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="20" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>251</v>
+        <v>258</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="23" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>253</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="23" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -6436,10 +6846,10 @@
         <v>1</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6447,10 +6857,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6458,10 +6868,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6469,10 +6879,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6480,10 +6890,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6491,10 +6901,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="256.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6502,10 +6912,10 @@
         <v>7</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="245.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6513,10 +6923,10 @@
         <v>8</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="223.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6524,10 +6934,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="243.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6535,86 +6945,86 @@
         <v>10</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="20" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="20" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="20" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="288.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="20" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="F14" s="23" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="G14" s="23" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="20" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="240.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B16" s="20" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="20" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="20" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -6651,272 +7061,272 @@
   <sheetData>
     <row r="1" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="28" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="B1" s="28"/>
     </row>
     <row r="2" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="26" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="26" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="26" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="31" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="B8" s="31"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="32" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="34" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="B10" s="33" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="34" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="B11" s="35" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="33" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="33" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="B13" s="33" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="33" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="B14" s="33" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="33" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="B15" s="33" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="33" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="B16" s="33" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="33" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="B17" s="33" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="33" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="B18" s="33" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="33" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="B19" s="33" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="33" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="B20" s="33" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="33" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="B21" s="33" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="28" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="B25" s="28"/>
     </row>
     <row r="26" customFormat="false" ht="283.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="26" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="B26" s="29" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="26" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="B27" s="29" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="36" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="B28" s="29" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="26" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="B29" s="29" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="26" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="B30" s="29" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="26" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="B31" s="29" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="26" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="B32" s="29" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="26" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="B33" s="29" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="37" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="B34" s="29" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="37"/>
       <c r="B35" s="29" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="37"/>
       <c r="B36" s="29" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="37"/>
       <c r="B37" s="29" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="37"/>
       <c r="B38" s="29" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="37"/>
       <c r="B39" s="30" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="37"/>
       <c r="B40" s="29" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="26" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="B41" s="30" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -6978,18 +7388,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="23" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="20" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -7023,25 +7433,25 @@
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="27" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="27" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="27" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="27" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -7075,10 +7485,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="38" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="B1" s="39" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7086,120 +7496,120 @@
     </row>
     <row r="3" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="41" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="B3" s="42" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="41"/>
       <c r="B4" s="42" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="41"/>
       <c r="B5" s="27" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="41"/>
       <c r="B6" s="27" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="41"/>
       <c r="B7" s="27" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="41"/>
       <c r="B8" s="43" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="41"/>
       <c r="B9" s="43"/>
       <c r="C9" s="29" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="41"/>
       <c r="B10" s="43"/>
       <c r="C10" s="29" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="41"/>
       <c r="B11" s="43"/>
       <c r="C11" s="27" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="41"/>
       <c r="B12" s="43"/>
       <c r="C12" s="29" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="41"/>
       <c r="B13" s="27" t="s">
-        <v>227</v>
+        <v>234</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="216.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="41"/>
       <c r="B14" s="44" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="41"/>
       <c r="B15" s="44"/>
       <c r="C15" s="45" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="41"/>
       <c r="B16" s="44"/>
       <c r="C16" s="45" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="41"/>
       <c r="B17" s="44"/>
       <c r="C17" s="45" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="41"/>
       <c r="B18" s="44"/>
       <c r="C18" s="29" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7208,13 +7618,13 @@
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="41"/>
       <c r="B20" s="46" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="41"/>
       <c r="B21" s="27" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7225,40 +7635,40 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="41" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="B24" s="27" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="41"/>
       <c r="B25" s="27" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="41"/>
       <c r="B26" s="27" t="s">
-        <v>239</v>
+        <v>246</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="41"/>
       <c r="B27" s="27" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="41"/>
       <c r="B28" s="29" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="41"/>
       <c r="B29" s="29" t="s">
-        <v>242</v>
+        <v>249</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7266,41 +7676,41 @@
     </row>
     <row r="31" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="41" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
       <c r="B31" s="29" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
       <c r="F31" s="48"/>
     </row>
     <row r="32" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="41"/>
       <c r="B32" s="29" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="41"/>
       <c r="B33" s="29" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="41"/>
       <c r="B34" s="29" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="41"/>
       <c r="B35" s="29" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="41"/>
       <c r="B36" s="29" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="C36" s="29"/>
     </row>

</xml_diff>

<commit_message>
[feat][OS][OS: Process, file, device, management]
</commit_message>
<xml_diff>
--- a/Operations-System/DevOps-Documents.xlsx
+++ b/Operations-System/DevOps-Documents.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="270">
   <si>
     <t xml:space="preserve">Operating System Concepts</t>
   </si>
@@ -1544,7 +1544,28 @@
         <family val="0"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve"> - A program(</t>
+      <t xml:space="preserve"> - A </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">program</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">(</t>
     </r>
     <r>
       <rPr>
@@ -1566,8 +1587,50 @@
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">) include instructions(các lệnh/ các phép toán).
- - A CPU execute instruction → process
- - A process(</t>
+ - A CPU execute instructions → </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">process
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> - A </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">process</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">(</t>
     </r>
     <r>
       <rPr>
@@ -2660,9 +2723,9 @@
       <rPr>
         <sz val="15"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="134"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> - The API specifies a set of functions that are available to an application programmer, including the parameters that are passed to each function and the return values the programmer can expect.
  - API is benefit concerns program portability(tính linh động), program to compile and run on any system that supports API,…
@@ -2673,9 +2736,9 @@
         <u val="single"/>
         <sz val="15"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="134"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">libc</t>
     </r>
@@ -2683,9 +2746,9 @@
       <rPr>
         <sz val="15"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="134"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">.
  - Behind the scenes, the f</t>
@@ -2695,9 +2758,9 @@
         <u val="single"/>
         <sz val="15"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="134"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">unctions that make up an API </t>
     </r>
@@ -2705,9 +2768,9 @@
       <rPr>
         <sz val="15"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="134"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">typically invoke the </t>
     </r>
@@ -2716,9 +2779,9 @@
         <u val="single"/>
         <sz val="15"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="134"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">actual system calls</t>
     </r>
@@ -2726,9 +2789,9 @@
       <rPr>
         <sz val="15"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="134"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> on behalf of the application programmer.
  → System-call Interface: that serves as the link to system calls made available by the operating system.
@@ -2746,9 +2809,9 @@
       <rPr>
         <sz val="15"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="134"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> - System calls can be grouped roughly into </t>
     </r>
@@ -2757,9 +2820,9 @@
         <u val="single"/>
         <sz val="15"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="134"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">six major categories</t>
     </r>
@@ -2767,9 +2830,9 @@
       <rPr>
         <sz val="15"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="134"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">: process control, fil management, device management, information maintenance, communications, and protection.</t>
     </r>
@@ -2784,6 +2847,7 @@
         <color theme="1"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> - Process control system calls are a </t>
     </r>
@@ -2794,6 +2858,7 @@
         <color theme="1"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">set of kernel-level interfaces</t>
     </r>
@@ -2803,6 +2868,7 @@
         <color theme="1"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> that allow user-space programs to create, manage, and terminate processes. They form a core component of </t>
     </r>
@@ -2813,6 +2879,7 @@
         <color theme="1"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">process management</t>
     </r>
@@ -2822,6 +2889,7 @@
         <color theme="1"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> in an operating system and </t>
     </r>
@@ -2832,6 +2900,7 @@
         <color theme="1"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">enable multitasking</t>
     </r>
@@ -2841,6 +2910,7 @@
         <color theme="1"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">, allowing the OS to execute multiple programs </t>
     </r>
@@ -2851,6 +2921,7 @@
         <color theme="1"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">concurrently</t>
     </r>
@@ -2860,8 +2931,342 @@
         <color theme="1"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">.</t>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.
+ - A running program needs to be able to halt(dừng) its execution either normally (end()) or abnormally (abort()) → a dump of memory is sometimes taken and an error message generated.
+ - A dump of memory: Is essentially a snapshot of the contents of a program (or the system's) memory at the moment an error or abnormal termination occurs. When an application crashes or is terminated unexpectedly due to a system call or an error trap, the operating system may capture all the data that was present in the memory at that instant.  Written to log file on disk.
+ - After halt, OS transfer control to the invoking </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">command interpreter</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">. Command interpreter read and continues the next command.
+ - A process executing one program may want to load() and execute() another program, this feature allows the </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">command interpreter to execute a program as directed</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">The control returns to the existing program when the new program terminates</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, we must save the memory image of the existing program; thus, we have effectively created a mechanism for one program to call another program. I</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">f both programs continue concurrently, we have created a new process to be multiprogrammed</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">. Often, there is a system call specifically for this purpose (create process()).
+ - If we create a new process, we should be able to control its execution. This control requires the ability to determine and reset the attributes of a process. We may also want to terminate a process that we created (terminate process()). we may need to wait for them to finish their execution, we may want to wait for a certain amount of time to pass (wait time()), we will want to wait for a specific event to occur (wait event()) the processes should then signal when that event has occurred (signal event()).
+ - Two or more </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">processes may share data</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, operating systems often provide system calls allowing a process to </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">lock</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (acquire_lock() and release_lock())shared data, no other process can access the data until the lock is released</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">File Management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Device Management</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> - A process may need several resources to execute—main memory, disk drives, access to files, and so on. If the resources are available, they can be granted, and control can be returned to the user process. Otherwise, the process will have to wait until sufficient resources are available.
+ - The various resources controlled by the operating system can be thought of as devices (disk drives,…), while others can be thought of as abstract or virtual devices (for example, files).
+ - Other operating systems allow unmanaged access to devices. The hazard then is the potential for device contention and perhaps deadlock.
+ - In fact, the </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">similarity between I/O devices and files is so great that many operating systems</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, including UNIX, merge the two into a </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">combined file –device structure</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">. The user interface can also make files and devices appear to be similar, even though the underlying system calls are dissimilar. This is another example of the many design decisions that go into building an operating system and user interface.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Information Maintenance</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> - Many </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">system calls</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> exist simply for the purpose of </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">transferring information</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> between the </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">user</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> program and the OS.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Communication</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> - There are two common models of interprocess communication: the </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">message-passing model</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> and the </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">shared-memory model</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.
+ - In the message-passing model: 
+  + messages can be exchanged between the processes either directly or indirectly through a common mailbox.
+ - In the shared-memory model:</t>
     </r>
   </si>
   <si>
@@ -5048,7 +5453,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="31">
+  <fonts count="34">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5074,41 +5479,55 @@
     <font>
       <sz val="30"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Linux Libertine O"/>
       <family val="0"/>
-      <charset val="134"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="25"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Linux Libertine O"/>
       <family val="0"/>
-      <charset val="134"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="20"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Linux Libertine O"/>
       <family val="0"/>
-      <charset val="134"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Linux Libertine O"/>
       <family val="0"/>
-      <charset val="134"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="15"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Linux Libertine O"/>
       <family val="0"/>
-      <charset val="134"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Linux Libertine O"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="30"/>
+      <color theme="1"/>
+      <name val="Linux Libertine O"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="15"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="0"/>
@@ -5129,13 +5548,6 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="15"/>
@@ -5161,10 +5573,19 @@
       <charset val="1"/>
     </font>
     <font>
+      <u val="single"/>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Linux Libertine O"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="15"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -5172,6 +5593,15 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -5327,13 +5757,13 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="30" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
@@ -5362,7 +5792,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5386,35 +5820,31 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5422,11 +5852,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5434,15 +5864,15 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5450,7 +5880,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="25" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5462,11 +5892,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="25" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5474,7 +5904,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5482,19 +5912,19 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5502,7 +5932,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="29" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5510,7 +5940,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5518,19 +5948,19 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5620,9 +6050,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>585360</xdr:colOff>
+      <xdr:colOff>585000</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>2118240</xdr:rowOff>
+      <xdr:rowOff>2117880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5636,7 +6066,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10237320" y="8324640"/>
-          <a:ext cx="4798080" cy="2795400"/>
+          <a:ext cx="4797720" cy="2795040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5657,9 +6087,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>661680</xdr:colOff>
+      <xdr:colOff>661320</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>1794240</xdr:rowOff>
+      <xdr:rowOff>1793880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5673,7 +6103,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10323000" y="11420280"/>
-          <a:ext cx="4788720" cy="2490480"/>
+          <a:ext cx="4788360" cy="2490120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5694,9 +6124,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>518760</xdr:colOff>
+      <xdr:colOff>518400</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>693000</xdr:rowOff>
+      <xdr:rowOff>692640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5710,7 +6140,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10170720" y="24355440"/>
-          <a:ext cx="4798080" cy="2900160"/>
+          <a:ext cx="4797720" cy="2899800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5904,8 +6334,8 @@
   </sheetPr>
   <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D49" colorId="64" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F48" activeCellId="0" sqref="F48"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E49" colorId="64" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G52" activeCellId="0" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="36.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5917,123 +6347,124 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="5" width="15.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="5" width="19.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="5" width="206.01"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="8" style="6" width="8.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="92.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="11" t="s">
+      <c r="A2" s="7"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
     </row>
     <row r="3" customFormat="false" ht="57.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="11" t="s">
+      <c r="A3" s="7"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="10"/>
+      <c r="G3" s="13"/>
     </row>
     <row r="4" customFormat="false" ht="96.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="11" t="s">
+      <c r="A4" s="7"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="10"/>
+      <c r="G4" s="13"/>
     </row>
     <row r="5" customFormat="false" ht="58.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="9" t="s">
+      <c r="A5" s="7"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
     </row>
     <row r="6" customFormat="false" ht="151.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="11" t="s">
+      <c r="A6" s="7"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="10"/>
+      <c r="G6" s="13"/>
     </row>
     <row r="7" customFormat="false" ht="300.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="12" t="s">
+      <c r="A7" s="7"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="15" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="183.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="12" t="s">
+      <c r="A8" s="7"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="15" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="187.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="13" t="s">
+      <c r="A9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="14" t="s">
         <v>18</v>
       </c>
       <c r="G9" s="5" t="s">
@@ -6041,479 +6472,479 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="57.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="11" t="s">
+      <c r="A10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="15" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="335" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="12" t="s">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="G11" s="16" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="126.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="12" t="s">
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="G12" s="10"/>
+      <c r="G12" s="13"/>
     </row>
     <row r="13" customFormat="false" ht="126.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="9" t="s">
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="G13" s="10"/>
+      <c r="G13" s="13"/>
     </row>
     <row r="14" customFormat="false" ht="216.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="11" t="s">
+      <c r="A14" s="7"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="G14" s="10"/>
-    </row>
-    <row r="15" customFormat="false" ht="126.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="12" t="s">
+      <c r="G14" s="13"/>
+    </row>
+    <row r="15" customFormat="false" ht="129.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="7"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="G15" s="15" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="91" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="6"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="12" t="s">
+      <c r="A16" s="7"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F16" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="G16" s="10"/>
+      <c r="G16" s="13"/>
     </row>
     <row r="17" customFormat="false" ht="133.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="6"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="9" t="s">
+      <c r="A17" s="7"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
     </row>
     <row r="18" customFormat="false" ht="335" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="6"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="15" t="s">
+      <c r="A18" s="7"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F18" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="10"/>
+      <c r="G18" s="13"/>
     </row>
     <row r="19" customFormat="false" ht="144.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="6"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="12" t="s">
+      <c r="A19" s="7"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="G19" s="10"/>
+      <c r="G19" s="13"/>
     </row>
     <row r="20" customFormat="false" ht="73.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="6"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="16" t="s">
+      <c r="A20" s="7"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="F20" s="12" t="s">
+      <c r="F20" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="G20" s="17" t="s">
+      <c r="G20" s="5" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="77.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="6"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="11" t="s">
+      <c r="A21" s="7"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="G21" s="5" t="s">
+      <c r="G21" s="15" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="78.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="6"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="11"/>
+      <c r="A22" s="7"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
       <c r="G22" s="5" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="101.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="6"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="11"/>
+      <c r="A23" s="7"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
       <c r="G23" s="5" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="6"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="12" t="s">
+      <c r="A24" s="7"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
     </row>
     <row r="25" customFormat="false" ht="220.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="6"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="9" t="s">
+      <c r="A25" s="7"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E25" s="12" t="s">
+      <c r="E25" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="F25" s="10" t="s">
+      <c r="F25" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="G25" s="10"/>
+      <c r="G25" s="13"/>
     </row>
     <row r="26" customFormat="false" ht="55.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="6"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="12" t="s">
+      <c r="A26" s="7"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="F26" s="10" t="s">
+      <c r="F26" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="G26" s="10"/>
+      <c r="G26" s="11"/>
     </row>
     <row r="27" customFormat="false" ht="38.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="6"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="12" t="s">
+      <c r="A27" s="7"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="F27" s="10" t="s">
+      <c r="F27" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="G27" s="10"/>
-    </row>
-    <row r="28" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="6"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="12" t="s">
+      <c r="G27" s="11"/>
+    </row>
+    <row r="28" customFormat="false" ht="53.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="7"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
     </row>
     <row r="29" customFormat="false" ht="257.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="6"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="12" t="s">
+      <c r="A29" s="7"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="F29" s="10" t="s">
+      <c r="F29" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="G29" s="10"/>
+      <c r="G29" s="13"/>
     </row>
     <row r="30" customFormat="false" ht="38.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="6"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="12" t="s">
+      <c r="A30" s="7"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="F30" s="10" t="s">
+      <c r="F30" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="G30" s="10"/>
+      <c r="G30" s="11"/>
     </row>
     <row r="31" customFormat="false" ht="106.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="6"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="8"/>
+      <c r="A31" s="7"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="9"/>
       <c r="D31" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="E31" s="10" t="s">
+      <c r="E31" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
     </row>
     <row r="32" customFormat="false" ht="56.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="6"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="8"/>
+      <c r="A32" s="7"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="9"/>
       <c r="D32" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="E32" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
     </row>
     <row r="33" customFormat="false" ht="46" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="6"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="8"/>
+      <c r="A33" s="7"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="9"/>
       <c r="D33" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="E33" s="10" t="s">
+      <c r="E33" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
     </row>
     <row r="34" customFormat="false" ht="464.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="6"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="8"/>
+      <c r="A34" s="7"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="9"/>
       <c r="D34" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E34" s="10" t="s">
+      <c r="E34" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
     </row>
     <row r="35" customFormat="false" ht="56.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="6"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="9" t="s">
+      <c r="A35" s="7"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="E35" s="12" t="s">
+      <c r="E35" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="F35" s="10" t="s">
+      <c r="F35" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="G35" s="10"/>
+      <c r="G35" s="13"/>
     </row>
     <row r="36" customFormat="false" ht="108.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="6"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="12" t="s">
+      <c r="A36" s="7"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="F36" s="10" t="s">
+      <c r="F36" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="G36" s="10"/>
+      <c r="G36" s="13"/>
     </row>
     <row r="37" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="6"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="12" t="s">
+      <c r="A37" s="7"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="F37" s="10" t="s">
+      <c r="F37" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="G37" s="10"/>
+      <c r="G37" s="11"/>
     </row>
     <row r="38" customFormat="false" ht="91" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="6"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="12" t="s">
+      <c r="A38" s="7"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="F38" s="10" t="s">
+      <c r="F38" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="G38" s="10"/>
+      <c r="G38" s="13"/>
     </row>
     <row r="39" customFormat="false" ht="144.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="6"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="12" t="s">
+      <c r="A39" s="7"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="F39" s="10" t="s">
+      <c r="F39" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="G39" s="10"/>
+      <c r="G39" s="13"/>
     </row>
     <row r="40" customFormat="false" ht="162.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="6"/>
-      <c r="B40" s="7"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="12" t="s">
+      <c r="A40" s="7"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="F40" s="10" t="s">
+      <c r="F40" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="G40" s="10"/>
-    </row>
-    <row r="41" customFormat="false" ht="88.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="6"/>
-      <c r="B41" s="7"/>
-      <c r="C41" s="8"/>
+      <c r="G40" s="13"/>
+    </row>
+    <row r="41" customFormat="false" ht="87.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="7"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="9"/>
       <c r="D41" s="4" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="574.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="6"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="8" t="s">
+      <c r="A42" s="7"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="9" t="s">
         <v>84</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E42" s="10" t="s">
+      <c r="E42" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="F42" s="10"/>
-      <c r="G42" s="10"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="13"/>
     </row>
     <row r="43" customFormat="false" ht="73.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="6"/>
-      <c r="B43" s="7"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="9" t="s">
+      <c r="A43" s="7"/>
+      <c r="B43" s="8"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="10" t="s">
         <v>87</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="F43" s="10" t="s">
+      <c r="F43" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="G43" s="10"/>
+      <c r="G43" s="13"/>
     </row>
     <row r="44" customFormat="false" ht="73.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="6"/>
-      <c r="B44" s="7"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="9"/>
+      <c r="A44" s="7"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="10"/>
       <c r="E44" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="F44" s="10" t="s">
+      <c r="F44" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="G44" s="10"/>
+      <c r="G44" s="13"/>
     </row>
     <row r="45" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="6"/>
-      <c r="B45" s="7"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="9"/>
+      <c r="A45" s="7"/>
+      <c r="B45" s="8"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="10"/>
       <c r="E45" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="F45" s="10" t="s">
+      <c r="F45" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="G45" s="10"/>
+      <c r="G45" s="11"/>
     </row>
     <row r="46" customFormat="false" ht="108.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="6"/>
-      <c r="B46" s="7"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="9"/>
+      <c r="A46" s="7"/>
+      <c r="B46" s="8"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="10"/>
       <c r="E46" s="5" t="s">
         <v>94</v>
       </c>
@@ -6522,48 +6953,52 @@
       </c>
       <c r="G46" s="18"/>
     </row>
-    <row r="47" customFormat="false" ht="180.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="6"/>
-      <c r="B47" s="7"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="9" t="s">
+    <row r="47" customFormat="false" ht="184.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="7"/>
+      <c r="B47" s="8"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="E47" s="5" t="s">
+      <c r="E47" s="13" t="s">
         <v>97</v>
       </c>
+      <c r="F47" s="13"/>
+      <c r="G47" s="13"/>
     </row>
     <row r="48" customFormat="false" ht="220.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="6"/>
-      <c r="B48" s="7"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="12" t="s">
+      <c r="A48" s="7"/>
+      <c r="B48" s="8"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="F48" s="5" t="s">
+      <c r="F48" s="11" t="s">
         <v>99</v>
       </c>
+      <c r="G48" s="11"/>
     </row>
     <row r="49" customFormat="false" ht="26.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="6"/>
-      <c r="B49" s="7"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="9"/>
+      <c r="A49" s="7"/>
+      <c r="B49" s="8"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="10"/>
       <c r="E49" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="F49" s="5" t="s">
+      <c r="F49" s="11" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="50" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="6"/>
-      <c r="B50" s="7"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="9"/>
+      <c r="G49" s="11"/>
+    </row>
+    <row r="50" customFormat="false" ht="285.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="7"/>
+      <c r="B50" s="8"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="10"/>
       <c r="E50" s="12"/>
-      <c r="F50" s="12" t="s">
+      <c r="F50" s="14" t="s">
         <v>102</v>
       </c>
       <c r="G50" s="19" t="s">
@@ -6571,106 +7006,123 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="6"/>
-      <c r="B51" s="7"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="9"/>
+      <c r="A51" s="7"/>
+      <c r="B51" s="8"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="10"/>
       <c r="E51" s="12"/>
-      <c r="F51" s="12"/>
-    </row>
-    <row r="52" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="6"/>
-      <c r="B52" s="7"/>
-      <c r="C52" s="8"/>
-      <c r="D52" s="9"/>
+      <c r="F51" s="14" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="141.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="7"/>
+      <c r="B52" s="8"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="10"/>
       <c r="E52" s="12"/>
-      <c r="F52" s="12"/>
+      <c r="F52" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="6"/>
-      <c r="B53" s="7"/>
-      <c r="C53" s="8"/>
-      <c r="D53" s="9"/>
+      <c r="A53" s="7"/>
+      <c r="B53" s="8"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="10"/>
       <c r="E53" s="12"/>
-      <c r="F53" s="12"/>
-    </row>
-    <row r="54" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="6"/>
-      <c r="B54" s="7"/>
-      <c r="C54" s="8"/>
-      <c r="D54" s="9"/>
+      <c r="F53" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="G53" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="71.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="7"/>
+      <c r="B54" s="8"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="10"/>
       <c r="E54" s="12"/>
-      <c r="F54" s="12"/>
+      <c r="F54" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="6"/>
-      <c r="B55" s="7"/>
-      <c r="C55" s="8"/>
-      <c r="D55" s="9"/>
+      <c r="A55" s="7"/>
+      <c r="B55" s="8"/>
+      <c r="C55" s="9"/>
+      <c r="D55" s="10"/>
       <c r="E55" s="12"/>
-      <c r="F55" s="12"/>
+      <c r="F55" s="14"/>
     </row>
     <row r="56" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="6"/>
-      <c r="B56" s="7"/>
-      <c r="C56" s="8"/>
+      <c r="A56" s="7"/>
+      <c r="B56" s="8"/>
+      <c r="C56" s="9"/>
     </row>
     <row r="57" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="6"/>
-      <c r="B57" s="7"/>
-      <c r="C57" s="8"/>
+      <c r="A57" s="7"/>
+      <c r="B57" s="8"/>
+      <c r="C57" s="9"/>
     </row>
     <row r="58" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="6"/>
-      <c r="B58" s="7"/>
+      <c r="A58" s="7"/>
+      <c r="B58" s="8"/>
     </row>
     <row r="59" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="6"/>
-      <c r="B59" s="7"/>
+      <c r="A59" s="7"/>
+      <c r="B59" s="8"/>
     </row>
     <row r="60" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="6"/>
-      <c r="B60" s="7" t="s">
+      <c r="A60" s="7"/>
+      <c r="B60" s="8" t="s">
         <v>51</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="75.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="6"/>
-      <c r="B61" s="7"/>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="70.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="7"/>
+      <c r="B61" s="8"/>
       <c r="C61" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="6"/>
-      <c r="B62" s="7"/>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="47.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="7"/>
+      <c r="B62" s="8"/>
       <c r="C62" s="3" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="6"/>
+      <c r="A63" s="7"/>
     </row>
     <row r="64" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="6"/>
+      <c r="A64" s="7"/>
     </row>
     <row r="65" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="6"/>
+      <c r="A65" s="7"/>
     </row>
     <row r="66" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="6"/>
+      <c r="A66" s="7"/>
     </row>
     <row r="67" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="6"/>
+      <c r="A67" s="7"/>
     </row>
     <row r="68" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="6"/>
+      <c r="A68" s="7"/>
     </row>
     <row r="69" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="6"/>
+      <c r="A69" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="57">
@@ -6762,26 +7214,26 @@
   <sheetData>
     <row r="1" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="20" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>258</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="23" t="s">
-        <v>259</v>
+        <v>266</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>260</v>
+        <v>267</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="23" t="s">
-        <v>261</v>
+        <v>268</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>262</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -6846,10 +7298,10 @@
         <v>1</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6857,10 +7309,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6868,10 +7320,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6879,10 +7331,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6890,10 +7342,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6901,10 +7353,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="256.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6912,10 +7364,10 @@
         <v>7</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="245.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6923,10 +7375,10 @@
         <v>8</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="223.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6934,10 +7386,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="243.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6945,86 +7397,86 @@
         <v>10</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="20" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="20" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="20" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="288.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="20" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="F14" s="23" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="G14" s="23" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="20" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="240.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B16" s="20" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="20" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="20" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -7061,272 +7513,272 @@
   <sheetData>
     <row r="1" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="28" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="B1" s="28"/>
     </row>
     <row r="2" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="26" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="26" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="26" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="31" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="B8" s="31"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="32" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="34" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="B10" s="33" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="34" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="B11" s="35" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="33" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="33" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="B13" s="33" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="33" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="B14" s="33" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="33" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="B15" s="33" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="33" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="B16" s="33" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="33" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="B17" s="33" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="33" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="B18" s="33" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="33" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="B19" s="33" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="33" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="B20" s="33" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="33" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="B21" s="33" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="28" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="B25" s="28"/>
     </row>
     <row r="26" customFormat="false" ht="283.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="26" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="B26" s="29" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="26" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="B27" s="29" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="36" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="B28" s="29" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="26" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="B29" s="29" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="26" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="B30" s="29" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="26" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="B31" s="29" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="26" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="B32" s="29" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="26" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="B33" s="29" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="37" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="B34" s="29" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="37"/>
       <c r="B35" s="29" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="37"/>
       <c r="B36" s="29" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="37"/>
       <c r="B37" s="29" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="37"/>
       <c r="B38" s="29" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="37"/>
       <c r="B39" s="30" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="37"/>
       <c r="B40" s="29" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="26" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="B41" s="30" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -7388,18 +7840,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="23" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="20" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -7433,25 +7885,25 @@
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="27" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="27" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="27" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="27" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>
@@ -7485,10 +7937,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="38" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="B1" s="39" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7496,120 +7948,120 @@
     </row>
     <row r="3" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="41" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="B3" s="42" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="41"/>
       <c r="B4" s="42" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="41"/>
       <c r="B5" s="27" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="41"/>
       <c r="B6" s="27" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="41"/>
       <c r="B7" s="27" t="s">
-        <v>227</v>
+        <v>234</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="41"/>
       <c r="B8" s="43" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="41"/>
       <c r="B9" s="43"/>
       <c r="C9" s="29" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="41"/>
       <c r="B10" s="43"/>
       <c r="C10" s="29" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="41"/>
       <c r="B11" s="43"/>
       <c r="C11" s="27" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="41"/>
       <c r="B12" s="43"/>
       <c r="C12" s="29" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="41"/>
       <c r="B13" s="27" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="216.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="41"/>
       <c r="B14" s="44" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="41"/>
       <c r="B15" s="44"/>
       <c r="C15" s="45" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="41"/>
       <c r="B16" s="44"/>
       <c r="C16" s="45" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="41"/>
       <c r="B17" s="44"/>
       <c r="C17" s="45" t="s">
-        <v>239</v>
+        <v>246</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="41"/>
       <c r="B18" s="44"/>
       <c r="C18" s="29" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7618,13 +8070,13 @@
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="41"/>
       <c r="B20" s="46" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="41"/>
       <c r="B21" s="27" t="s">
-        <v>242</v>
+        <v>249</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7635,40 +8087,40 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="41" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
       <c r="B24" s="27" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="41"/>
       <c r="B25" s="27" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="41"/>
       <c r="B26" s="27" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="41"/>
       <c r="B27" s="27" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="41"/>
       <c r="B28" s="29" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="41"/>
       <c r="B29" s="29" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7676,41 +8128,41 @@
     </row>
     <row r="31" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="41" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="B31" s="29" t="s">
-        <v>251</v>
+        <v>258</v>
       </c>
       <c r="F31" s="48"/>
     </row>
     <row r="32" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="41"/>
       <c r="B32" s="29" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="41"/>
       <c r="B33" s="29" t="s">
-        <v>253</v>
+        <v>260</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="41"/>
       <c r="B34" s="29" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="41"/>
       <c r="B35" s="29" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="41"/>
       <c r="B36" s="29" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="C36" s="29"/>
     </row>

</xml_diff>

<commit_message>
[feat][OS][System calls: Communications, Protections + System Services: Filemanagement, Status Information, File modificators,...]
</commit_message>
<xml_diff>
--- a/Operations-System/DevOps-Documents.xlsx
+++ b/Operations-System/DevOps-Documents.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="275">
   <si>
     <t xml:space="preserve">Operating System Concepts</t>
   </si>
@@ -3265,9 +3265,149 @@
       </rPr>
       <t xml:space="preserve">.
  - In the message-passing model: 
-  + messages can be exchanged between the processes either directly or indirectly through a common mailbox.
- - In the shared-memory model:</t>
-    </r>
+  + Messages can be exchanged(a connection must be opened) between the processes either directly or indirectly through a common mailbox.
+  + Each computer in a network has a </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">host name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> by which it is commonly known. A host also has a network identifier, such as an IP address. 
+  + Similarly, each process has a </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">process name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, and this name is translated into an identifier by which the operating system can refer to the process.
+  + The source of the communication, known as the </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">client</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, and the receiving daemon, known as a </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">server</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, then exchange messages
+ - In the shared-memory model:
+  + Processes create and gain access to regions of memory owned by other processes.
+ - </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Shared memory allows maximum speed and convenience of communication</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, since it can be done at memory transfer speeds when it takes place within a computer. Problems exist, however, in the areas of protection and synchronization between the processes sharing memory.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Protection</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Protection provides a mechanism for controlling access to the resources provided by a computer system.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Services</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - At the lowest level is hardware → Next is the OS → The system services → Application programs.
+ - System services: provide a convenient environment for program development and execution.
+ - File management:
+ - Status information: 
+  + Simply ask the system for the date, time, amount of available memory space,…
+  + More complex: detailed performance, logging, and debugging information…
+ - File modification
+ - Programming-language support
+ - Program loading and execution: 
+  + Once a program is assembled or compiled, it must be loaded into memory to be executed. 
+  + The system may provide absolute loaders, relocatable loaders, linkage editors, and overlay loaders. 
+  + Debugging systems for either higher-level languages or machine language are needed as well.
+ - Communications:
+  + These programs provide the mechanism for creating virtual connections among processes, users, and computer systems. 
+  + They allow users to send messages to one another’s screens, to browse web pages, to send e-mail messages, to log in remotely, or to transfer files from one machine to another.
+ - Background services:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linkers and Loaders</t>
   </si>
   <si>
     <t xml:space="preserve">Processes</t>
@@ -5792,7 +5932,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6050,9 +6190,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>585000</xdr:colOff>
+      <xdr:colOff>584640</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>2117880</xdr:rowOff>
+      <xdr:rowOff>2117520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6066,7 +6206,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10237320" y="8324640"/>
-          <a:ext cx="4797720" cy="2795040"/>
+          <a:ext cx="4797360" cy="2794680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6087,9 +6227,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>661320</xdr:colOff>
+      <xdr:colOff>660960</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>1793880</xdr:rowOff>
+      <xdr:rowOff>1793520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6103,7 +6243,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10323000" y="11420280"/>
-          <a:ext cx="4788360" cy="2490120"/>
+          <a:ext cx="4788000" cy="2489760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6124,9 +6264,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>518400</xdr:colOff>
+      <xdr:colOff>518040</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>692640</xdr:rowOff>
+      <xdr:rowOff>692280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6140,7 +6280,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10170720" y="24355440"/>
-          <a:ext cx="4797720" cy="2899800"/>
+          <a:ext cx="4797360" cy="2899440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6332,10 +6472,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G69"/>
+  <dimension ref="A1:G72"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E49" colorId="64" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G52" activeCellId="0" sqref="G52"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D53" colorId="64" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G54" activeCellId="0" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="36.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6540,7 +6680,7 @@
       </c>
       <c r="G14" s="13"/>
     </row>
-    <row r="15" customFormat="false" ht="129.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="126.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="9"/>
@@ -6707,7 +6847,7 @@
       </c>
       <c r="G27" s="11"/>
     </row>
-    <row r="28" customFormat="false" ht="53.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="7"/>
       <c r="B28" s="8"/>
       <c r="C28" s="9"/>
@@ -6876,7 +7016,7 @@
       </c>
       <c r="G40" s="13"/>
     </row>
-    <row r="41" customFormat="false" ht="87.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="7"/>
       <c r="B41" s="8"/>
       <c r="C41" s="9"/>
@@ -6992,7 +7132,7 @@
       </c>
       <c r="G49" s="11"/>
     </row>
-    <row r="50" customFormat="false" ht="285.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="280.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="7"/>
       <c r="B50" s="8"/>
       <c r="C50" s="9"/>
@@ -7015,7 +7155,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="141.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="138.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="7"/>
       <c r="B52" s="8"/>
       <c r="C52" s="9"/>
@@ -7041,7 +7181,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="71.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="190.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="7"/>
       <c r="B54" s="8"/>
       <c r="C54" s="9"/>
@@ -7060,57 +7200,77 @@
       <c r="C55" s="9"/>
       <c r="D55" s="10"/>
       <c r="E55" s="12"/>
-      <c r="F55" s="14"/>
-    </row>
-    <row r="56" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F55" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="G55" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="281" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="7"/>
       <c r="B56" s="8"/>
       <c r="C56" s="9"/>
-    </row>
-    <row r="57" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D56" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="7"/>
       <c r="B57" s="8"/>
       <c r="C57" s="9"/>
+      <c r="D57" s="4" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="7"/>
       <c r="B58" s="8"/>
+      <c r="C58" s="9"/>
     </row>
     <row r="59" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="7"/>
       <c r="B59" s="8"/>
-    </row>
-    <row r="60" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C59" s="9"/>
+    </row>
+    <row r="60" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="7"/>
-      <c r="B60" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="70.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="8"/>
+      <c r="C60" s="9"/>
+    </row>
+    <row r="61" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="7"/>
       <c r="B61" s="8"/>
-      <c r="C61" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="47.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="62" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="7"/>
       <c r="B62" s="8"/>
-      <c r="C62" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="63" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="7"/>
-    </row>
-    <row r="64" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B63" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="70.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="7"/>
-    </row>
-    <row r="65" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B64" s="8"/>
+      <c r="C64" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="47.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="7"/>
+      <c r="B65" s="8"/>
+      <c r="C65" s="3" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="7"/>
@@ -7124,10 +7284,19 @@
     <row r="69" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="7"/>
     </row>
+    <row r="70" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="7"/>
+    </row>
+    <row r="71" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="7"/>
+    </row>
+    <row r="72" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="7"/>
+    </row>
   </sheetData>
-  <mergeCells count="57">
-    <mergeCell ref="A1:A69"/>
-    <mergeCell ref="B1:B59"/>
+  <mergeCells count="58">
+    <mergeCell ref="A1:A72"/>
+    <mergeCell ref="B1:B62"/>
     <mergeCell ref="C1:C41"/>
     <mergeCell ref="D1:D4"/>
     <mergeCell ref="E1:G1"/>
@@ -7170,7 +7339,7 @@
     <mergeCell ref="F38:G38"/>
     <mergeCell ref="F39:G39"/>
     <mergeCell ref="F40:G40"/>
-    <mergeCell ref="C42:C57"/>
+    <mergeCell ref="C42:C60"/>
     <mergeCell ref="E42:G42"/>
     <mergeCell ref="D43:D46"/>
     <mergeCell ref="F43:G43"/>
@@ -7182,7 +7351,8 @@
     <mergeCell ref="F48:G48"/>
     <mergeCell ref="E49:E55"/>
     <mergeCell ref="F49:G49"/>
-    <mergeCell ref="B60:B62"/>
+    <mergeCell ref="E56:G56"/>
+    <mergeCell ref="B63:B65"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
@@ -7214,26 +7384,26 @@
   <sheetData>
     <row r="1" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="20" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="23" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="23" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -7298,10 +7468,10 @@
         <v>1</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7309,10 +7479,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7320,10 +7490,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7331,10 +7501,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7342,10 +7512,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7353,10 +7523,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="256.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7364,10 +7534,10 @@
         <v>7</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="245.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7375,10 +7545,10 @@
         <v>8</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="223.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7386,10 +7556,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="243.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7397,86 +7567,86 @@
         <v>10</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="20" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="20" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="20" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="288.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="20" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="F14" s="23" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="G14" s="23" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="20" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="240.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B16" s="20" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="20" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="20" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -7513,272 +7683,272 @@
   <sheetData>
     <row r="1" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="28" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="B1" s="28"/>
     </row>
     <row r="2" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="26" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="26" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="26" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="31" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="B8" s="31"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="32" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="34" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="B10" s="33" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="34" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="B11" s="35" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="33" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="33" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="B13" s="33" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="33" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="B14" s="33" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="33" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="B15" s="33" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="33" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="B16" s="33" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="33" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="B17" s="33" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="33" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="B18" s="33" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="33" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="B19" s="33" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="33" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="B20" s="33" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="33" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="B21" s="33" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="28" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="B25" s="28"/>
     </row>
     <row r="26" customFormat="false" ht="283.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="26" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="B26" s="29" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="26" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="B27" s="29" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="36" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="B28" s="29" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="26" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="B29" s="29" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="26" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="B30" s="29" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="26" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="B31" s="29" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="26" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="B32" s="29" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="26" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="B33" s="29" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="37" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="B34" s="29" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="37"/>
       <c r="B35" s="29" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="37"/>
       <c r="B36" s="29" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="37"/>
       <c r="B37" s="29" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="37"/>
       <c r="B38" s="29" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="37"/>
       <c r="B39" s="30" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="37"/>
       <c r="B40" s="29" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="26" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="B41" s="30" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -7840,18 +8010,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="23" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="20" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -7885,25 +8055,25 @@
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="27" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="27" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="27" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="27" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -7937,10 +8107,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="38" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="B1" s="39" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7948,120 +8118,120 @@
     </row>
     <row r="3" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="41" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="B3" s="42" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="41"/>
       <c r="B4" s="42" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="41"/>
       <c r="B5" s="27" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="41"/>
       <c r="B6" s="27" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="41"/>
       <c r="B7" s="27" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="41"/>
       <c r="B8" s="43" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="41"/>
       <c r="B9" s="43"/>
       <c r="C9" s="29" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="41"/>
       <c r="B10" s="43"/>
       <c r="C10" s="29" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="41"/>
       <c r="B11" s="43"/>
       <c r="C11" s="27" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="41"/>
       <c r="B12" s="43"/>
       <c r="C12" s="29" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="41"/>
       <c r="B13" s="27" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="216.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="41"/>
       <c r="B14" s="44" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="41"/>
       <c r="B15" s="44"/>
       <c r="C15" s="45" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="41"/>
       <c r="B16" s="44"/>
       <c r="C16" s="45" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="41"/>
       <c r="B17" s="44"/>
       <c r="C17" s="45" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="41"/>
       <c r="B18" s="44"/>
       <c r="C18" s="29" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8070,13 +8240,13 @@
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="41"/>
       <c r="B20" s="46" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="41"/>
       <c r="B21" s="27" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8087,40 +8257,40 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="41" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="B24" s="27" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="41"/>
       <c r="B25" s="27" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="41"/>
       <c r="B26" s="27" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="41"/>
       <c r="B27" s="27" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="41"/>
       <c r="B28" s="29" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="41"/>
       <c r="B29" s="29" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8128,41 +8298,41 @@
     </row>
     <row r="31" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="41" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="B31" s="29" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="F31" s="48"/>
     </row>
     <row r="32" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="41"/>
       <c r="B32" s="29" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="41"/>
       <c r="B33" s="29" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="41"/>
       <c r="B34" s="29" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="41"/>
       <c r="B35" s="29" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="41"/>
       <c r="B36" s="29" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="C36" s="29"/>
     </row>

</xml_diff>

<commit_message>
[feat][OS][OS: Linkers and Loaders]
</commit_message>
<xml_diff>
--- a/Operations-System/DevOps-Documents.xlsx
+++ b/Operations-System/DevOps-Documents.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="276">
   <si>
     <t xml:space="preserve">Operating System Concepts</t>
   </si>
@@ -3410,6 +3410,296 @@
     <t xml:space="preserve">Linkers and Loaders</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> - Usually, a program resides on disk as a binary executable file. To run on a CPU, the program must be brought into memory and placed in the context of process:
+  + Source files (source program ex: main.c, main.java, main.py,…) compiled into object files(designed to be loaded into any physical memory location, a format known as an </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">relocatable object file</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">).
+  + The </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">linker</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">combines relocatable object files</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">other object file or libraries</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> into a single </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">binary executable file</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.
+  + A </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">loader</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> is used to </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">load the binary executable file into memory</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, where it is eligible to run on a CPU core.
+  + Relocation: which assigns final addresses to the program parts and adjusts code and data in the program to match those addresses.
+- When a </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">program name is entered on the command line</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> on UNIX systems—for example, ./main —the </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">shell first creates a new process</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> to run the program using the </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">fork() system call</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">. The shell then </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">invokes the loader with the exec() system call</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">passing exec() the name of the executable file</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">. The loader then </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">loads the specified program into memory</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> using the address space of the newly created process.</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">Processes</t>
   </si>
   <si>
@@ -5593,7 +5883,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="34">
+  <fonts count="35">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5741,6 +6031,14 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Linux Libertine O"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
@@ -5897,13 +6195,13 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="31" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="34" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
@@ -5992,11 +6290,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6004,15 +6302,15 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6020,7 +6318,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6032,11 +6330,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6044,7 +6342,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6052,19 +6350,19 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6072,7 +6370,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="30" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6080,7 +6378,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6088,19 +6386,19 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="34" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6190,9 +6488,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>584640</xdr:colOff>
+      <xdr:colOff>583920</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>2117520</xdr:rowOff>
+      <xdr:rowOff>2116800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6206,7 +6504,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10237320" y="8324640"/>
-          <a:ext cx="4797360" cy="2794680"/>
+          <a:ext cx="4796640" cy="2793960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6227,9 +6525,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>660960</xdr:colOff>
+      <xdr:colOff>660240</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>1793520</xdr:rowOff>
+      <xdr:rowOff>1792800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6243,7 +6541,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10323000" y="11420280"/>
-          <a:ext cx="4788000" cy="2489760"/>
+          <a:ext cx="4787280" cy="2489040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6264,9 +6562,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>518040</xdr:colOff>
+      <xdr:colOff>517320</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>692280</xdr:rowOff>
+      <xdr:rowOff>691560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6280,7 +6578,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10170720" y="24355440"/>
-          <a:ext cx="4797360" cy="2899440"/>
+          <a:ext cx="4796640" cy="2898720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6472,10 +6770,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G72"/>
+  <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D53" colorId="64" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G54" activeCellId="0" sqref="G54"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D56" colorId="64" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G59" activeCellId="0" sqref="G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="36.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7214,17 +7512,24 @@
       <c r="D56" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="E56" s="5" t="s">
+      <c r="E56" s="11" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="57" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F56" s="11"/>
+      <c r="G56" s="11"/>
+    </row>
+    <row r="57" customFormat="false" ht="123.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="7"/>
       <c r="B57" s="8"/>
       <c r="C57" s="9"/>
       <c r="D57" s="4" t="s">
         <v>115</v>
       </c>
+      <c r="E57" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="F57" s="11"/>
+      <c r="G57" s="11"/>
     </row>
     <row r="58" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="7"/>
@@ -7255,21 +7560,21 @@
         <v>51</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="70.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="7"/>
       <c r="B64" s="8"/>
       <c r="C64" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="47.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="7"/>
       <c r="B65" s="8"/>
       <c r="C65" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7293,8 +7598,9 @@
     <row r="72" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="7"/>
     </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="58">
+  <mergeCells count="59">
     <mergeCell ref="A1:A72"/>
     <mergeCell ref="B1:B62"/>
     <mergeCell ref="C1:C41"/>
@@ -7352,6 +7658,7 @@
     <mergeCell ref="E49:E55"/>
     <mergeCell ref="F49:G49"/>
     <mergeCell ref="E56:G56"/>
+    <mergeCell ref="E57:G57"/>
     <mergeCell ref="B63:B65"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -7384,26 +7691,26 @@
   <sheetData>
     <row r="1" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="20" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="23" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="23" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -7468,10 +7775,10 @@
         <v>1</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7479,10 +7786,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7490,10 +7797,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7501,10 +7808,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7512,10 +7819,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7523,10 +7830,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="256.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7534,10 +7841,10 @@
         <v>7</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="245.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7545,10 +7852,10 @@
         <v>8</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="223.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7556,10 +7863,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="243.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7567,86 +7874,86 @@
         <v>10</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="20" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="20" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="20" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="288.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F14" s="23" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="G14" s="23" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="20" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="240.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B16" s="20" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="20" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="20" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -7683,272 +7990,272 @@
   <sheetData>
     <row r="1" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="28" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B1" s="28"/>
     </row>
     <row r="2" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="26" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="26" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="26" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="31" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B8" s="31"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="32" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="34" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B10" s="33" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="34" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B11" s="35" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="33" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="33" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B13" s="33" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="33" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B14" s="33" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="33" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B15" s="33" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="33" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B16" s="33" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="33" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B17" s="33" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="33" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B18" s="33" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="33" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B19" s="33" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="33" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B20" s="33" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="33" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B21" s="33" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="28" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B25" s="28"/>
     </row>
     <row r="26" customFormat="false" ht="283.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="26" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B26" s="29" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="26" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B27" s="29" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="36" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B28" s="29" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="26" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B29" s="29" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="26" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B30" s="29" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="26" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B31" s="29" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="26" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B32" s="29" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="26" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B33" s="29" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="37" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B34" s="29" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="37"/>
       <c r="B35" s="29" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="37"/>
       <c r="B36" s="29" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="37"/>
       <c r="B37" s="29" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="37"/>
       <c r="B38" s="29" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="37"/>
       <c r="B39" s="30" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="37"/>
       <c r="B40" s="29" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="26" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B41" s="30" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -8010,18 +8317,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="23" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="20" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -8055,25 +8362,25 @@
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="27" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="27" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="27" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="27" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -8107,10 +8414,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="38" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B1" s="39" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8118,120 +8425,120 @@
     </row>
     <row r="3" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="41" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B3" s="42" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="41"/>
       <c r="B4" s="42" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="41"/>
       <c r="B5" s="27" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="41"/>
       <c r="B6" s="27" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="41"/>
       <c r="B7" s="27" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="41"/>
       <c r="B8" s="43" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="41"/>
       <c r="B9" s="43"/>
       <c r="C9" s="29" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="41"/>
       <c r="B10" s="43"/>
       <c r="C10" s="29" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="41"/>
       <c r="B11" s="43"/>
       <c r="C11" s="27" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="41"/>
       <c r="B12" s="43"/>
       <c r="C12" s="29" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="41"/>
       <c r="B13" s="27" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="216.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="41"/>
       <c r="B14" s="44" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="41"/>
       <c r="B15" s="44"/>
       <c r="C15" s="45" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="41"/>
       <c r="B16" s="44"/>
       <c r="C16" s="45" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="41"/>
       <c r="B17" s="44"/>
       <c r="C17" s="45" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="41"/>
       <c r="B18" s="44"/>
       <c r="C18" s="29" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8240,13 +8547,13 @@
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="41"/>
       <c r="B20" s="46" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="41"/>
       <c r="B21" s="27" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8257,40 +8564,40 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="41" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B24" s="27" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="41"/>
       <c r="B25" s="27" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="41"/>
       <c r="B26" s="27" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="41"/>
       <c r="B27" s="27" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="41"/>
       <c r="B28" s="29" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="41"/>
       <c r="B29" s="29" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8298,41 +8605,41 @@
     </row>
     <row r="31" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="41" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B31" s="29" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="F31" s="48"/>
     </row>
     <row r="32" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="41"/>
       <c r="B32" s="29" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="41"/>
       <c r="B33" s="29" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="41"/>
       <c r="B34" s="29" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="41"/>
       <c r="B35" s="29" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="41"/>
       <c r="B36" s="29" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C36" s="29"/>
     </row>

</xml_diff>

<commit_message>
[feat][OS][Process Scheduling: Scheduling Queues]
</commit_message>
<xml_diff>
--- a/Operations-System/DevOps-Documents.xlsx
+++ b/Operations-System/DevOps-Documents.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="315">
   <si>
     <t xml:space="preserve">Operating System Concepts</t>
   </si>
@@ -5023,13 +5023,325 @@
     <t xml:space="preserve">Threads</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> - A process is a program, that performs single </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">thread</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> of execution. 
+ - </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Single thread</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> of control allows the process to </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">perform only one task at a time</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.
+ - Most modern operating systems allow a process to have </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">multiple threads</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> of execution and thus to </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">perform more than one task at a time</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">. (multiple core system).
+ - On systems that support threads, the PCB is expanded to include information for each thread.</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">Process Scheduling</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> - Multiple programming: Several processes (each an independent instance of a program) are loaded into memory and can be scheduled by the operating system.
+ - Multiple thread: A thread is a lightweight unit of execution within a process. A process can have one or more threads, which share the same virtual address space and resources like heap and global variables.
+ - Process scheduler: Selects an available process (possibly from a set of several available processes) for program execution on a core.
+ - CPU core:
+  + A system single CPU core will never perform more than one process running at a time.
+  + A multicore system can run multiple processes at one time.
+ - If more </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">processes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> than cores, processes wait until a core is free and can be rescheduled.
+ - An I/O-bound process: spends more of its time doing I/O than it spends doing computations.
+ - A CPU-bound process, in contrast, generates I/O requests infrequently, using more of its time doing computations.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Scheduling queues</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> - Ready queue: A linked list store processes(process control block: PCB) </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ready</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">waiting</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> to execute on a CPU’s core.
+ - Processes that are waiting for a certain event to occur are placed in a </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">wait queue</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Queueing diagram</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">: A common representation of </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">process scheduling</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.
+ 1. When program (executable file) load from disk into memory →  A new process is initially (state = “new”) 
+ 2. After initialization, put process in the ready queue (state = “ready”).
+ 2. The process allocated a CPU core and is executing (state = “running”).
+ 3. One several events could occur:
+  - issue an I/O request and then process placed in </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">I/O wait queue</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (state = “waiting”) waiting for I/O complete. If I/O complete the process moved into ready queue.
+  - create a chill process (status = “new”) and while parent process (status = “waiting”) awaits the child’s termination in waiting queue. When child process termination, process moved into ready queue.
+  - could be removed forcibly from the core (time slice expired, interrupt,...). Process moved into ready queue.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">CPU Scheduling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Context switch</t>
+  </si>
+  <si>
     <t xml:space="preserve">Threads &amp; Concurrency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CPU Scheduling</t>
   </si>
   <si>
     <t xml:space="preserve">Kiến Trúc về Microservice</t>
@@ -7206,7 +7518,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="36">
+  <fonts count="37">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -7374,6 +7686,12 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Linux Libertine O"/>
+      <family val="0"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -7527,17 +7845,17 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="32" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="33" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="35" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="36" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="50">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -7622,19 +7940,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -7642,15 +7956,15 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -7658,7 +7972,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="28" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -7670,11 +7984,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="28" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -7682,7 +7996,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -7690,19 +8004,19 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -7710,7 +8024,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="31" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="32" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -7718,7 +8032,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -7726,19 +8040,19 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="35" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="36" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -7828,9 +8142,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>581760</xdr:colOff>
+      <xdr:colOff>581400</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>2114640</xdr:rowOff>
+      <xdr:rowOff>2114280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7844,7 +8158,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10237320" y="8324640"/>
-          <a:ext cx="4794480" cy="2791800"/>
+          <a:ext cx="4794120" cy="2791440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7865,9 +8179,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>658080</xdr:colOff>
+      <xdr:colOff>657720</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>1790640</xdr:rowOff>
+      <xdr:rowOff>1790280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7881,7 +8195,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10323000" y="11420280"/>
-          <a:ext cx="4785120" cy="2486880"/>
+          <a:ext cx="4784760" cy="2486520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7902,9 +8216,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>515160</xdr:colOff>
+      <xdr:colOff>514800</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>689400</xdr:rowOff>
+      <xdr:rowOff>689040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7918,7 +8232,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10170720" y="24355440"/>
-          <a:ext cx="4794480" cy="2896560"/>
+          <a:ext cx="4794120" cy="2896200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8110,10 +8424,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G88"/>
+  <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D73" colorId="64" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G79" activeCellId="0" sqref="G79"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D74" colorId="64" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F76" activeCellId="0" sqref="F76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="36.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9036,11 +9350,11 @@
       <c r="D70" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="E70" s="21" t="s">
+      <c r="E70" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="F70" s="21"/>
-      <c r="G70" s="21"/>
+      <c r="F70" s="11"/>
+      <c r="G70" s="11"/>
     </row>
     <row r="71" customFormat="false" ht="310.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="7"/>
@@ -9054,9 +9368,10 @@
       <c r="E71" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="F71" s="5" t="s">
+      <c r="F71" s="11" t="s">
         <v>145</v>
       </c>
+      <c r="G71" s="11"/>
     </row>
     <row r="72" customFormat="false" ht="176.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="7"/>
@@ -9066,9 +9381,10 @@
       <c r="E72" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="F72" s="5" t="s">
+      <c r="F72" s="11" t="s">
         <v>147</v>
       </c>
+      <c r="G72" s="11"/>
     </row>
     <row r="73" customFormat="false" ht="193.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="7"/>
@@ -9078,11 +9394,12 @@
       <c r="E73" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="F73" s="5" t="s">
+      <c r="F73" s="11" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="74" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G73" s="11"/>
+    </row>
+    <row r="74" customFormat="false" ht="70.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="7"/>
       <c r="B74" s="8"/>
       <c r="C74" s="9"/>
@@ -9090,48 +9407,68 @@
       <c r="E74" s="14" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="75" customFormat="false" ht="36.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F74" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="G74" s="11"/>
+    </row>
+    <row r="75" customFormat="false" ht="158.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="7"/>
       <c r="B75" s="8"/>
       <c r="C75" s="9"/>
-      <c r="D75" s="4" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D75" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="211.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="7"/>
       <c r="B76" s="8"/>
       <c r="C76" s="9"/>
+      <c r="D76" s="10"/>
+      <c r="E76" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="F76" s="5" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="77" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="7"/>
       <c r="B77" s="8"/>
       <c r="C77" s="9"/>
+      <c r="D77" s="10"/>
+      <c r="E77" s="14" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="78" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="7"/>
       <c r="B78" s="8"/>
       <c r="C78" s="9"/>
-    </row>
-    <row r="79" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D78" s="10"/>
+      <c r="E78" s="14" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="70.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="7"/>
       <c r="B79" s="8"/>
-      <c r="C79" s="9"/>
-    </row>
-    <row r="80" customFormat="false" ht="70.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C79" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="47.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="7"/>
       <c r="B80" s="8"/>
       <c r="C80" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="47.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="7"/>
-      <c r="B81" s="8"/>
-      <c r="C81" s="3" t="s">
-        <v>153</v>
-      </c>
     </row>
     <row r="82" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="7"/>
@@ -9151,12 +9488,10 @@
     <row r="87" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="7"/>
     </row>
-    <row r="88" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="7"/>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="82">
-    <mergeCell ref="A1:A88"/>
+  <mergeCells count="84">
+    <mergeCell ref="A1:A87"/>
     <mergeCell ref="B1:B69"/>
     <mergeCell ref="C1:C41"/>
     <mergeCell ref="D1:D4"/>
@@ -9231,13 +9566,15 @@
     <mergeCell ref="F69:G69"/>
     <mergeCell ref="D70:D74"/>
     <mergeCell ref="E70:G70"/>
-    <mergeCell ref="B71:B81"/>
-    <mergeCell ref="C71:C79"/>
+    <mergeCell ref="B71:B80"/>
+    <mergeCell ref="C71:C78"/>
     <mergeCell ref="F71:G71"/>
     <mergeCell ref="F72:G72"/>
     <mergeCell ref="F73:G73"/>
     <mergeCell ref="F74:G74"/>
-    <mergeCell ref="D75:D79"/>
+    <mergeCell ref="D75:D78"/>
+    <mergeCell ref="E75:G75"/>
+    <mergeCell ref="F76:G76"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
@@ -9262,33 +9599,33 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="22" width="23.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="22" width="57.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="3" style="22" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="21" width="23.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="21" width="57.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="3" style="21" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="22" t="s">
-        <v>304</v>
-      </c>
-      <c r="B1" s="25" t="s">
-        <v>305</v>
+      <c r="A1" s="21" t="s">
+        <v>309</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="25" t="s">
-        <v>306</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>307</v>
+      <c r="A2" s="24" t="s">
+        <v>311</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="25" t="s">
-        <v>308</v>
-      </c>
-      <c r="B3" s="25" t="s">
-        <v>309</v>
+      <c r="A3" s="24" t="s">
+        <v>313</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -9338,200 +9675,200 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="22" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="22" width="39.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="22" width="95.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="22" width="60.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="22" width="58.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="22" width="50"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="22" width="49.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="8" style="22" width="9.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="21" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="21" width="39.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="21" width="95.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="21" width="60.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="21" width="58.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="21" width="50"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="21" width="49.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="8" style="21" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="22" t="n">
+      <c r="A1" s="21" t="n">
         <v>1</v>
       </c>
-      <c r="B1" s="22" t="s">
-        <v>154</v>
-      </c>
-      <c r="C1" s="23" t="s">
-        <v>155</v>
+      <c r="B1" s="21" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="22" t="n">
+      <c r="A2" s="21" t="n">
         <v>2</v>
       </c>
-      <c r="B2" s="22" t="s">
-        <v>156</v>
-      </c>
-      <c r="C2" s="23" t="s">
-        <v>157</v>
+      <c r="B2" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="22" t="n">
+      <c r="A3" s="21" t="n">
         <v>3</v>
       </c>
-      <c r="B3" s="24" t="s">
-        <v>158</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>159</v>
+      <c r="B3" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="22" t="n">
+      <c r="A4" s="21" t="n">
         <v>4</v>
       </c>
-      <c r="B4" s="22" t="s">
-        <v>160</v>
-      </c>
-      <c r="C4" s="25" t="s">
-        <v>161</v>
+      <c r="B4" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="22" t="n">
+      <c r="A5" s="21" t="n">
         <v>5</v>
       </c>
-      <c r="B5" s="22" t="s">
-        <v>162</v>
-      </c>
-      <c r="C5" s="25" t="s">
-        <v>163</v>
+      <c r="B5" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="22" t="n">
+      <c r="A6" s="21" t="n">
         <v>6</v>
       </c>
-      <c r="B6" s="22" t="s">
-        <v>164</v>
-      </c>
-      <c r="C6" s="25" t="s">
-        <v>165</v>
+      <c r="B6" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="256.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="22" t="n">
+      <c r="A7" s="21" t="n">
         <v>7</v>
       </c>
-      <c r="B7" s="22" t="s">
-        <v>166</v>
-      </c>
-      <c r="C7" s="26" t="s">
-        <v>167</v>
+      <c r="B7" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="245.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="22" t="n">
+      <c r="A8" s="21" t="n">
         <v>8</v>
       </c>
-      <c r="B8" s="22" t="s">
-        <v>168</v>
-      </c>
-      <c r="C8" s="23" t="s">
-        <v>169</v>
+      <c r="B8" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="223.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="22" t="n">
+      <c r="A9" s="21" t="n">
         <v>9</v>
       </c>
-      <c r="B9" s="22" t="s">
-        <v>170</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>171</v>
+      <c r="B9" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="243.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="22" t="n">
+      <c r="A10" s="21" t="n">
         <v>10</v>
       </c>
-      <c r="B10" s="22" t="s">
-        <v>172</v>
-      </c>
-      <c r="C10" s="25" t="s">
-        <v>173</v>
-      </c>
-      <c r="D10" s="27" t="s">
-        <v>174</v>
+      <c r="B10" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>178</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="22" t="s">
-        <v>175</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>176</v>
+      <c r="B11" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="22" t="s">
-        <v>177</v>
-      </c>
-      <c r="C12" s="25" t="s">
-        <v>178</v>
+      <c r="B12" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="22" t="s">
-        <v>179</v>
-      </c>
-      <c r="C13" s="25" t="s">
-        <v>180</v>
+      <c r="B13" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="288.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="22" t="s">
-        <v>181</v>
-      </c>
-      <c r="C14" s="25" t="s">
-        <v>182</v>
-      </c>
-      <c r="D14" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="E14" s="25" t="s">
-        <v>184</v>
-      </c>
-      <c r="F14" s="25" t="s">
-        <v>185</v>
-      </c>
-      <c r="G14" s="25" t="s">
+      <c r="B14" s="21" t="s">
         <v>186</v>
       </c>
+      <c r="C14" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>188</v>
+      </c>
+      <c r="E14" s="24" t="s">
+        <v>189</v>
+      </c>
+      <c r="F14" s="24" t="s">
+        <v>190</v>
+      </c>
+      <c r="G14" s="24" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="22" t="s">
-        <v>187</v>
-      </c>
-      <c r="C15" s="25" t="s">
-        <v>188</v>
+      <c r="B15" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="C15" s="24" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="240.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="22" t="s">
-        <v>189</v>
+      <c r="B16" s="21" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="22" t="s">
-        <v>190</v>
-      </c>
-      <c r="C17" s="23" t="s">
-        <v>191</v>
+      <c r="B17" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="22" t="s">
-        <v>192</v>
-      </c>
-      <c r="C18" s="23" t="s">
-        <v>193</v>
+      <c r="B18" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -9562,278 +9899,278 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="28" width="72.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="29" width="139.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="27" width="72.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="28" width="139.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="30" t="s">
-        <v>194</v>
-      </c>
-      <c r="B1" s="30"/>
+      <c r="A1" s="29" t="s">
+        <v>199</v>
+      </c>
+      <c r="B1" s="29"/>
     </row>
     <row r="2" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="28" t="s">
-        <v>195</v>
-      </c>
-      <c r="B2" s="31" t="s">
-        <v>196</v>
+      <c r="A2" s="27" t="s">
+        <v>200</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="28" t="s">
-        <v>197</v>
-      </c>
-      <c r="B3" s="32" t="s">
-        <v>198</v>
+      <c r="A3" s="27" t="s">
+        <v>202</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="28" t="s">
-        <v>199</v>
-      </c>
-      <c r="B4" s="32" t="s">
-        <v>200</v>
+      <c r="A4" s="27" t="s">
+        <v>204</v>
+      </c>
+      <c r="B4" s="31" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="28" t="s">
-        <v>201</v>
-      </c>
-      <c r="B5" s="32" t="s">
-        <v>202</v>
+      <c r="A5" s="27" t="s">
+        <v>206</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="33" t="s">
-        <v>203</v>
-      </c>
-      <c r="B8" s="33"/>
+      <c r="A8" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="B8" s="32"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="34" t="s">
-        <v>204</v>
-      </c>
-      <c r="B9" s="35" t="s">
-        <v>205</v>
+      <c r="A9" s="33" t="s">
+        <v>209</v>
+      </c>
+      <c r="B9" s="34" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="36" t="s">
-        <v>206</v>
-      </c>
-      <c r="B10" s="35" t="s">
-        <v>207</v>
+      <c r="A10" s="35" t="s">
+        <v>211</v>
+      </c>
+      <c r="B10" s="34" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="36" t="s">
-        <v>208</v>
-      </c>
-      <c r="B11" s="37" t="s">
-        <v>209</v>
+      <c r="A11" s="35" t="s">
+        <v>213</v>
+      </c>
+      <c r="B11" s="36" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="35" t="s">
-        <v>210</v>
-      </c>
-      <c r="B12" s="35" t="s">
-        <v>211</v>
+      <c r="A12" s="34" t="s">
+        <v>215</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="35" t="s">
-        <v>212</v>
-      </c>
-      <c r="B13" s="35" t="s">
-        <v>213</v>
+      <c r="A13" s="34" t="s">
+        <v>217</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="35" t="s">
-        <v>214</v>
-      </c>
-      <c r="B14" s="35" t="s">
-        <v>215</v>
+      <c r="A14" s="34" t="s">
+        <v>219</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="35" t="s">
-        <v>216</v>
-      </c>
-      <c r="B15" s="35" t="s">
-        <v>217</v>
+      <c r="A15" s="34" t="s">
+        <v>221</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="35" t="s">
-        <v>218</v>
-      </c>
-      <c r="B16" s="35" t="s">
-        <v>219</v>
+      <c r="A16" s="34" t="s">
+        <v>223</v>
+      </c>
+      <c r="B16" s="34" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="35" t="s">
-        <v>220</v>
-      </c>
-      <c r="B17" s="35" t="s">
-        <v>221</v>
+      <c r="A17" s="34" t="s">
+        <v>225</v>
+      </c>
+      <c r="B17" s="34" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="35" t="s">
-        <v>222</v>
-      </c>
-      <c r="B18" s="35" t="s">
-        <v>223</v>
+      <c r="A18" s="34" t="s">
+        <v>227</v>
+      </c>
+      <c r="B18" s="34" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="35" t="s">
-        <v>224</v>
-      </c>
-      <c r="B19" s="35" t="s">
-        <v>225</v>
+      <c r="A19" s="34" t="s">
+        <v>229</v>
+      </c>
+      <c r="B19" s="34" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="35" t="s">
-        <v>226</v>
-      </c>
-      <c r="B20" s="35" t="s">
-        <v>227</v>
+      <c r="A20" s="34" t="s">
+        <v>231</v>
+      </c>
+      <c r="B20" s="34" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="35" t="s">
-        <v>228</v>
-      </c>
-      <c r="B21" s="35" t="s">
-        <v>229</v>
+      <c r="A21" s="34" t="s">
+        <v>233</v>
+      </c>
+      <c r="B21" s="34" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="30" t="s">
-        <v>230</v>
-      </c>
-      <c r="B25" s="30"/>
+      <c r="A25" s="29" t="s">
+        <v>235</v>
+      </c>
+      <c r="B25" s="29"/>
     </row>
     <row r="26" customFormat="false" ht="283.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="28" t="s">
-        <v>231</v>
-      </c>
-      <c r="B26" s="31" t="s">
-        <v>232</v>
+      <c r="A26" s="27" t="s">
+        <v>236</v>
+      </c>
+      <c r="B26" s="30" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="28" t="s">
-        <v>233</v>
-      </c>
-      <c r="B27" s="31" t="s">
-        <v>234</v>
+      <c r="A27" s="27" t="s">
+        <v>238</v>
+      </c>
+      <c r="B27" s="30" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="38" t="s">
-        <v>235</v>
-      </c>
-      <c r="B28" s="31" t="s">
-        <v>236</v>
+      <c r="A28" s="37" t="s">
+        <v>240</v>
+      </c>
+      <c r="B28" s="30" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="28" t="s">
-        <v>237</v>
-      </c>
-      <c r="B29" s="31" t="s">
-        <v>238</v>
+      <c r="A29" s="27" t="s">
+        <v>242</v>
+      </c>
+      <c r="B29" s="30" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="28" t="s">
-        <v>239</v>
-      </c>
-      <c r="B30" s="31" t="s">
-        <v>240</v>
+      <c r="A30" s="27" t="s">
+        <v>244</v>
+      </c>
+      <c r="B30" s="30" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="28" t="s">
-        <v>241</v>
-      </c>
-      <c r="B31" s="31" t="s">
-        <v>242</v>
+      <c r="A31" s="27" t="s">
+        <v>246</v>
+      </c>
+      <c r="B31" s="30" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="28" t="s">
-        <v>243</v>
-      </c>
-      <c r="B32" s="31" t="s">
-        <v>244</v>
+      <c r="A32" s="27" t="s">
+        <v>248</v>
+      </c>
+      <c r="B32" s="30" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="28" t="s">
-        <v>245</v>
-      </c>
-      <c r="B33" s="31" t="s">
-        <v>246</v>
+      <c r="A33" s="27" t="s">
+        <v>250</v>
+      </c>
+      <c r="B33" s="30" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="39" t="s">
-        <v>247</v>
-      </c>
-      <c r="B34" s="31" t="s">
-        <v>248</v>
+      <c r="A34" s="38" t="s">
+        <v>252</v>
+      </c>
+      <c r="B34" s="30" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="39"/>
-      <c r="B35" s="31" t="s">
-        <v>249</v>
+      <c r="A35" s="38"/>
+      <c r="B35" s="30" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="39"/>
-      <c r="B36" s="31" t="s">
-        <v>250</v>
+      <c r="A36" s="38"/>
+      <c r="B36" s="30" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="39"/>
-      <c r="B37" s="31" t="s">
-        <v>251</v>
+      <c r="A37" s="38"/>
+      <c r="B37" s="30" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="39"/>
-      <c r="B38" s="31" t="s">
-        <v>252</v>
+      <c r="A38" s="38"/>
+      <c r="B38" s="30" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="39"/>
-      <c r="B39" s="32" t="s">
-        <v>253</v>
+      <c r="A39" s="38"/>
+      <c r="B39" s="31" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="39"/>
-      <c r="B40" s="31" t="s">
-        <v>254</v>
+      <c r="A40" s="38"/>
+      <c r="B40" s="30" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="28" t="s">
-        <v>255</v>
-      </c>
-      <c r="B41" s="32" t="s">
-        <v>256</v>
+      <c r="A41" s="27" t="s">
+        <v>260</v>
+      </c>
+      <c r="B41" s="31" t="s">
+        <v>261</v>
       </c>
     </row>
   </sheetData>
@@ -9889,24 +10226,24 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="22" width="37.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="22" width="77.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="21" width="37.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="21" width="77.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
-        <v>257</v>
-      </c>
-      <c r="B1" s="25" t="s">
-        <v>258</v>
+      <c r="A1" s="24" t="s">
+        <v>262</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="22" t="s">
-        <v>259</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>260</v>
+      <c r="A2" s="21" t="s">
+        <v>264</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -9933,32 +10270,32 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="29" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="29" width="60.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="28" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="28" width="60.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="29" t="s">
-        <v>261</v>
+      <c r="A2" s="28" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="29" t="s">
-        <v>262</v>
+      <c r="A4" s="28" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="29" t="s">
-        <v>263</v>
+      <c r="A6" s="28" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="29" t="s">
-        <v>264</v>
+      <c r="A8" s="28" t="s">
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -9985,241 +10322,241 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="29" width="28.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="29" width="49.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="29" width="69.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="28" width="28.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="28" width="49.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="28" width="69.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="40" t="s">
-        <v>265</v>
-      </c>
-      <c r="B1" s="41" t="s">
-        <v>266</v>
+      <c r="A1" s="39" t="s">
+        <v>270</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="42"/>
+      <c r="A2" s="41"/>
     </row>
     <row r="3" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="43" t="s">
-        <v>267</v>
-      </c>
-      <c r="B3" s="44" t="s">
-        <v>268</v>
-      </c>
-      <c r="C3" s="31" t="s">
-        <v>269</v>
+      <c r="A3" s="42" t="s">
+        <v>272</v>
+      </c>
+      <c r="B3" s="43" t="s">
+        <v>273</v>
+      </c>
+      <c r="C3" s="30" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="43"/>
-      <c r="B4" s="44" t="s">
-        <v>270</v>
-      </c>
-      <c r="C4" s="31" t="s">
-        <v>271</v>
+      <c r="A4" s="42"/>
+      <c r="B4" s="43" t="s">
+        <v>275</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="43"/>
-      <c r="B5" s="29" t="s">
-        <v>272</v>
+      <c r="A5" s="42"/>
+      <c r="B5" s="28" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="43"/>
-      <c r="B6" s="29" t="s">
-        <v>273</v>
+      <c r="A6" s="42"/>
+      <c r="B6" s="28" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="43"/>
-      <c r="B7" s="29" t="s">
-        <v>274</v>
+      <c r="A7" s="42"/>
+      <c r="B7" s="28" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="43"/>
-      <c r="B8" s="45" t="s">
-        <v>275</v>
-      </c>
-      <c r="C8" s="31" t="s">
-        <v>276</v>
+      <c r="A8" s="42"/>
+      <c r="B8" s="44" t="s">
+        <v>280</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="43"/>
-      <c r="B9" s="45"/>
-      <c r="C9" s="31" t="s">
-        <v>277</v>
+      <c r="A9" s="42"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="30" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="43"/>
-      <c r="B10" s="45"/>
-      <c r="C10" s="31" t="s">
-        <v>278</v>
+      <c r="A10" s="42"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="30" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="43"/>
-      <c r="B11" s="45"/>
-      <c r="C11" s="29" t="s">
-        <v>279</v>
+      <c r="A11" s="42"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="28" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="43"/>
-      <c r="B12" s="45"/>
-      <c r="C12" s="31" t="s">
-        <v>280</v>
+      <c r="A12" s="42"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="30" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="43"/>
-      <c r="B13" s="29" t="s">
-        <v>281</v>
+      <c r="A13" s="42"/>
+      <c r="B13" s="28" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="216.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="43"/>
-      <c r="B14" s="46" t="s">
-        <v>282</v>
-      </c>
-      <c r="C14" s="31" t="s">
-        <v>283</v>
+      <c r="A14" s="42"/>
+      <c r="B14" s="45" t="s">
+        <v>287</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="43"/>
-      <c r="B15" s="46"/>
-      <c r="C15" s="47" t="s">
-        <v>284</v>
+      <c r="A15" s="42"/>
+      <c r="B15" s="45"/>
+      <c r="C15" s="46" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="43"/>
-      <c r="B16" s="46"/>
-      <c r="C16" s="47" t="s">
-        <v>285</v>
+      <c r="A16" s="42"/>
+      <c r="B16" s="45"/>
+      <c r="C16" s="46" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="43"/>
-      <c r="B17" s="46"/>
-      <c r="C17" s="47" t="s">
-        <v>286</v>
+      <c r="A17" s="42"/>
+      <c r="B17" s="45"/>
+      <c r="C17" s="46" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="43"/>
-      <c r="B18" s="46"/>
-      <c r="C18" s="31" t="s">
-        <v>287</v>
+      <c r="A18" s="42"/>
+      <c r="B18" s="45"/>
+      <c r="C18" s="30" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="43"/>
+      <c r="A19" s="42"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="43"/>
-      <c r="B20" s="48" t="s">
-        <v>288</v>
+      <c r="A20" s="42"/>
+      <c r="B20" s="47" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="43"/>
-      <c r="B21" s="29" t="s">
-        <v>289</v>
+      <c r="A21" s="42"/>
+      <c r="B21" s="28" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="42"/>
+      <c r="A22" s="41"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="42"/>
+      <c r="A23" s="41"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="43" t="s">
-        <v>290</v>
-      </c>
-      <c r="B24" s="29" t="s">
-        <v>291</v>
+      <c r="A24" s="42" t="s">
+        <v>295</v>
+      </c>
+      <c r="B24" s="28" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="43"/>
-      <c r="B25" s="29" t="s">
-        <v>292</v>
+      <c r="A25" s="42"/>
+      <c r="B25" s="28" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="43"/>
-      <c r="B26" s="29" t="s">
-        <v>293</v>
+      <c r="A26" s="42"/>
+      <c r="B26" s="28" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="43"/>
-      <c r="B27" s="29" t="s">
-        <v>294</v>
+      <c r="A27" s="42"/>
+      <c r="B27" s="28" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="43"/>
-      <c r="B28" s="31" t="s">
-        <v>295</v>
+      <c r="A28" s="42"/>
+      <c r="B28" s="30" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="43"/>
-      <c r="B29" s="31" t="s">
-        <v>296</v>
+      <c r="A29" s="42"/>
+      <c r="B29" s="30" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="49"/>
+      <c r="A30" s="48"/>
     </row>
     <row r="31" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="43" t="s">
-        <v>297</v>
-      </c>
-      <c r="B31" s="31" t="s">
-        <v>298</v>
-      </c>
-      <c r="F31" s="50"/>
+      <c r="A31" s="42" t="s">
+        <v>302</v>
+      </c>
+      <c r="B31" s="30" t="s">
+        <v>303</v>
+      </c>
+      <c r="F31" s="49"/>
     </row>
     <row r="32" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="43"/>
-      <c r="B32" s="31" t="s">
-        <v>299</v>
+      <c r="A32" s="42"/>
+      <c r="B32" s="30" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="43"/>
-      <c r="B33" s="31" t="s">
-        <v>300</v>
+      <c r="A33" s="42"/>
+      <c r="B33" s="30" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="43"/>
-      <c r="B34" s="31" t="s">
-        <v>301</v>
+      <c r="A34" s="42"/>
+      <c r="B34" s="30" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="43"/>
-      <c r="B35" s="31" t="s">
-        <v>302</v>
+      <c r="A35" s="42"/>
+      <c r="B35" s="30" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="43"/>
-      <c r="B36" s="31" t="s">
-        <v>303</v>
-      </c>
-      <c r="C36" s="31"/>
+      <c r="A36" s="42"/>
+      <c r="B36" s="30" t="s">
+        <v>308</v>
+      </c>
+      <c r="C36" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
[feat][OS][OS: CPU Scheduling + Switch Context]
</commit_message>
<xml_diff>
--- a/Operations-System/DevOps-Documents.xlsx
+++ b/Operations-System/DevOps-Documents.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="330">
   <si>
     <t xml:space="preserve">Operating System Concepts</t>
   </si>
@@ -5146,43 +5146,15 @@
     <t xml:space="preserve">Process Scheduling</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="15"/>
-        <color theme="1"/>
-        <rFont val="Linux Libertine O"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> - Multiple programming: Several processes (each an independent instance of a program) are loaded into memory and can be scheduled by the operating system.
+    <t xml:space="preserve"> - Multiple programming: Several processes (each an independent instance of a program) are loaded into memory and can be scheduled by the operating system.
  - Multiple thread: A thread is a lightweight unit of execution within a process. A process can have one or more threads, which share the same virtual address space and resources like heap and global variables.
  - Process scheduler: Selects an available process (possibly from a set of several available processes) for program execution on a core.
  - CPU core:
   + A system single CPU core will never perform more than one process running at a time.
   + A multicore system can run multiple processes at one time.
- - If more </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15"/>
-        <color theme="1"/>
-        <rFont val="Linux Libertine O"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">processes</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15"/>
-        <color theme="1"/>
-        <rFont val="Linux Libertine O"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> than cores, processes wait until a core is free and can be rescheduled.
+ - If more processes than cores, processes wait until a core is free and can be rescheduled.
  - An I/O-bound process: spends more of its time doing I/O than it spends doing computations.
  - A CPU-bound process, in contrast, generates I/O requests infrequently, using more of its time doing computations.</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">Scheduling queues</t>
@@ -5338,7 +5310,174 @@
     <t xml:space="preserve">CPU Scheduling</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> - CPU scheduler is to </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">select</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> from among the processes that are in the ready queue and </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">allocate a CPU core</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> to one of them.
+ - CPU scheduler triggered </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">periodically</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (timer interrupt every 100 ms) wakes up to </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">evaluate state of all processes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> in the system (waiting in ready queue, exhausted its allotted time slice,…).
+ →  Ensure no single process can monopolize(độc quyền) the CPU.
+       Enforce fairness among processes
+       Crucial for responsiveness(khả năng đáp ứng) in a multitasking environment.
+ - </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Swapping</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> is intermediate form of scheduling:
+  + Swap out: Remove a process from memory (from contention for the CPU) to disk and store status, reduce degree of multiprogramming.
+  + Swap in: Reintroduced process into memory.</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">Context switch</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - A system call or interrupt occurs → the OS saves the state of the currently running process (its CPU registers, program counter, and other essential data) into its PCB → Then the OS selects a new process from the ready queue, loads its saved state from its PCB into the CPU registers →  Resumes execution of that process.
+ - Context-switch times are highly dependent on hardware support.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operations on Processes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Process Creation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Process Termination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interprocess Communication</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPC in Shared-Memory Systems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPC in Message-Passing Systems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Naming</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Synchronization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buffering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Examples of IPC Systems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Communication in Client-Server Systems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sockets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remote Procedure Calls</t>
   </si>
   <si>
     <t xml:space="preserve">Threads &amp; Concurrency</t>
@@ -7688,8 +7827,8 @@
     <font>
       <sz val="15"/>
       <color theme="1"/>
-      <name val="Linux Libertine O"/>
-      <family val="0"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -7855,7 +7994,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -7938,6 +8077,10 @@
     </xf>
     <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -8142,9 +8285,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>581400</xdr:colOff>
+      <xdr:colOff>581040</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>2114280</xdr:rowOff>
+      <xdr:rowOff>2113920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8158,7 +8301,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10237320" y="8324640"/>
-          <a:ext cx="4794120" cy="2791440"/>
+          <a:ext cx="4793760" cy="2791080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8179,9 +8322,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>657720</xdr:colOff>
+      <xdr:colOff>657360</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>1790280</xdr:rowOff>
+      <xdr:rowOff>1789920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8195,7 +8338,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10323000" y="11420280"/>
-          <a:ext cx="4784760" cy="2486520"/>
+          <a:ext cx="4784400" cy="2486160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8216,9 +8359,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>514800</xdr:colOff>
+      <xdr:colOff>514440</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>689040</xdr:rowOff>
+      <xdr:rowOff>688680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8232,7 +8375,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10170720" y="24355440"/>
-          <a:ext cx="4794120" cy="2896200"/>
+          <a:ext cx="4793760" cy="2895840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8424,10 +8567,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G1048576"/>
+  <dimension ref="A1:G99"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D74" colorId="64" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F76" activeCellId="0" sqref="F76"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E78" colorId="64" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F84" activeCellId="0" sqref="F84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="36.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9419,9 +9562,11 @@
       <c r="D75" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="E75" s="5" t="s">
+      <c r="E75" s="11" t="s">
         <v>153</v>
       </c>
+      <c r="F75" s="11"/>
+      <c r="G75" s="11"/>
     </row>
     <row r="76" customFormat="false" ht="211.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="7"/>
@@ -9431,11 +9576,12 @@
       <c r="E76" s="14" t="s">
         <v>154</v>
       </c>
-      <c r="F76" s="5" t="s">
+      <c r="F76" s="11" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="77" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G76" s="11"/>
+    </row>
+    <row r="77" customFormat="false" ht="138.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="7"/>
       <c r="B77" s="8"/>
       <c r="C77" s="9"/>
@@ -9443,55 +9589,193 @@
       <c r="E77" s="14" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="78" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F77" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="50.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="7"/>
       <c r="B78" s="8"/>
       <c r="C78" s="9"/>
       <c r="D78" s="10"/>
       <c r="E78" s="14" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="70.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>158</v>
+      </c>
+      <c r="F78" s="21" t="s">
+        <v>159</v>
+      </c>
+      <c r="G78" s="21"/>
+    </row>
+    <row r="79" customFormat="false" ht="36.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="7"/>
       <c r="B79" s="8"/>
-      <c r="C79" s="3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="47.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C79" s="9"/>
+      <c r="D79" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="E79" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="F79" s="21"/>
+      <c r="G79" s="21"/>
+    </row>
+    <row r="80" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="7"/>
       <c r="B80" s="8"/>
-      <c r="C80" s="3" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C80" s="9"/>
+      <c r="D80" s="10"/>
+      <c r="E80" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="F80" s="21"/>
+      <c r="G80" s="21"/>
+    </row>
+    <row r="81" customFormat="false" ht="61.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="7"/>
-    </row>
-    <row r="82" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B81" s="8"/>
+      <c r="C81" s="9"/>
+      <c r="D81" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="E81" s="14"/>
+      <c r="F81" s="14"/>
+      <c r="G81" s="14"/>
+    </row>
+    <row r="82" customFormat="false" ht="61.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="7"/>
-    </row>
-    <row r="83" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B82" s="8"/>
+      <c r="C82" s="9"/>
+      <c r="D82" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="E82" s="14"/>
+      <c r="F82" s="14"/>
+      <c r="G82" s="14"/>
+    </row>
+    <row r="83" customFormat="false" ht="36.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="7"/>
+      <c r="B83" s="8"/>
+      <c r="C83" s="9"/>
+      <c r="D83" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="E83" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="F83" s="21"/>
+      <c r="G83" s="21"/>
     </row>
     <row r="84" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="7"/>
+      <c r="B84" s="8"/>
+      <c r="C84" s="9"/>
+      <c r="D84" s="10"/>
+      <c r="E84" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="F84" s="21"/>
+      <c r="G84" s="21"/>
     </row>
     <row r="85" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="7"/>
-    </row>
-    <row r="86" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B85" s="8"/>
+      <c r="C85" s="9"/>
+      <c r="D85" s="10"/>
+      <c r="E85" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="F85" s="21"/>
+      <c r="G85" s="21"/>
+    </row>
+    <row r="86" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="7"/>
-    </row>
-    <row r="87" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B86" s="8"/>
+      <c r="C86" s="9"/>
+      <c r="D86" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="E86" s="14"/>
+      <c r="F86" s="14"/>
+      <c r="G86" s="14"/>
+    </row>
+    <row r="87" customFormat="false" ht="36.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="7"/>
-    </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="B87" s="8"/>
+      <c r="C87" s="9"/>
+      <c r="D87" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="E87" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="F87" s="21"/>
+      <c r="G87" s="21"/>
+    </row>
+    <row r="88" customFormat="false" ht="52.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="7"/>
+      <c r="B88" s="8"/>
+      <c r="C88" s="9"/>
+      <c r="D88" s="10"/>
+      <c r="E88" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="F88" s="21"/>
+      <c r="G88" s="21"/>
+    </row>
+    <row r="89" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="7"/>
+      <c r="B89" s="8"/>
+      <c r="C89" s="9"/>
+      <c r="D89" s="10"/>
+      <c r="E89" s="14"/>
+      <c r="F89" s="21"/>
+    </row>
+    <row r="90" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="7"/>
+      <c r="B90" s="8"/>
+      <c r="C90" s="9"/>
+      <c r="D90" s="10"/>
+      <c r="E90" s="14"/>
+      <c r="F90" s="21"/>
+    </row>
+    <row r="91" customFormat="false" ht="70.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="7"/>
+      <c r="B91" s="8"/>
+      <c r="C91" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="47.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="7"/>
+      <c r="B92" s="8"/>
+      <c r="C92" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="7"/>
+    </row>
+    <row r="94" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="7"/>
+    </row>
+    <row r="95" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="7"/>
+    </row>
+    <row r="96" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="7"/>
+    </row>
+    <row r="97" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="7"/>
+    </row>
+    <row r="98" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="7"/>
+    </row>
+    <row r="99" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="7"/>
+    </row>
   </sheetData>
-  <mergeCells count="84">
-    <mergeCell ref="A1:A87"/>
+  <mergeCells count="99">
+    <mergeCell ref="A1:A99"/>
     <mergeCell ref="B1:B69"/>
     <mergeCell ref="C1:C41"/>
     <mergeCell ref="D1:D4"/>
@@ -9566,8 +9850,8 @@
     <mergeCell ref="F69:G69"/>
     <mergeCell ref="D70:D74"/>
     <mergeCell ref="E70:G70"/>
-    <mergeCell ref="B71:B80"/>
-    <mergeCell ref="C71:C78"/>
+    <mergeCell ref="B71:B92"/>
+    <mergeCell ref="C71:C88"/>
     <mergeCell ref="F71:G71"/>
     <mergeCell ref="F72:G72"/>
     <mergeCell ref="F73:G73"/>
@@ -9575,6 +9859,21 @@
     <mergeCell ref="D75:D78"/>
     <mergeCell ref="E75:G75"/>
     <mergeCell ref="F76:G76"/>
+    <mergeCell ref="F77:G77"/>
+    <mergeCell ref="F78:G78"/>
+    <mergeCell ref="D79:D80"/>
+    <mergeCell ref="F79:G79"/>
+    <mergeCell ref="F80:G80"/>
+    <mergeCell ref="E81:G81"/>
+    <mergeCell ref="E82:G82"/>
+    <mergeCell ref="D83:D85"/>
+    <mergeCell ref="F83:G83"/>
+    <mergeCell ref="F84:G84"/>
+    <mergeCell ref="F85:G85"/>
+    <mergeCell ref="E86:G86"/>
+    <mergeCell ref="D87:D88"/>
+    <mergeCell ref="F87:G87"/>
+    <mergeCell ref="F88:G88"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
@@ -9599,33 +9898,33 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="21" width="23.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="21" width="57.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="3" style="21" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="22" width="23.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="22" width="57.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="3" style="22" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="21" t="s">
-        <v>309</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>310</v>
+      <c r="A1" s="22" t="s">
+        <v>324</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="24" t="s">
-        <v>311</v>
-      </c>
-      <c r="B2" s="24" t="s">
-        <v>312</v>
+      <c r="A2" s="25" t="s">
+        <v>326</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="24" t="s">
-        <v>313</v>
-      </c>
-      <c r="B3" s="24" t="s">
-        <v>314</v>
+      <c r="A3" s="25" t="s">
+        <v>328</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>329</v>
       </c>
     </row>
   </sheetData>
@@ -9675,200 +9974,200 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="21" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="21" width="39.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="21" width="95.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="21" width="60.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="21" width="58.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="21" width="50"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="21" width="49.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="8" style="21" width="9.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="22" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="22" width="39.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="22" width="95.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="22" width="60.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="22" width="58.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="22" width="50"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="22" width="49.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="8" style="22" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="21" t="n">
+      <c r="A1" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="B1" s="21" t="s">
-        <v>159</v>
-      </c>
-      <c r="C1" s="22" t="s">
-        <v>160</v>
+      <c r="B1" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="21" t="n">
+      <c r="A2" s="22" t="n">
         <v>2</v>
       </c>
-      <c r="B2" s="21" t="s">
-        <v>161</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>162</v>
+      <c r="B2" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="21" t="n">
+      <c r="A3" s="22" t="n">
         <v>3</v>
       </c>
-      <c r="B3" s="23" t="s">
-        <v>163</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>164</v>
+      <c r="B3" s="24" t="s">
+        <v>178</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="21" t="n">
+      <c r="A4" s="22" t="n">
         <v>4</v>
       </c>
-      <c r="B4" s="21" t="s">
-        <v>165</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>166</v>
+      <c r="B4" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="21" t="n">
+      <c r="A5" s="22" t="n">
         <v>5</v>
       </c>
-      <c r="B5" s="21" t="s">
-        <v>167</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>168</v>
+      <c r="B5" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="21" t="n">
+      <c r="A6" s="22" t="n">
         <v>6</v>
       </c>
-      <c r="B6" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>170</v>
+      <c r="B6" s="22" t="s">
+        <v>184</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="256.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="21" t="n">
+      <c r="A7" s="22" t="n">
         <v>7</v>
       </c>
-      <c r="B7" s="21" t="s">
-        <v>171</v>
-      </c>
-      <c r="C7" s="25" t="s">
-        <v>172</v>
+      <c r="B7" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="245.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="21" t="n">
+      <c r="A8" s="22" t="n">
         <v>8</v>
       </c>
-      <c r="B8" s="21" t="s">
-        <v>173</v>
-      </c>
-      <c r="C8" s="22" t="s">
-        <v>174</v>
+      <c r="B8" s="22" t="s">
+        <v>188</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="223.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="21" t="n">
+      <c r="A9" s="22" t="n">
         <v>9</v>
       </c>
-      <c r="B9" s="21" t="s">
-        <v>175</v>
-      </c>
-      <c r="C9" s="22" t="s">
-        <v>176</v>
+      <c r="B9" s="22" t="s">
+        <v>190</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="243.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="21" t="n">
+      <c r="A10" s="22" t="n">
         <v>10</v>
       </c>
-      <c r="B10" s="21" t="s">
-        <v>177</v>
-      </c>
-      <c r="C10" s="24" t="s">
-        <v>178</v>
-      </c>
-      <c r="D10" s="26" t="s">
-        <v>179</v>
+      <c r="B10" s="22" t="s">
+        <v>192</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>193</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="21" t="s">
-        <v>180</v>
-      </c>
-      <c r="C11" s="24" t="s">
-        <v>181</v>
+      <c r="B11" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="21" t="s">
-        <v>182</v>
-      </c>
-      <c r="C12" s="24" t="s">
-        <v>183</v>
+      <c r="B12" s="22" t="s">
+        <v>197</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="21" t="s">
-        <v>184</v>
-      </c>
-      <c r="C13" s="24" t="s">
-        <v>185</v>
+      <c r="B13" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="288.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="21" t="s">
-        <v>186</v>
-      </c>
-      <c r="C14" s="24" t="s">
-        <v>187</v>
-      </c>
-      <c r="D14" s="22" t="s">
-        <v>188</v>
-      </c>
-      <c r="E14" s="24" t="s">
-        <v>189</v>
-      </c>
-      <c r="F14" s="24" t="s">
-        <v>190</v>
-      </c>
-      <c r="G14" s="24" t="s">
-        <v>191</v>
+      <c r="B14" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>202</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>203</v>
+      </c>
+      <c r="E14" s="25" t="s">
+        <v>204</v>
+      </c>
+      <c r="F14" s="25" t="s">
+        <v>205</v>
+      </c>
+      <c r="G14" s="25" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="21" t="s">
-        <v>192</v>
-      </c>
-      <c r="C15" s="24" t="s">
-        <v>193</v>
+      <c r="B15" s="22" t="s">
+        <v>207</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="240.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="21" t="s">
-        <v>194</v>
+      <c r="B16" s="22" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="21" t="s">
-        <v>195</v>
-      </c>
-      <c r="C17" s="22" t="s">
-        <v>196</v>
+      <c r="B17" s="22" t="s">
+        <v>210</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="21" t="s">
-        <v>197</v>
-      </c>
-      <c r="C18" s="22" t="s">
-        <v>198</v>
+      <c r="B18" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -9899,278 +10198,278 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="27" width="72.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="28" width="139.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="28" width="72.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="29" width="139.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="29" t="s">
-        <v>199</v>
-      </c>
-      <c r="B1" s="29"/>
+      <c r="A1" s="30" t="s">
+        <v>214</v>
+      </c>
+      <c r="B1" s="30"/>
     </row>
     <row r="2" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="27" t="s">
-        <v>200</v>
-      </c>
-      <c r="B2" s="30" t="s">
-        <v>201</v>
+      <c r="A2" s="28" t="s">
+        <v>215</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="27" t="s">
-        <v>202</v>
-      </c>
-      <c r="B3" s="31" t="s">
-        <v>203</v>
+      <c r="A3" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="27" t="s">
-        <v>204</v>
-      </c>
-      <c r="B4" s="31" t="s">
-        <v>205</v>
+      <c r="A4" s="28" t="s">
+        <v>219</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="27" t="s">
-        <v>206</v>
-      </c>
-      <c r="B5" s="31" t="s">
-        <v>207</v>
+      <c r="A5" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="32" t="s">
-        <v>208</v>
-      </c>
-      <c r="B8" s="32"/>
+      <c r="A8" s="33" t="s">
+        <v>223</v>
+      </c>
+      <c r="B8" s="33"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="33" t="s">
-        <v>209</v>
-      </c>
-      <c r="B9" s="34" t="s">
-        <v>210</v>
+      <c r="A9" s="34" t="s">
+        <v>224</v>
+      </c>
+      <c r="B9" s="35" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="35" t="s">
-        <v>211</v>
-      </c>
-      <c r="B10" s="34" t="s">
-        <v>212</v>
+      <c r="A10" s="36" t="s">
+        <v>226</v>
+      </c>
+      <c r="B10" s="35" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="35" t="s">
-        <v>213</v>
-      </c>
-      <c r="B11" s="36" t="s">
-        <v>214</v>
+      <c r="A11" s="36" t="s">
+        <v>228</v>
+      </c>
+      <c r="B11" s="37" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="34" t="s">
-        <v>215</v>
-      </c>
-      <c r="B12" s="34" t="s">
-        <v>216</v>
+      <c r="A12" s="35" t="s">
+        <v>230</v>
+      </c>
+      <c r="B12" s="35" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="34" t="s">
-        <v>217</v>
-      </c>
-      <c r="B13" s="34" t="s">
-        <v>218</v>
+      <c r="A13" s="35" t="s">
+        <v>232</v>
+      </c>
+      <c r="B13" s="35" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="34" t="s">
-        <v>219</v>
-      </c>
-      <c r="B14" s="34" t="s">
-        <v>220</v>
+      <c r="A14" s="35" t="s">
+        <v>234</v>
+      </c>
+      <c r="B14" s="35" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="34" t="s">
-        <v>221</v>
-      </c>
-      <c r="B15" s="34" t="s">
-        <v>222</v>
+      <c r="A15" s="35" t="s">
+        <v>236</v>
+      </c>
+      <c r="B15" s="35" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="34" t="s">
-        <v>223</v>
-      </c>
-      <c r="B16" s="34" t="s">
-        <v>224</v>
+      <c r="A16" s="35" t="s">
+        <v>238</v>
+      </c>
+      <c r="B16" s="35" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="34" t="s">
-        <v>225</v>
-      </c>
-      <c r="B17" s="34" t="s">
-        <v>226</v>
+      <c r="A17" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="B17" s="35" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="34" t="s">
-        <v>227</v>
-      </c>
-      <c r="B18" s="34" t="s">
-        <v>228</v>
+      <c r="A18" s="35" t="s">
+        <v>242</v>
+      </c>
+      <c r="B18" s="35" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="34" t="s">
-        <v>229</v>
-      </c>
-      <c r="B19" s="34" t="s">
-        <v>230</v>
+      <c r="A19" s="35" t="s">
+        <v>244</v>
+      </c>
+      <c r="B19" s="35" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="34" t="s">
-        <v>231</v>
-      </c>
-      <c r="B20" s="34" t="s">
-        <v>232</v>
+      <c r="A20" s="35" t="s">
+        <v>246</v>
+      </c>
+      <c r="B20" s="35" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="34" t="s">
-        <v>233</v>
-      </c>
-      <c r="B21" s="34" t="s">
-        <v>234</v>
+      <c r="A21" s="35" t="s">
+        <v>248</v>
+      </c>
+      <c r="B21" s="35" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="29" t="s">
-        <v>235</v>
-      </c>
-      <c r="B25" s="29"/>
+      <c r="A25" s="30" t="s">
+        <v>250</v>
+      </c>
+      <c r="B25" s="30"/>
     </row>
     <row r="26" customFormat="false" ht="283.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="27" t="s">
-        <v>236</v>
-      </c>
-      <c r="B26" s="30" t="s">
-        <v>237</v>
+      <c r="A26" s="28" t="s">
+        <v>251</v>
+      </c>
+      <c r="B26" s="31" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="27" t="s">
-        <v>238</v>
-      </c>
-      <c r="B27" s="30" t="s">
-        <v>239</v>
+      <c r="A27" s="28" t="s">
+        <v>253</v>
+      </c>
+      <c r="B27" s="31" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="37" t="s">
-        <v>240</v>
-      </c>
-      <c r="B28" s="30" t="s">
-        <v>241</v>
+      <c r="A28" s="38" t="s">
+        <v>255</v>
+      </c>
+      <c r="B28" s="31" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="27" t="s">
-        <v>242</v>
-      </c>
-      <c r="B29" s="30" t="s">
-        <v>243</v>
+      <c r="A29" s="28" t="s">
+        <v>257</v>
+      </c>
+      <c r="B29" s="31" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="27" t="s">
-        <v>244</v>
-      </c>
-      <c r="B30" s="30" t="s">
-        <v>245</v>
+      <c r="A30" s="28" t="s">
+        <v>259</v>
+      </c>
+      <c r="B30" s="31" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="27" t="s">
-        <v>246</v>
-      </c>
-      <c r="B31" s="30" t="s">
-        <v>247</v>
+      <c r="A31" s="28" t="s">
+        <v>261</v>
+      </c>
+      <c r="B31" s="31" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="27" t="s">
-        <v>248</v>
-      </c>
-      <c r="B32" s="30" t="s">
-        <v>249</v>
+      <c r="A32" s="28" t="s">
+        <v>263</v>
+      </c>
+      <c r="B32" s="31" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="27" t="s">
-        <v>250</v>
-      </c>
-      <c r="B33" s="30" t="s">
-        <v>251</v>
+      <c r="A33" s="28" t="s">
+        <v>265</v>
+      </c>
+      <c r="B33" s="31" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="38" t="s">
-        <v>252</v>
-      </c>
-      <c r="B34" s="30" t="s">
-        <v>253</v>
+      <c r="A34" s="39" t="s">
+        <v>267</v>
+      </c>
+      <c r="B34" s="31" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="38"/>
-      <c r="B35" s="30" t="s">
-        <v>254</v>
+      <c r="A35" s="39"/>
+      <c r="B35" s="31" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="38"/>
-      <c r="B36" s="30" t="s">
-        <v>255</v>
+      <c r="A36" s="39"/>
+      <c r="B36" s="31" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="38"/>
-      <c r="B37" s="30" t="s">
-        <v>256</v>
+      <c r="A37" s="39"/>
+      <c r="B37" s="31" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="38"/>
-      <c r="B38" s="30" t="s">
-        <v>257</v>
+      <c r="A38" s="39"/>
+      <c r="B38" s="31" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="38"/>
-      <c r="B39" s="31" t="s">
-        <v>258</v>
+      <c r="A39" s="39"/>
+      <c r="B39" s="32" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="38"/>
-      <c r="B40" s="30" t="s">
-        <v>259</v>
+      <c r="A40" s="39"/>
+      <c r="B40" s="31" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="27" t="s">
-        <v>260</v>
-      </c>
-      <c r="B41" s="31" t="s">
-        <v>261</v>
+      <c r="A41" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="B41" s="32" t="s">
+        <v>276</v>
       </c>
     </row>
   </sheetData>
@@ -10226,24 +10525,24 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="21" width="37.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="21" width="77.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="22" width="37.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="22" width="77.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="24" t="s">
-        <v>262</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>263</v>
+      <c r="A1" s="25" t="s">
+        <v>277</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="21" t="s">
-        <v>264</v>
-      </c>
-      <c r="B2" s="24" t="s">
-        <v>265</v>
+      <c r="A2" s="22" t="s">
+        <v>279</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -10270,32 +10569,32 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="28" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="28" width="60.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="29" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="29" width="60.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="28" t="s">
-        <v>266</v>
+      <c r="A2" s="29" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="28" t="s">
-        <v>267</v>
+      <c r="A4" s="29" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="28" t="s">
-        <v>268</v>
+      <c r="A6" s="29" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="28" t="s">
-        <v>269</v>
+      <c r="A8" s="29" t="s">
+        <v>284</v>
       </c>
     </row>
   </sheetData>
@@ -10322,241 +10621,241 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="28" width="28.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="28" width="49.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="28" width="69.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="29" width="28.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="29" width="49.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="29" width="69.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="39" t="s">
-        <v>270</v>
-      </c>
-      <c r="B1" s="40" t="s">
-        <v>271</v>
+      <c r="A1" s="40" t="s">
+        <v>285</v>
+      </c>
+      <c r="B1" s="41" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="41"/>
+      <c r="A2" s="42"/>
     </row>
     <row r="3" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="42" t="s">
-        <v>272</v>
-      </c>
-      <c r="B3" s="43" t="s">
-        <v>273</v>
-      </c>
-      <c r="C3" s="30" t="s">
-        <v>274</v>
+      <c r="A3" s="43" t="s">
+        <v>287</v>
+      </c>
+      <c r="B3" s="44" t="s">
+        <v>288</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="42"/>
-      <c r="B4" s="43" t="s">
-        <v>275</v>
-      </c>
-      <c r="C4" s="30" t="s">
-        <v>276</v>
+      <c r="A4" s="43"/>
+      <c r="B4" s="44" t="s">
+        <v>290</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="42"/>
-      <c r="B5" s="28" t="s">
-        <v>277</v>
+      <c r="A5" s="43"/>
+      <c r="B5" s="29" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="42"/>
-      <c r="B6" s="28" t="s">
-        <v>278</v>
+      <c r="A6" s="43"/>
+      <c r="B6" s="29" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="42"/>
-      <c r="B7" s="28" t="s">
-        <v>279</v>
+      <c r="A7" s="43"/>
+      <c r="B7" s="29" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="42"/>
-      <c r="B8" s="44" t="s">
-        <v>280</v>
-      </c>
-      <c r="C8" s="30" t="s">
-        <v>281</v>
+      <c r="A8" s="43"/>
+      <c r="B8" s="45" t="s">
+        <v>295</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="42"/>
-      <c r="B9" s="44"/>
-      <c r="C9" s="30" t="s">
-        <v>282</v>
+      <c r="A9" s="43"/>
+      <c r="B9" s="45"/>
+      <c r="C9" s="31" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="42"/>
-      <c r="B10" s="44"/>
-      <c r="C10" s="30" t="s">
-        <v>283</v>
+      <c r="A10" s="43"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="31" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="42"/>
-      <c r="B11" s="44"/>
-      <c r="C11" s="28" t="s">
-        <v>284</v>
+      <c r="A11" s="43"/>
+      <c r="B11" s="45"/>
+      <c r="C11" s="29" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="42"/>
-      <c r="B12" s="44"/>
-      <c r="C12" s="30" t="s">
-        <v>285</v>
+      <c r="A12" s="43"/>
+      <c r="B12" s="45"/>
+      <c r="C12" s="31" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="42"/>
-      <c r="B13" s="28" t="s">
-        <v>286</v>
+      <c r="A13" s="43"/>
+      <c r="B13" s="29" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="216.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="42"/>
-      <c r="B14" s="45" t="s">
-        <v>287</v>
-      </c>
-      <c r="C14" s="30" t="s">
-        <v>288</v>
+      <c r="A14" s="43"/>
+      <c r="B14" s="46" t="s">
+        <v>302</v>
+      </c>
+      <c r="C14" s="31" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="42"/>
-      <c r="B15" s="45"/>
-      <c r="C15" s="46" t="s">
-        <v>289</v>
+      <c r="A15" s="43"/>
+      <c r="B15" s="46"/>
+      <c r="C15" s="47" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="42"/>
-      <c r="B16" s="45"/>
-      <c r="C16" s="46" t="s">
-        <v>290</v>
+      <c r="A16" s="43"/>
+      <c r="B16" s="46"/>
+      <c r="C16" s="47" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="42"/>
-      <c r="B17" s="45"/>
-      <c r="C17" s="46" t="s">
-        <v>291</v>
+      <c r="A17" s="43"/>
+      <c r="B17" s="46"/>
+      <c r="C17" s="47" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="42"/>
-      <c r="B18" s="45"/>
-      <c r="C18" s="30" t="s">
-        <v>292</v>
+      <c r="A18" s="43"/>
+      <c r="B18" s="46"/>
+      <c r="C18" s="31" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="42"/>
+      <c r="A19" s="43"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="42"/>
-      <c r="B20" s="47" t="s">
-        <v>293</v>
+      <c r="A20" s="43"/>
+      <c r="B20" s="48" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="42"/>
-      <c r="B21" s="28" t="s">
-        <v>294</v>
+      <c r="A21" s="43"/>
+      <c r="B21" s="29" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="41"/>
+      <c r="A22" s="42"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="41"/>
+      <c r="A23" s="42"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="42" t="s">
-        <v>295</v>
-      </c>
-      <c r="B24" s="28" t="s">
-        <v>296</v>
+      <c r="A24" s="43" t="s">
+        <v>310</v>
+      </c>
+      <c r="B24" s="29" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="42"/>
-      <c r="B25" s="28" t="s">
-        <v>297</v>
+      <c r="A25" s="43"/>
+      <c r="B25" s="29" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="42"/>
-      <c r="B26" s="28" t="s">
-        <v>298</v>
+      <c r="A26" s="43"/>
+      <c r="B26" s="29" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="42"/>
-      <c r="B27" s="28" t="s">
-        <v>299</v>
+      <c r="A27" s="43"/>
+      <c r="B27" s="29" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="42"/>
-      <c r="B28" s="30" t="s">
-        <v>300</v>
+      <c r="A28" s="43"/>
+      <c r="B28" s="31" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="42"/>
-      <c r="B29" s="30" t="s">
-        <v>301</v>
+      <c r="A29" s="43"/>
+      <c r="B29" s="31" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="48"/>
+      <c r="A30" s="49"/>
     </row>
     <row r="31" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="42" t="s">
-        <v>302</v>
-      </c>
-      <c r="B31" s="30" t="s">
-        <v>303</v>
-      </c>
-      <c r="F31" s="49"/>
+      <c r="A31" s="43" t="s">
+        <v>317</v>
+      </c>
+      <c r="B31" s="31" t="s">
+        <v>318</v>
+      </c>
+      <c r="F31" s="50"/>
     </row>
     <row r="32" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="42"/>
-      <c r="B32" s="30" t="s">
-        <v>304</v>
+      <c r="A32" s="43"/>
+      <c r="B32" s="31" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="42"/>
-      <c r="B33" s="30" t="s">
-        <v>305</v>
+      <c r="A33" s="43"/>
+      <c r="B33" s="31" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="42"/>
-      <c r="B34" s="30" t="s">
-        <v>306</v>
+      <c r="A34" s="43"/>
+      <c r="B34" s="31" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="42"/>
-      <c r="B35" s="30" t="s">
-        <v>307</v>
+      <c r="A35" s="43"/>
+      <c r="B35" s="31" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="42"/>
-      <c r="B36" s="30" t="s">
-        <v>308</v>
-      </c>
-      <c r="C36" s="30"/>
+      <c r="A36" s="43"/>
+      <c r="B36" s="31" t="s">
+        <v>323</v>
+      </c>
+      <c r="C36" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
[feat][OS][1. Process: Creation + Termination /n 2. Interprocess Communication: Shared memory + Messaging]
</commit_message>
<xml_diff>
--- a/Operations-System/DevOps-Documents.xlsx
+++ b/Operations-System/DevOps-Documents.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="336">
   <si>
     <t xml:space="preserve">Operating System Concepts</t>
   </si>
@@ -5447,19 +5447,600 @@
     <t xml:space="preserve">Process Creation</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> - A process (parent) may create several new processes (children). Each of these new processes may in turn create other processes, forming a </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">tree of processes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.
+ - Most operating systems identify processes according to a unique </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">process identifie</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (or </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">pid</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">).
+ - The systemd process (which always has a pid of 1) serves as the </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">root parent process</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> for all user processes, and is the first user process created when the system boots.
+ - A child process may be able to </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">obtain its resources</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> directly from </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">OS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, the </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">parent may have to partition</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> its resources among its children, or it may be able to </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">share some resources</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.
+ - When a child process created:
+  + The parent process continues to execute concurrently or waits until some or all of its children have terminated.
+  + The child process is a duplicate of the parent process or has a new program loaded into it.
+ - Create child process in Linux:
+  + F</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ork()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> system call used to create a new process by duplicating (resources, </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">program</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, address space,...) parent process. Fork() will </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">return zero for child process, non-zero(pid of child process) for parent process</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">. 
+  + Child process exec() to load new program from disk into memory and begin execution. If not exec(), child process execute program duplicated from parent. And finish with </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">exits()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> system call and clean up resources. 
+  + In synchronous environment, parent process temporarily blocked with wait() for child process finish and clean up resources.
+  + In asynchronous environment (concurency / parallel, context-switch, single-core, multiple-core), parent and child process execution separate.
+</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">Process Termination</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> - Process terminates with </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">exit()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> system call and return value for waiting parent process (via the wait() system call) and all resources (physical and virtual memory, open files, I/O buffers) deallocated and reclaimed.
+ - A process can be terminated by system call exit(), can by parent process or other user’s processes.
+ - </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Zombie process</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">: When a child process terminates (exits()), but parent process not invoke wait() → child process not released.
+ - </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Orphans process</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">: A child process terminates (exits()) but parent process not invoke wait() and terminates. But in traditional system (init process) or modern system (system process) periodically invokes wait() to releasing the orphan’s process in process-table entry.</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">Interprocess Communication</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> - Processes executing concurrently in the OS may be </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">independent</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (not share data with processes) or </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">cooperating</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (share data / affect or affected by processes) processes.
+ - Why need cooperating processes:
+  + Information sharing between processes.
+  + Computation speedup: break task into subtasks and executing parallel (multiple processor cores).
+  + Modularity: System divided into separate processes or threads.
+ - Cooperating processes require an </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">interprocess communication (IPC)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> mechanism that will allow exchange data: </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">shared memory</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">message passing</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.
+ - Shared memory: 
+  + A region of memory shared by cooperating processes, processes can exchange information (reading, writing).
+  + Faster than message passing.
+ - Message passing: 
+  + Messages exchanged by message queue between the cooperating processes.
+  + Useful for smaller data.
+  + Easier to implement in a distributed system.</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">IPC in Shared-Memory Systems</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> - A shared-memory region resides in the address space of the process creating the </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">shared-memory segment</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">. And other processes that wish to communicate using this shared-memory segment must </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">attach</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> it to their address space.
+ - Restriction: prevent one process from accessing another process’s memory.
+ → Shared memory requires that two or more processes agree to remove this restriction.
+ - Process control form of data, location and ensuring not writing same location simultaneously.</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">IPC in Message-Passing Systems</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> - A mechanism to allow processes to communicate and to synchronize their actions without sharing the same address space.
+ - Useful in a distributed environment, where the communicating processes may reside on different computers connected by a network.
+ - System-level implementation is straight-forward if fixed-sized messages, but difficult if variable-sized → tradeoff.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve"> - Communication link</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">Naming</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Direct communication:
+ Symmetry: 
+  - Each process that want communicate must explicitly name the recipient or sender of communication:
+   + send(P, message) —Send a message to process P.
+   + receive(Q, message) —Receive a message from process Q.
+  - Communication link in this scheme has the following properties:
+   + A link is established automatically between every of processes, and know identity of each other.
+   + A link is associated with exactly two processes.
+   + Between each pair of processes, there exists exactly one link.
+ Asymmetry:
+  - follows: 
+   + send(P, message) —Send a message to process P.
+   + receive(id, message) —Receive a message from any process. The variable id is set to the name of the process with which communication has taken place.
+→ The disadvantage in both of these schemes (symmetric and asymmetric) is the limited modularity of the resulting process definitions. Changing the identifier of a process may necessitate examining all other process definitions.
+</t>
   </si>
   <si>
     <t xml:space="preserve">Synchronization</t>
@@ -7827,8 +8408,8 @@
     <font>
       <sz val="15"/>
       <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <name val="Linux Libertine O"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -8079,7 +8660,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -8285,9 +8866,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>581040</xdr:colOff>
+      <xdr:colOff>580680</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>2113920</xdr:rowOff>
+      <xdr:rowOff>2113560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8301,7 +8882,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10237320" y="8324640"/>
-          <a:ext cx="4793760" cy="2791080"/>
+          <a:ext cx="4793400" cy="2790720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8322,9 +8903,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>657360</xdr:colOff>
+      <xdr:colOff>657000</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>1789920</xdr:rowOff>
+      <xdr:rowOff>1789560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8338,7 +8919,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10323000" y="11420280"/>
-          <a:ext cx="4784400" cy="2486160"/>
+          <a:ext cx="4784040" cy="2485800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8359,9 +8940,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>514440</xdr:colOff>
+      <xdr:colOff>514080</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>688680</xdr:rowOff>
+      <xdr:rowOff>688320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8375,7 +8956,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10170720" y="24355440"/>
-          <a:ext cx="4793760" cy="2895840"/>
+          <a:ext cx="4793400" cy="2895480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8567,10 +9148,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G99"/>
+  <dimension ref="A1:G100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E78" colorId="64" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F84" activeCellId="0" sqref="F84"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D81" colorId="64" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E82" activeCellId="0" sqref="E82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="36.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8775,7 +9356,7 @@
       </c>
       <c r="G14" s="13"/>
     </row>
-    <row r="15" customFormat="false" ht="126.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="129.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="9"/>
@@ -8942,7 +9523,7 @@
       </c>
       <c r="G27" s="11"/>
     </row>
-    <row r="28" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="53.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="7"/>
       <c r="B28" s="8"/>
       <c r="C28" s="9"/>
@@ -9111,7 +9692,7 @@
       </c>
       <c r="G40" s="13"/>
     </row>
-    <row r="41" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="87.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="7"/>
       <c r="B41" s="8"/>
       <c r="C41" s="9"/>
@@ -9227,7 +9808,7 @@
       </c>
       <c r="G49" s="11"/>
     </row>
-    <row r="50" customFormat="false" ht="280.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="285.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="7"/>
       <c r="B50" s="8"/>
       <c r="C50" s="9"/>
@@ -9250,7 +9831,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="138.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="141.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="7"/>
       <c r="B52" s="8"/>
       <c r="C52" s="9"/>
@@ -9263,7 +9844,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="7"/>
       <c r="B53" s="8"/>
       <c r="C53" s="9"/>
@@ -9276,7 +9857,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="190.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="193.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="7"/>
       <c r="B54" s="8"/>
       <c r="C54" s="9"/>
@@ -9589,9 +10170,10 @@
       <c r="E77" s="14" t="s">
         <v>156</v>
       </c>
-      <c r="F77" s="5" t="s">
+      <c r="F77" s="11" t="s">
         <v>157</v>
       </c>
+      <c r="G77" s="11"/>
     </row>
     <row r="78" customFormat="false" ht="50.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="7"/>
@@ -9601,12 +10183,12 @@
       <c r="E78" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="F78" s="21" t="s">
+      <c r="F78" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="G78" s="21"/>
-    </row>
-    <row r="79" customFormat="false" ht="36.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G78" s="11"/>
+    </row>
+    <row r="79" customFormat="false" ht="263.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="7"/>
       <c r="B79" s="8"/>
       <c r="C79" s="9"/>
@@ -9616,65 +10198,75 @@
       <c r="E79" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="F79" s="21"/>
-      <c r="G79" s="21"/>
-    </row>
-    <row r="80" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F79" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="G79" s="11"/>
+    </row>
+    <row r="80" customFormat="false" ht="106.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="7"/>
       <c r="B80" s="8"/>
       <c r="C80" s="9"/>
       <c r="D80" s="10"/>
       <c r="E80" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="F80" s="21"/>
-      <c r="G80" s="21"/>
-    </row>
-    <row r="81" customFormat="false" ht="61.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>163</v>
+      </c>
+      <c r="F80" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="G80" s="11"/>
+    </row>
+    <row r="81" customFormat="false" ht="228.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="7"/>
       <c r="B81" s="8"/>
       <c r="C81" s="9"/>
       <c r="D81" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="E81" s="14"/>
-      <c r="F81" s="14"/>
-      <c r="G81" s="14"/>
-    </row>
-    <row r="82" customFormat="false" ht="61.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>165</v>
+      </c>
+      <c r="E81" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="F81" s="11"/>
+      <c r="G81" s="11"/>
+    </row>
+    <row r="82" customFormat="false" ht="88.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="7"/>
       <c r="B82" s="8"/>
       <c r="C82" s="9"/>
       <c r="D82" s="10" t="s">
-        <v>164</v>
-      </c>
-      <c r="E82" s="14"/>
-      <c r="F82" s="14"/>
-      <c r="G82" s="14"/>
-    </row>
-    <row r="83" customFormat="false" ht="36.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>167</v>
+      </c>
+      <c r="E82" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="F82" s="11"/>
+      <c r="G82" s="11"/>
+    </row>
+    <row r="83" customFormat="false" ht="71.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="7"/>
       <c r="B83" s="8"/>
       <c r="C83" s="9"/>
       <c r="D83" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="E83" s="14" t="s">
-        <v>166</v>
+        <v>169</v>
+      </c>
+      <c r="E83" s="21" t="s">
+        <v>170</v>
       </c>
       <c r="F83" s="21"/>
       <c r="G83" s="21"/>
     </row>
-    <row r="84" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="281" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="7"/>
       <c r="B84" s="8"/>
       <c r="C84" s="9"/>
       <c r="D84" s="10"/>
       <c r="E84" s="14" t="s">
-        <v>167</v>
-      </c>
-      <c r="F84" s="21"/>
-      <c r="G84" s="21"/>
+        <v>171</v>
+      </c>
+      <c r="F84" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="G84" s="11"/>
     </row>
     <row r="85" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="7"/>
@@ -9682,53 +10274,56 @@
       <c r="C85" s="9"/>
       <c r="D85" s="10"/>
       <c r="E85" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="F85" s="21"/>
-      <c r="G85" s="21"/>
-    </row>
-    <row r="86" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>173</v>
+      </c>
+      <c r="F85" s="11"/>
+      <c r="G85" s="11"/>
+    </row>
+    <row r="86" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="7"/>
       <c r="B86" s="8"/>
       <c r="C86" s="9"/>
-      <c r="D86" s="10" t="s">
-        <v>169</v>
-      </c>
-      <c r="E86" s="14"/>
-      <c r="F86" s="14"/>
-      <c r="G86" s="14"/>
-    </row>
-    <row r="87" customFormat="false" ht="36.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D86" s="10"/>
+      <c r="E86" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="F86" s="11"/>
+      <c r="G86" s="11"/>
+    </row>
+    <row r="87" customFormat="false" ht="44.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="7"/>
       <c r="B87" s="8"/>
       <c r="C87" s="9"/>
       <c r="D87" s="10" t="s">
-        <v>170</v>
-      </c>
-      <c r="E87" s="14" t="s">
-        <v>171</v>
-      </c>
-      <c r="F87" s="21"/>
-      <c r="G87" s="21"/>
-    </row>
-    <row r="88" customFormat="false" ht="52.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>175</v>
+      </c>
+      <c r="E87" s="12"/>
+      <c r="F87" s="12"/>
+      <c r="G87" s="12"/>
+    </row>
+    <row r="88" customFormat="false" ht="36.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="7"/>
       <c r="B88" s="8"/>
       <c r="C88" s="9"/>
-      <c r="D88" s="10"/>
+      <c r="D88" s="10" t="s">
+        <v>176</v>
+      </c>
       <c r="E88" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="F88" s="21"/>
-      <c r="G88" s="21"/>
-    </row>
-    <row r="89" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>177</v>
+      </c>
+      <c r="F88" s="11"/>
+      <c r="G88" s="11"/>
+    </row>
+    <row r="89" customFormat="false" ht="53.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="7"/>
       <c r="B89" s="8"/>
       <c r="C89" s="9"/>
       <c r="D89" s="10"/>
-      <c r="E89" s="14"/>
-      <c r="F89" s="21"/>
+      <c r="E89" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="F89" s="11"/>
+      <c r="G89" s="11"/>
     </row>
     <row r="90" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="7"/>
@@ -9736,24 +10331,29 @@
       <c r="C90" s="9"/>
       <c r="D90" s="10"/>
       <c r="E90" s="14"/>
-      <c r="F90" s="21"/>
-    </row>
-    <row r="91" customFormat="false" ht="70.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F90" s="19"/>
+    </row>
+    <row r="91" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="7"/>
       <c r="B91" s="8"/>
-      <c r="C91" s="3" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="47.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C91" s="9"/>
+      <c r="D91" s="10"/>
+      <c r="E91" s="14"/>
+      <c r="F91" s="19"/>
+    </row>
+    <row r="92" customFormat="false" ht="70.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="7"/>
       <c r="B92" s="8"/>
       <c r="C92" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="47.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="7"/>
+      <c r="B93" s="8"/>
+      <c r="C93" s="3" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="93" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="7"/>
     </row>
     <row r="94" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="7"/>
@@ -9773,9 +10373,12 @@
     <row r="99" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="7"/>
     </row>
+    <row r="100" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="7"/>
+    </row>
   </sheetData>
-  <mergeCells count="99">
-    <mergeCell ref="A1:A99"/>
+  <mergeCells count="100">
+    <mergeCell ref="A1:A100"/>
     <mergeCell ref="B1:B69"/>
     <mergeCell ref="C1:C41"/>
     <mergeCell ref="D1:D4"/>
@@ -9850,8 +10453,8 @@
     <mergeCell ref="F69:G69"/>
     <mergeCell ref="D70:D74"/>
     <mergeCell ref="E70:G70"/>
-    <mergeCell ref="B71:B92"/>
-    <mergeCell ref="C71:C88"/>
+    <mergeCell ref="B71:B93"/>
+    <mergeCell ref="C71:C89"/>
     <mergeCell ref="F71:G71"/>
     <mergeCell ref="F72:G72"/>
     <mergeCell ref="F73:G73"/>
@@ -9866,14 +10469,15 @@
     <mergeCell ref="F80:G80"/>
     <mergeCell ref="E81:G81"/>
     <mergeCell ref="E82:G82"/>
-    <mergeCell ref="D83:D85"/>
-    <mergeCell ref="F83:G83"/>
+    <mergeCell ref="D83:D86"/>
+    <mergeCell ref="E83:G83"/>
     <mergeCell ref="F84:G84"/>
     <mergeCell ref="F85:G85"/>
-    <mergeCell ref="E86:G86"/>
-    <mergeCell ref="D87:D88"/>
-    <mergeCell ref="F87:G87"/>
+    <mergeCell ref="F86:G86"/>
+    <mergeCell ref="E87:G87"/>
+    <mergeCell ref="D88:D89"/>
     <mergeCell ref="F88:G88"/>
+    <mergeCell ref="F89:G89"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
@@ -9905,26 +10509,26 @@
   <sheetData>
     <row r="1" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="22" t="s">
-        <v>324</v>
+        <v>330</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>325</v>
+        <v>331</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
-        <v>326</v>
+        <v>332</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>327</v>
+        <v>333</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="25" t="s">
-        <v>328</v>
+        <v>334</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>329</v>
+        <v>335</v>
       </c>
     </row>
   </sheetData>
@@ -9989,10 +10593,10 @@
         <v>1</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10000,10 +10604,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10011,10 +10615,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10022,10 +10626,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10033,10 +10637,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10044,10 +10648,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="256.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10055,10 +10659,10 @@
         <v>7</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="245.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10066,10 +10670,10 @@
         <v>8</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="223.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10077,10 +10681,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="243.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10088,86 +10692,86 @@
         <v>10</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="22" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="22" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="22" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="288.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="22" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="E14" s="25" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="F14" s="25" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="G14" s="25" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="22" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="240.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B16" s="22" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="22" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="22" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -10204,272 +10808,272 @@
   <sheetData>
     <row r="1" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="30" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="B1" s="30"/>
     </row>
     <row r="2" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="28" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="28" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="28" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="28" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="33" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="B8" s="33"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="34" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="B9" s="35" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="36" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="B10" s="35" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="36" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="35" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="B12" s="35" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="35" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="B13" s="35" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="35" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="B14" s="35" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="35" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="B15" s="35" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="35" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="B16" s="35" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="35" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="B17" s="35" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="35" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="B18" s="35" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="35" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="B19" s="35" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="35" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="B20" s="35" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="35" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="B21" s="35" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="30" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="B25" s="30"/>
     </row>
     <row r="26" customFormat="false" ht="283.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="28" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="B26" s="31" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="28" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="B27" s="31" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="38" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="B28" s="31" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="28" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="B29" s="31" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="28" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="B30" s="31" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="28" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="B31" s="31" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="28" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="B32" s="31" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="28" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="B33" s="31" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="39" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
       <c r="B34" s="31" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="39"/>
       <c r="B35" s="31" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="39"/>
       <c r="B36" s="31" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="39"/>
       <c r="B37" s="31" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="39"/>
       <c r="B38" s="31" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="39"/>
       <c r="B39" s="32" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="39"/>
       <c r="B40" s="31" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="28" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="B41" s="32" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -10531,18 +11135,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="25" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -10576,25 +11180,25 @@
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="29" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="29" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="29" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="29" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>
@@ -10628,10 +11232,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="40" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="B1" s="41" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10639,120 +11243,120 @@
     </row>
     <row r="3" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="43" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="B3" s="44" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="43"/>
       <c r="B4" s="44" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>291</v>
+        <v>297</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="43"/>
       <c r="B5" s="29" t="s">
-        <v>292</v>
+        <v>298</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="43"/>
       <c r="B6" s="29" t="s">
-        <v>293</v>
+        <v>299</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="43"/>
       <c r="B7" s="29" t="s">
-        <v>294</v>
+        <v>300</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="43"/>
       <c r="B8" s="45" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="C8" s="31" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="43"/>
       <c r="B9" s="45"/>
       <c r="C9" s="31" t="s">
-        <v>297</v>
+        <v>303</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="43"/>
       <c r="B10" s="45"/>
       <c r="C10" s="31" t="s">
-        <v>298</v>
+        <v>304</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="43"/>
       <c r="B11" s="45"/>
       <c r="C11" s="29" t="s">
-        <v>299</v>
+        <v>305</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="43"/>
       <c r="B12" s="45"/>
       <c r="C12" s="31" t="s">
-        <v>300</v>
+        <v>306</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="43"/>
       <c r="B13" s="29" t="s">
-        <v>301</v>
+        <v>307</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="216.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="43"/>
       <c r="B14" s="46" t="s">
-        <v>302</v>
+        <v>308</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>303</v>
+        <v>309</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="43"/>
       <c r="B15" s="46"/>
       <c r="C15" s="47" t="s">
-        <v>304</v>
+        <v>310</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="43"/>
       <c r="B16" s="46"/>
       <c r="C16" s="47" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="43"/>
       <c r="B17" s="46"/>
       <c r="C17" s="47" t="s">
-        <v>306</v>
+        <v>312</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="43"/>
       <c r="B18" s="46"/>
       <c r="C18" s="31" t="s">
-        <v>307</v>
+        <v>313</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10761,13 +11365,13 @@
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="43"/>
       <c r="B20" s="48" t="s">
-        <v>308</v>
+        <v>314</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="43"/>
       <c r="B21" s="29" t="s">
-        <v>309</v>
+        <v>315</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10778,40 +11382,40 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="43" t="s">
-        <v>310</v>
+        <v>316</v>
       </c>
       <c r="B24" s="29" t="s">
-        <v>311</v>
+        <v>317</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="43"/>
       <c r="B25" s="29" t="s">
-        <v>312</v>
+        <v>318</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="43"/>
       <c r="B26" s="29" t="s">
-        <v>313</v>
+        <v>319</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="43"/>
       <c r="B27" s="29" t="s">
-        <v>314</v>
+        <v>320</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="43"/>
       <c r="B28" s="31" t="s">
-        <v>315</v>
+        <v>321</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="43"/>
       <c r="B29" s="31" t="s">
-        <v>316</v>
+        <v>322</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10819,41 +11423,41 @@
     </row>
     <row r="31" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="43" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
       <c r="B31" s="31" t="s">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="F31" s="50"/>
     </row>
     <row r="32" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="43"/>
       <c r="B32" s="31" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="43"/>
       <c r="B33" s="31" t="s">
-        <v>320</v>
+        <v>326</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="43"/>
       <c r="B34" s="31" t="s">
-        <v>321</v>
+        <v>327</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="43"/>
       <c r="B35" s="31" t="s">
-        <v>322</v>
+        <v>328</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="43"/>
       <c r="B36" s="31" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="C36" s="31"/>
     </row>

</xml_diff>

<commit_message>
[feat][OS][IPC-Messaging system: Directly, Indirectly, Synchronous, Asynchronous, Buffering]
</commit_message>
<xml_diff>
--- a/Operations-System/DevOps-Documents.xlsx
+++ b/Operations-System/DevOps-Documents.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="338">
   <si>
     <t xml:space="preserve">Operating System Concepts</t>
   </si>
@@ -5999,28 +5999,10 @@
     <t xml:space="preserve">IPC in Message-Passing Systems</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="15"/>
-        <color theme="1"/>
-        <rFont val="Linux Libertine O"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> - A mechanism to allow processes to communicate and to synchronize their actions without sharing the same address space.
+    <t xml:space="preserve"> - A mechanism to allow processes to communicate and to synchronize their actions without sharing the same address space.
  - Useful in a distributed environment, where the communicating processes may reside on different computers connected by a network.
  - System-level implementation is straight-forward if fixed-sized messages, but difficult if variable-sized → tradeoff.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15"/>
-        <color theme="1"/>
-        <rFont val="Linux Libertine O"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve"> - Communication link</t>
-    </r>
+ - Communication link</t>
   </si>
   <si>
     <t xml:space="preserve">Naming</t>
@@ -6046,7 +6028,102 @@
     <t xml:space="preserve">Synchronization</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> - Message passing may be either </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">blocking or non-blocking</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> also known as </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">synchronous and asynchronous</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">:
+  + Blocking send: The sending process is blocked until the message is received by the receiving process or by the mailbox.
+  + Non-blocking send: The sending process sends the message and resumes operation.
+  + Blocking receive: The receiver blocks until a message is available.
+  + Non-blocking receive: The receiver retrieves either a valid message or a null.</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">Buffering</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Messages exchanged by communicating processes reside in a </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">temporary queue</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Linux Libertine O"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">. Basically, such queues can be implemented in three ways:
+ - Zero capacity: Queue has a maximum length of zero; thus, the link cannot have any messages waiting in it. The sender must block until the recipient receives the message.
+ - Bounded capacity: The queue has finite length n; thus, at most n messages can reside in it. If the queue is not full when a new message is sent, the message is placed in the queue (either the message is copied or a pointer to the message is kept), and the sender can continue execution without waiting. If the link is full, the sender
+must block until space is available in the queue.
+ - Unbounded capacity: The queue’s length is potentially infinite; thus, any number of messages can wait in it. The sender never blocks.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Examples of IPC Systems</t>
@@ -8238,7 +8315,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="37">
+  <fonts count="36">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -8406,12 +8483,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="15"/>
-      <color theme="1"/>
-      <name val="Linux Libertine O"/>
-      <family val="0"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -8565,17 +8636,17 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="32" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="36" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="35" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="50">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -8660,19 +8731,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -8680,15 +8747,15 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -8696,7 +8763,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -8708,11 +8775,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -8720,7 +8787,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -8728,19 +8795,19 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -8748,7 +8815,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="32" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="31" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -8756,7 +8823,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -8764,19 +8831,19 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="36" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="35" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -8866,9 +8933,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>580680</xdr:colOff>
+      <xdr:colOff>580320</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>2113560</xdr:rowOff>
+      <xdr:rowOff>2113200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8882,7 +8949,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10237320" y="8324640"/>
-          <a:ext cx="4793400" cy="2790720"/>
+          <a:ext cx="4793040" cy="2790360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8903,9 +8970,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>657000</xdr:colOff>
+      <xdr:colOff>656640</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>1789560</xdr:rowOff>
+      <xdr:rowOff>1789200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8919,7 +8986,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10323000" y="11420280"/>
-          <a:ext cx="4784040" cy="2485800"/>
+          <a:ext cx="4783680" cy="2485440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8940,9 +9007,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>514080</xdr:colOff>
+      <xdr:colOff>513720</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>688320</xdr:rowOff>
+      <xdr:rowOff>687960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8956,7 +9023,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10170720" y="24355440"/>
-          <a:ext cx="4793400" cy="2895480"/>
+          <a:ext cx="4793040" cy="2895120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9150,8 +9217,8 @@
   </sheetPr>
   <dimension ref="A1:G100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D81" colorId="64" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E82" activeCellId="0" sqref="E82"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D84" colorId="64" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F86" activeCellId="0" sqref="F86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="36.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9356,7 +9423,7 @@
       </c>
       <c r="G14" s="13"/>
     </row>
-    <row r="15" customFormat="false" ht="129.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="126.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="9"/>
@@ -9523,7 +9590,7 @@
       </c>
       <c r="G27" s="11"/>
     </row>
-    <row r="28" customFormat="false" ht="53.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="7"/>
       <c r="B28" s="8"/>
       <c r="C28" s="9"/>
@@ -9692,7 +9759,7 @@
       </c>
       <c r="G40" s="13"/>
     </row>
-    <row r="41" customFormat="false" ht="87.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="7"/>
       <c r="B41" s="8"/>
       <c r="C41" s="9"/>
@@ -9808,7 +9875,7 @@
       </c>
       <c r="G49" s="11"/>
     </row>
-    <row r="50" customFormat="false" ht="285.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="280.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="7"/>
       <c r="B50" s="8"/>
       <c r="C50" s="9"/>
@@ -9831,7 +9898,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="141.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="138.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="7"/>
       <c r="B52" s="8"/>
       <c r="C52" s="9"/>
@@ -9857,7 +9924,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="193.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="190.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="7"/>
       <c r="B54" s="8"/>
       <c r="C54" s="9"/>
@@ -10249,11 +10316,11 @@
       <c r="D83" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="E83" s="21" t="s">
+      <c r="E83" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="F83" s="21"/>
-      <c r="G83" s="21"/>
+      <c r="F83" s="11"/>
+      <c r="G83" s="11"/>
     </row>
     <row r="84" customFormat="false" ht="281" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="7"/>
@@ -10268,7 +10335,7 @@
       </c>
       <c r="G84" s="11"/>
     </row>
-    <row r="85" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="88.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="7"/>
       <c r="B85" s="8"/>
       <c r="C85" s="9"/>
@@ -10276,26 +10343,30 @@
       <c r="E85" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="F85" s="11"/>
+      <c r="F85" s="11" t="s">
+        <v>174</v>
+      </c>
       <c r="G85" s="11"/>
     </row>
-    <row r="86" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="106.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="7"/>
       <c r="B86" s="8"/>
       <c r="C86" s="9"/>
       <c r="D86" s="10"/>
       <c r="E86" s="14" t="s">
-        <v>174</v>
-      </c>
-      <c r="F86" s="11"/>
+        <v>175</v>
+      </c>
+      <c r="F86" s="11" t="s">
+        <v>176</v>
+      </c>
       <c r="G86" s="11"/>
     </row>
-    <row r="87" customFormat="false" ht="44.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="7"/>
       <c r="B87" s="8"/>
       <c r="C87" s="9"/>
       <c r="D87" s="10" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="E87" s="12"/>
       <c r="F87" s="12"/>
@@ -10306,21 +10377,21 @@
       <c r="B88" s="8"/>
       <c r="C88" s="9"/>
       <c r="D88" s="10" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="E88" s="14" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="F88" s="11"/>
       <c r="G88" s="11"/>
     </row>
-    <row r="89" customFormat="false" ht="53.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="52.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="7"/>
       <c r="B89" s="8"/>
       <c r="C89" s="9"/>
       <c r="D89" s="10"/>
       <c r="E89" s="14" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="F89" s="11"/>
       <c r="G89" s="11"/>
@@ -10345,7 +10416,7 @@
       <c r="A92" s="7"/>
       <c r="B92" s="8"/>
       <c r="C92" s="3" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="47.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10502,33 +10573,33 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="22" width="23.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="22" width="57.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="3" style="22" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="21" width="23.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="21" width="57.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="3" style="21" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="22" t="s">
-        <v>330</v>
-      </c>
-      <c r="B1" s="25" t="s">
-        <v>331</v>
+      <c r="A1" s="21" t="s">
+        <v>332</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="25" t="s">
-        <v>332</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>333</v>
+      <c r="A2" s="24" t="s">
+        <v>334</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="25" t="s">
-        <v>334</v>
-      </c>
-      <c r="B3" s="25" t="s">
-        <v>335</v>
+      <c r="A3" s="24" t="s">
+        <v>336</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>337</v>
       </c>
     </row>
   </sheetData>
@@ -10578,200 +10649,200 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="22" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="22" width="39.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="22" width="95.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="22" width="60.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="22" width="58.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="22" width="50"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="22" width="49.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="8" style="22" width="9.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="21" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="21" width="39.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="21" width="95.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="21" width="60.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="21" width="58.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="21" width="50"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="21" width="49.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="8" style="21" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="22" t="n">
+      <c r="A1" s="21" t="n">
         <v>1</v>
       </c>
-      <c r="B1" s="22" t="s">
-        <v>180</v>
-      </c>
-      <c r="C1" s="23" t="s">
-        <v>181</v>
+      <c r="B1" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="22" t="n">
+      <c r="A2" s="21" t="n">
         <v>2</v>
       </c>
-      <c r="B2" s="22" t="s">
-        <v>182</v>
-      </c>
-      <c r="C2" s="23" t="s">
-        <v>183</v>
+      <c r="B2" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="22" t="n">
+      <c r="A3" s="21" t="n">
         <v>3</v>
       </c>
-      <c r="B3" s="24" t="s">
-        <v>184</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>185</v>
+      <c r="B3" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="22" t="n">
+      <c r="A4" s="21" t="n">
         <v>4</v>
       </c>
-      <c r="B4" s="22" t="s">
-        <v>186</v>
-      </c>
-      <c r="C4" s="25" t="s">
-        <v>187</v>
+      <c r="B4" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="22" t="n">
+      <c r="A5" s="21" t="n">
         <v>5</v>
       </c>
-      <c r="B5" s="22" t="s">
-        <v>188</v>
-      </c>
-      <c r="C5" s="25" t="s">
-        <v>189</v>
+      <c r="B5" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="22" t="n">
+      <c r="A6" s="21" t="n">
         <v>6</v>
       </c>
-      <c r="B6" s="22" t="s">
-        <v>190</v>
-      </c>
-      <c r="C6" s="25" t="s">
-        <v>191</v>
+      <c r="B6" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="256.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="22" t="n">
+      <c r="A7" s="21" t="n">
         <v>7</v>
       </c>
-      <c r="B7" s="22" t="s">
-        <v>192</v>
-      </c>
-      <c r="C7" s="26" t="s">
-        <v>193</v>
+      <c r="B7" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="245.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="22" t="n">
+      <c r="A8" s="21" t="n">
         <v>8</v>
       </c>
-      <c r="B8" s="22" t="s">
-        <v>194</v>
-      </c>
-      <c r="C8" s="23" t="s">
-        <v>195</v>
+      <c r="B8" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="223.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="22" t="n">
+      <c r="A9" s="21" t="n">
         <v>9</v>
       </c>
-      <c r="B9" s="22" t="s">
-        <v>196</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>197</v>
+      <c r="B9" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="243.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="22" t="n">
+      <c r="A10" s="21" t="n">
         <v>10</v>
       </c>
-      <c r="B10" s="22" t="s">
-        <v>198</v>
-      </c>
-      <c r="C10" s="25" t="s">
-        <v>199</v>
-      </c>
-      <c r="D10" s="27" t="s">
+      <c r="B10" s="21" t="s">
         <v>200</v>
       </c>
+      <c r="C10" s="24" t="s">
+        <v>201</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="22" t="s">
-        <v>201</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>202</v>
+      <c r="B11" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="22" t="s">
-        <v>203</v>
-      </c>
-      <c r="C12" s="25" t="s">
-        <v>204</v>
+      <c r="B12" s="21" t="s">
+        <v>205</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="22" t="s">
-        <v>205</v>
-      </c>
-      <c r="C13" s="25" t="s">
-        <v>206</v>
+      <c r="B13" s="21" t="s">
+        <v>207</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="288.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="22" t="s">
-        <v>207</v>
-      </c>
-      <c r="C14" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="D14" s="23" t="s">
+      <c r="B14" s="21" t="s">
         <v>209</v>
       </c>
-      <c r="E14" s="25" t="s">
+      <c r="C14" s="24" t="s">
         <v>210</v>
       </c>
-      <c r="F14" s="25" t="s">
+      <c r="D14" s="22" t="s">
         <v>211</v>
       </c>
-      <c r="G14" s="25" t="s">
+      <c r="E14" s="24" t="s">
         <v>212</v>
       </c>
+      <c r="F14" s="24" t="s">
+        <v>213</v>
+      </c>
+      <c r="G14" s="24" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="22" t="s">
-        <v>213</v>
-      </c>
-      <c r="C15" s="25" t="s">
-        <v>214</v>
+      <c r="B15" s="21" t="s">
+        <v>215</v>
+      </c>
+      <c r="C15" s="24" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="240.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="22" t="s">
-        <v>215</v>
+      <c r="B16" s="21" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="22" t="s">
-        <v>216</v>
-      </c>
-      <c r="C17" s="23" t="s">
-        <v>217</v>
+      <c r="B17" s="21" t="s">
+        <v>218</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="22" t="s">
-        <v>218</v>
-      </c>
-      <c r="C18" s="23" t="s">
-        <v>219</v>
+      <c r="B18" s="21" t="s">
+        <v>220</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -10802,278 +10873,278 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="28" width="72.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="29" width="139.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="27" width="72.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="28" width="139.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="30" t="s">
-        <v>220</v>
-      </c>
-      <c r="B1" s="30"/>
+      <c r="A1" s="29" t="s">
+        <v>222</v>
+      </c>
+      <c r="B1" s="29"/>
     </row>
     <row r="2" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="28" t="s">
-        <v>221</v>
-      </c>
-      <c r="B2" s="31" t="s">
-        <v>222</v>
+      <c r="A2" s="27" t="s">
+        <v>223</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="28" t="s">
-        <v>223</v>
-      </c>
-      <c r="B3" s="32" t="s">
-        <v>224</v>
+      <c r="A3" s="27" t="s">
+        <v>225</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="28" t="s">
-        <v>225</v>
-      </c>
-      <c r="B4" s="32" t="s">
-        <v>226</v>
+      <c r="A4" s="27" t="s">
+        <v>227</v>
+      </c>
+      <c r="B4" s="31" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="28" t="s">
-        <v>227</v>
-      </c>
-      <c r="B5" s="32" t="s">
-        <v>228</v>
+      <c r="A5" s="27" t="s">
+        <v>229</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="33" t="s">
-        <v>229</v>
-      </c>
-      <c r="B8" s="33"/>
+      <c r="A8" s="32" t="s">
+        <v>231</v>
+      </c>
+      <c r="B8" s="32"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="34" t="s">
-        <v>230</v>
-      </c>
-      <c r="B9" s="35" t="s">
-        <v>231</v>
+      <c r="A9" s="33" t="s">
+        <v>232</v>
+      </c>
+      <c r="B9" s="34" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="36" t="s">
-        <v>232</v>
-      </c>
-      <c r="B10" s="35" t="s">
-        <v>233</v>
+      <c r="A10" s="35" t="s">
+        <v>234</v>
+      </c>
+      <c r="B10" s="34" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="36" t="s">
-        <v>234</v>
-      </c>
-      <c r="B11" s="37" t="s">
-        <v>235</v>
+      <c r="A11" s="35" t="s">
+        <v>236</v>
+      </c>
+      <c r="B11" s="36" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="35" t="s">
-        <v>236</v>
-      </c>
-      <c r="B12" s="35" t="s">
-        <v>237</v>
+      <c r="A12" s="34" t="s">
+        <v>238</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="35" t="s">
-        <v>238</v>
-      </c>
-      <c r="B13" s="35" t="s">
-        <v>239</v>
+      <c r="A13" s="34" t="s">
+        <v>240</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="35" t="s">
-        <v>240</v>
-      </c>
-      <c r="B14" s="35" t="s">
-        <v>241</v>
+      <c r="A14" s="34" t="s">
+        <v>242</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="35" t="s">
-        <v>242</v>
-      </c>
-      <c r="B15" s="35" t="s">
-        <v>243</v>
+      <c r="A15" s="34" t="s">
+        <v>244</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="35" t="s">
-        <v>244</v>
-      </c>
-      <c r="B16" s="35" t="s">
-        <v>245</v>
+      <c r="A16" s="34" t="s">
+        <v>246</v>
+      </c>
+      <c r="B16" s="34" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="35" t="s">
-        <v>246</v>
-      </c>
-      <c r="B17" s="35" t="s">
-        <v>247</v>
+      <c r="A17" s="34" t="s">
+        <v>248</v>
+      </c>
+      <c r="B17" s="34" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="35" t="s">
-        <v>248</v>
-      </c>
-      <c r="B18" s="35" t="s">
-        <v>249</v>
+      <c r="A18" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="B18" s="34" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="35" t="s">
-        <v>250</v>
-      </c>
-      <c r="B19" s="35" t="s">
-        <v>251</v>
+      <c r="A19" s="34" t="s">
+        <v>252</v>
+      </c>
+      <c r="B19" s="34" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="35" t="s">
-        <v>252</v>
-      </c>
-      <c r="B20" s="35" t="s">
-        <v>253</v>
+      <c r="A20" s="34" t="s">
+        <v>254</v>
+      </c>
+      <c r="B20" s="34" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="35" t="s">
-        <v>254</v>
-      </c>
-      <c r="B21" s="35" t="s">
-        <v>255</v>
+      <c r="A21" s="34" t="s">
+        <v>256</v>
+      </c>
+      <c r="B21" s="34" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="30" t="s">
-        <v>256</v>
-      </c>
-      <c r="B25" s="30"/>
+      <c r="A25" s="29" t="s">
+        <v>258</v>
+      </c>
+      <c r="B25" s="29"/>
     </row>
     <row r="26" customFormat="false" ht="283.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="28" t="s">
-        <v>257</v>
-      </c>
-      <c r="B26" s="31" t="s">
-        <v>258</v>
+      <c r="A26" s="27" t="s">
+        <v>259</v>
+      </c>
+      <c r="B26" s="30" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="28" t="s">
-        <v>259</v>
-      </c>
-      <c r="B27" s="31" t="s">
-        <v>260</v>
+      <c r="A27" s="27" t="s">
+        <v>261</v>
+      </c>
+      <c r="B27" s="30" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="38" t="s">
-        <v>261</v>
-      </c>
-      <c r="B28" s="31" t="s">
-        <v>262</v>
+      <c r="A28" s="37" t="s">
+        <v>263</v>
+      </c>
+      <c r="B28" s="30" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="28" t="s">
-        <v>263</v>
-      </c>
-      <c r="B29" s="31" t="s">
-        <v>264</v>
+      <c r="A29" s="27" t="s">
+        <v>265</v>
+      </c>
+      <c r="B29" s="30" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="28" t="s">
-        <v>265</v>
-      </c>
-      <c r="B30" s="31" t="s">
-        <v>266</v>
+      <c r="A30" s="27" t="s">
+        <v>267</v>
+      </c>
+      <c r="B30" s="30" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="28" t="s">
-        <v>267</v>
-      </c>
-      <c r="B31" s="31" t="s">
-        <v>268</v>
+      <c r="A31" s="27" t="s">
+        <v>269</v>
+      </c>
+      <c r="B31" s="30" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="28" t="s">
-        <v>269</v>
-      </c>
-      <c r="B32" s="31" t="s">
-        <v>270</v>
+      <c r="A32" s="27" t="s">
+        <v>271</v>
+      </c>
+      <c r="B32" s="30" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="28" t="s">
-        <v>271</v>
-      </c>
-      <c r="B33" s="31" t="s">
-        <v>272</v>
+      <c r="A33" s="27" t="s">
+        <v>273</v>
+      </c>
+      <c r="B33" s="30" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="39" t="s">
-        <v>273</v>
-      </c>
-      <c r="B34" s="31" t="s">
-        <v>274</v>
+      <c r="A34" s="38" t="s">
+        <v>275</v>
+      </c>
+      <c r="B34" s="30" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="39"/>
-      <c r="B35" s="31" t="s">
-        <v>275</v>
+      <c r="A35" s="38"/>
+      <c r="B35" s="30" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="39"/>
-      <c r="B36" s="31" t="s">
-        <v>276</v>
+      <c r="A36" s="38"/>
+      <c r="B36" s="30" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="39"/>
-      <c r="B37" s="31" t="s">
-        <v>277</v>
+      <c r="A37" s="38"/>
+      <c r="B37" s="30" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="39"/>
-      <c r="B38" s="31" t="s">
-        <v>278</v>
+      <c r="A38" s="38"/>
+      <c r="B38" s="30" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="39"/>
-      <c r="B39" s="32" t="s">
-        <v>279</v>
+      <c r="A39" s="38"/>
+      <c r="B39" s="31" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="39"/>
-      <c r="B40" s="31" t="s">
-        <v>280</v>
+      <c r="A40" s="38"/>
+      <c r="B40" s="30" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="28" t="s">
-        <v>281</v>
-      </c>
-      <c r="B41" s="32" t="s">
-        <v>282</v>
+      <c r="A41" s="27" t="s">
+        <v>283</v>
+      </c>
+      <c r="B41" s="31" t="s">
+        <v>284</v>
       </c>
     </row>
   </sheetData>
@@ -11129,24 +11200,24 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="22" width="37.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="22" width="77.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="21" width="37.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="21" width="77.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
-        <v>283</v>
-      </c>
-      <c r="B1" s="25" t="s">
-        <v>284</v>
+      <c r="A1" s="24" t="s">
+        <v>285</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="22" t="s">
-        <v>285</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>286</v>
+      <c r="A2" s="21" t="s">
+        <v>287</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>288</v>
       </c>
     </row>
   </sheetData>
@@ -11173,32 +11244,32 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="29" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="29" width="60.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="28" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="28" width="60.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="29" t="s">
-        <v>287</v>
+      <c r="A2" s="28" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="29" t="s">
-        <v>288</v>
+      <c r="A4" s="28" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="29" t="s">
-        <v>289</v>
+      <c r="A6" s="28" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="29" t="s">
-        <v>290</v>
+      <c r="A8" s="28" t="s">
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -11225,241 +11296,241 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="29" width="28.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="29" width="49.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="29" width="69.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="28" width="28.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="28" width="49.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="28" width="69.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="40" t="s">
-        <v>291</v>
-      </c>
-      <c r="B1" s="41" t="s">
-        <v>292</v>
+      <c r="A1" s="39" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="42"/>
+      <c r="A2" s="41"/>
     </row>
     <row r="3" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="43" t="s">
-        <v>293</v>
-      </c>
-      <c r="B3" s="44" t="s">
-        <v>294</v>
-      </c>
-      <c r="C3" s="31" t="s">
+      <c r="A3" s="42" t="s">
         <v>295</v>
       </c>
+      <c r="B3" s="43" t="s">
+        <v>296</v>
+      </c>
+      <c r="C3" s="30" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="43"/>
-      <c r="B4" s="44" t="s">
-        <v>296</v>
-      </c>
-      <c r="C4" s="31" t="s">
-        <v>297</v>
+      <c r="A4" s="42"/>
+      <c r="B4" s="43" t="s">
+        <v>298</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="43"/>
-      <c r="B5" s="29" t="s">
-        <v>298</v>
+      <c r="A5" s="42"/>
+      <c r="B5" s="28" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="43"/>
-      <c r="B6" s="29" t="s">
-        <v>299</v>
+      <c r="A6" s="42"/>
+      <c r="B6" s="28" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="43"/>
-      <c r="B7" s="29" t="s">
-        <v>300</v>
+      <c r="A7" s="42"/>
+      <c r="B7" s="28" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="43"/>
-      <c r="B8" s="45" t="s">
-        <v>301</v>
-      </c>
-      <c r="C8" s="31" t="s">
-        <v>302</v>
+      <c r="A8" s="42"/>
+      <c r="B8" s="44" t="s">
+        <v>303</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="43"/>
-      <c r="B9" s="45"/>
-      <c r="C9" s="31" t="s">
-        <v>303</v>
+      <c r="A9" s="42"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="30" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="43"/>
-      <c r="B10" s="45"/>
-      <c r="C10" s="31" t="s">
-        <v>304</v>
+      <c r="A10" s="42"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="30" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="43"/>
-      <c r="B11" s="45"/>
-      <c r="C11" s="29" t="s">
-        <v>305</v>
+      <c r="A11" s="42"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="28" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="43"/>
-      <c r="B12" s="45"/>
-      <c r="C12" s="31" t="s">
-        <v>306</v>
+      <c r="A12" s="42"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="30" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="43"/>
-      <c r="B13" s="29" t="s">
-        <v>307</v>
+      <c r="A13" s="42"/>
+      <c r="B13" s="28" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="216.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="43"/>
-      <c r="B14" s="46" t="s">
-        <v>308</v>
-      </c>
-      <c r="C14" s="31" t="s">
-        <v>309</v>
+      <c r="A14" s="42"/>
+      <c r="B14" s="45" t="s">
+        <v>310</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="43"/>
-      <c r="B15" s="46"/>
-      <c r="C15" s="47" t="s">
-        <v>310</v>
+      <c r="A15" s="42"/>
+      <c r="B15" s="45"/>
+      <c r="C15" s="46" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="43"/>
-      <c r="B16" s="46"/>
-      <c r="C16" s="47" t="s">
-        <v>311</v>
+      <c r="A16" s="42"/>
+      <c r="B16" s="45"/>
+      <c r="C16" s="46" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="43"/>
-      <c r="B17" s="46"/>
-      <c r="C17" s="47" t="s">
-        <v>312</v>
+      <c r="A17" s="42"/>
+      <c r="B17" s="45"/>
+      <c r="C17" s="46" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="43"/>
-      <c r="B18" s="46"/>
-      <c r="C18" s="31" t="s">
-        <v>313</v>
+      <c r="A18" s="42"/>
+      <c r="B18" s="45"/>
+      <c r="C18" s="30" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="43"/>
+      <c r="A19" s="42"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="43"/>
-      <c r="B20" s="48" t="s">
-        <v>314</v>
+      <c r="A20" s="42"/>
+      <c r="B20" s="47" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="43"/>
-      <c r="B21" s="29" t="s">
-        <v>315</v>
+      <c r="A21" s="42"/>
+      <c r="B21" s="28" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="42"/>
+      <c r="A22" s="41"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="42"/>
+      <c r="A23" s="41"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="43" t="s">
-        <v>316</v>
-      </c>
-      <c r="B24" s="29" t="s">
-        <v>317</v>
+      <c r="A24" s="42" t="s">
+        <v>318</v>
+      </c>
+      <c r="B24" s="28" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="43"/>
-      <c r="B25" s="29" t="s">
-        <v>318</v>
+      <c r="A25" s="42"/>
+      <c r="B25" s="28" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="43"/>
-      <c r="B26" s="29" t="s">
-        <v>319</v>
+      <c r="A26" s="42"/>
+      <c r="B26" s="28" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="43"/>
-      <c r="B27" s="29" t="s">
-        <v>320</v>
+      <c r="A27" s="42"/>
+      <c r="B27" s="28" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="43"/>
-      <c r="B28" s="31" t="s">
-        <v>321</v>
+      <c r="A28" s="42"/>
+      <c r="B28" s="30" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="43"/>
-      <c r="B29" s="31" t="s">
-        <v>322</v>
+      <c r="A29" s="42"/>
+      <c r="B29" s="30" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="49"/>
+      <c r="A30" s="48"/>
     </row>
     <row r="31" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="43" t="s">
-        <v>323</v>
-      </c>
-      <c r="B31" s="31" t="s">
-        <v>324</v>
-      </c>
-      <c r="F31" s="50"/>
+      <c r="A31" s="42" t="s">
+        <v>325</v>
+      </c>
+      <c r="B31" s="30" t="s">
+        <v>326</v>
+      </c>
+      <c r="F31" s="49"/>
     </row>
     <row r="32" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="43"/>
-      <c r="B32" s="31" t="s">
-        <v>325</v>
+      <c r="A32" s="42"/>
+      <c r="B32" s="30" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="43"/>
-      <c r="B33" s="31" t="s">
-        <v>326</v>
+      <c r="A33" s="42"/>
+      <c r="B33" s="30" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="43"/>
-      <c r="B34" s="31" t="s">
-        <v>327</v>
+      <c r="A34" s="42"/>
+      <c r="B34" s="30" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="43"/>
-      <c r="B35" s="31" t="s">
-        <v>328</v>
+      <c r="A35" s="42"/>
+      <c r="B35" s="30" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="43"/>
-      <c r="B36" s="31" t="s">
-        <v>329</v>
-      </c>
-      <c r="C36" s="31"/>
+      <c r="A36" s="42"/>
+      <c r="B36" s="30" t="s">
+        <v>331</v>
+      </c>
+      <c r="C36" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>